<commit_message>
update facebook sdk to 8.1
</commit_message>
<xml_diff>
--- a/Assets/Language.xlsx
+++ b/Assets/Language.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="490" uniqueCount="470">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="534" uniqueCount="513">
   <si>
     <t xml:space="preserve">内                       国 </t>
   </si>
@@ -79,9 +79,8 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="宋体"/>
+        <rFont val="微软雅黑"/>
         <charset val="134"/>
-        <scheme val="minor"/>
       </rPr>
       <t xml:space="preserve">You have </t>
     </r>
@@ -89,9 +88,8 @@
       <rPr>
         <sz val="11"/>
         <color rgb="FFFF0000"/>
-        <rFont val="宋体"/>
+        <rFont val="微软雅黑"/>
         <charset val="134"/>
-        <scheme val="minor"/>
       </rPr>
       <t>&lt;color=#FF8A01&gt;{0}&lt;/color&gt;</t>
     </r>
@@ -99,9 +97,8 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="宋体"/>
+        <rFont val="微软雅黑"/>
         <charset val="134"/>
-        <scheme val="minor"/>
       </rPr>
       <t xml:space="preserve"> tickets</t>
     </r>
@@ -144,9 +141,8 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="宋体"/>
+        <rFont val="微软雅黑"/>
         <charset val="134"/>
-        <scheme val="minor"/>
       </rPr>
       <t xml:space="preserve">You must have </t>
     </r>
@@ -154,9 +150,8 @@
       <rPr>
         <sz val="11"/>
         <color rgb="FFFF0000"/>
-        <rFont val="宋体"/>
+        <rFont val="微软雅黑"/>
         <charset val="134"/>
-        <scheme val="minor"/>
       </rPr>
       <t>&lt;color=#F4D10F&gt;{0}&lt;/color&gt;</t>
     </r>
@@ -164,9 +159,8 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="宋体"/>
+        <rFont val="微软雅黑"/>
         <charset val="134"/>
-        <scheme val="minor"/>
       </rPr>
       <t xml:space="preserve"> tickets to participate in the Lucky Draw.</t>
     </r>
@@ -532,6 +526,18 @@
     <t>アバター</t>
   </si>
   <si>
+    <t>Me_New</t>
+  </si>
+  <si>
+    <t>NEW</t>
+  </si>
+  <si>
+    <t>новый</t>
+  </si>
+  <si>
+    <t>新しい</t>
+  </si>
+  <si>
     <t>Me_Unlock</t>
   </si>
   <si>
@@ -784,13 +790,13 @@
     <t>Task_Des_BuyTicketByGoldOnce</t>
   </si>
   <si>
-    <t>Cost{0} coins</t>
+    <t>Cost {0} coins</t>
   </si>
   <si>
     <t>Стоимость {0} монет</t>
   </si>
   <si>
-    <t>{0}コインを過ごします</t>
+    <t>{0} コインを過ごします</t>
   </si>
   <si>
     <t>Task_Des_BuyTicketByRvOnce</t>
@@ -1508,6 +1514,180 @@
   </si>
   <si>
     <t>歴史的な記録を発見し、データが更新されています。</t>
+  </si>
+  <si>
+    <t>Rules_PlaySlots</t>
+  </si>
+  <si>
+    <t>1.Spin and match 3 X symbols to win coin or other reward.
+2.Google are not sponsor are they involved in any Hi Spin sweepstakes or prize draws.
+3.Hi Spin is a sweepstakes application.
+4.For offical rules, please see:</t>
+  </si>
+  <si>
+    <t>1.Spin и матч 3 X символов, чтобы выиграть монеты или иное вознаграждение.
+2.Google не является спонсором, если они участвуют в розыгрышах или розыгрышах призов Hi Spin.
+3.Hi Спин является приложением тотализаторов.
+4.Официальные правила см.</t>
+  </si>
+  <si>
+    <t>1.3つのXシンボルをスピンして一致させ、コインまたはその他の報酬を獲得します。
+2.Googleはスポンサーではなく、HiSpinの懸賞や賞品の抽選に参加しています。
+3.Hiスピンは懸賞アプリです。
+4.公式規則については、以下を参照してください。</t>
+  </si>
+  <si>
+    <t>Rules_PlaySlotsTitle</t>
+  </si>
+  <si>
+    <t>How to win</t>
+  </si>
+  <si>
+    <t>Как победить</t>
+  </si>
+  <si>
+    <t>勝つ方法</t>
+  </si>
+  <si>
+    <t>Rules_PlaySlotsBottom</t>
+  </si>
+  <si>
+    <t>TERMS &amp; CONDITIONS</t>
+  </si>
+  <si>
+    <t>СРОКИ И УСЛОВИЯ</t>
+  </si>
+  <si>
+    <t>Rules_BettingFront</t>
+  </si>
+  <si>
+    <t>1.There is a prize of 1,000 USD in the LuckyDraw every day.
+2.You must have {0} tickets to participate in the Lucky Draw. More tickets you have, more chance to win.
+3.Every day at UTC 08:00:00, all your tickets will be automatically put into the prize pool, and  the Lucky Draw will be done.
+4.There will be many winners with different bonus.</t>
+  </si>
+  <si>
+    <t>1.Существует приз 1000 долларов в LuckyDraw каждый день.
+2.Вы должны иметь {0} билетов на участие в розыгрыше. Больше билетов - больше шансов выиграть.
+3.Каждый день в UTC 08:00:00, все билеты будут автоматически помещаются в призовой фонд, а Лаки Draw будет сделано.
+4.Будет много победителей с разными бонусами.</t>
+  </si>
+  <si>
+    <t>1.LuckyDrawには毎日1,000米ドルの賞金があります。
+2.ラッキードローに参加するには、{0}枚のチケットが必要です。 あなたが持っているより多くのチケット、より多くのチャンス。
+3.毎日08：00：00UTCに、すべての抽選チケットが自動的に賞金プールに入れられますとドローが完了します。
+4.別のボーナスを持つ多くの勝者があるでしょう。</t>
+  </si>
+  <si>
+    <t>Rules_BettingBehind</t>
+  </si>
+  <si>
+    <t>1st $200
+2nd - 3th prize $100
+4nd - 16th prize $20
+17nd - 50th prize $10</t>
+  </si>
+  <si>
+    <t>1-й $ 200
+2-3 приз $ 100
+4-16 приз $ 20
+17-50 приз $ 10</t>
+  </si>
+  <si>
+    <t>最初の$ 200
+2位-3位賞金$ 100
+4位-16位賞金$ 20
+17位-50位賞金$ 10</t>
+  </si>
+  <si>
+    <t>Rules_InviteFrineds</t>
+  </si>
+  <si>
+    <t>1.You can earn points by friends watch ad and complete tasks, and you can also get points from a friends of friends.
+&lt;color=#FFE200&gt;We will give 75% of AD revenue to players. So, You will earn 50% of your close friends’ AD revenue and 25% of your unfamiliar friends’ AD revenue.&lt;/color&gt;
+2.Every day UTC 10:00:00, you can review yesterday’s income from friends.
+3.Points can be exchanged for money, 100,000 points equals 1 USD.
+4.&lt;color=#FFE200&gt;You can earn HUGE Pts by completing the tasks in the offer.&lt;/color&gt;</t>
+  </si>
+  <si>
+    <t>1.Вы можете зарабатывать очки, когда друзья смотрят рекламу и выполняют задания, а также вы можете получать очки от друзей друзей.
+&lt;color=#FFE200&gt; Мы будем отдавать игрокам 75% дохода от рекламы. Таким образом, вы будете получать 50% дохода от рекламы ваших близких друзей и 25% дохода от рекламы незнакомых друзей.&lt;/color&gt;
+2.Каждый день по UTC 10:00:00 вы можете просматривать вчерашний доход от друзей.
+3.Points можно обменять на деньги, 100000 точек составляет 1 USD.
+4.&lt;color=#FFE200&gt;You может заработать ОГРОМНЫЙ оч, выполнив задачи в предложении. &lt;/color&gt;</t>
+  </si>
+  <si>
+    <t>1.友達が広告を見てタスクを完了することでポイントを獲得できます。また、友達の友達からポイントを獲得することもできます。
+&lt;color=＃FFE200&gt;2.私たちは、プレイヤーに広告収入の75％を与えます。 つまり、親しい友人のAD収益の50％と、なじみのない友人のAD収益の25％を獲得できます。&lt;/color&gt;
+3.毎日UTC10：00：00、友達からの昨日の収入を確認できます。
+ポイントはお金と交換できます。100,000ポイントは1米ドルに相当します。
+4.&lt;color=＃FFE200&gt;オファーのタスクを完了すると、巨大なポイントを獲得できます。&lt;/color&gt;</t>
+  </si>
+  <si>
+    <t>Rules_Me</t>
+  </si>
+  <si>
+    <t>1.Play slots to get experience for upgrade level.
+2.Upgrade the level will unlock new avatars and get tickets, also increase the multiplier of getting tickets.
+3.The ticket multiplier is used to increase tickets obtained by slots.</t>
+  </si>
+  <si>
+    <t>1.Играйте в слоты, чтобы получить опыт для повышения уровня.
+2.Повышение уровня будет разблокировать новые аватары и получить билеты, а также увеличить множитель получения билетов.
+3.Мультипликатор билет используется для увеличения билетов, полученных по слотам «.</t>
+  </si>
+  <si>
+    <t>1.「スロットをプレイして、アップグレードレベルの経験を積んでください。
+2.アップグレードレベルは、新しいアバターのロックを解除し、チケットを取得、またチケットを得るための乗数を増加します。
+3.チケット乗数は、スロットによって取得されるチケットを増やすために使用されます。」</t>
+  </si>
+  <si>
+    <t>Rules_Cashout</t>
+  </si>
+  <si>
+    <t>1.Win the jackpot and other cash prizes in the Lucky Draw.
+2.Compete every day in the task and win cash directly!
+3.Refer friends and get direct cash and lots of tickets!</t>
+  </si>
+  <si>
+    <t>1.Выиграйте джекпот и другие денежные призы в Lucky Draw.
+2.Compete каждый день в задаче и выиграть наличные деньги напрямую!
+3.Приглашайте друзей и получайте наличные и много билетов!</t>
+  </si>
+  <si>
+    <t>1.ラッキードローでジャックポットとその他の賞金を獲得します。
+2.タスクで毎日競争し、直接現金を獲得してください！
+3.友達を紹介して、入現金とその興を手に付けましょう！</t>
+  </si>
+  <si>
+    <t>Rules_CashoutTitle</t>
+  </si>
+  <si>
+    <t>HOW TO MAKE MONEY</t>
+  </si>
+  <si>
+    <t>КАК ЗАРАБОТАТЬ</t>
+  </si>
+  <si>
+    <t>お金を稼ぐ方法</t>
+  </si>
+  <si>
+    <t>Rules_Offerwall</t>
+  </si>
+  <si>
+    <t>1.Complete the sponsor's task and get a lot of points.
+2.After completing the task, the sponsor will review the results and increase your points as soon as possible. It may take 1-3 days.
+3.If your close friends complete the task, you will earn extra 50% points, and extra 25%  from unfamiliar friends.</t>
+  </si>
+  <si>
+    <t>1.Complete задача спонсора и получить много очков.
+2.После завершения задания, спонсор обзор результатов и увеличить ваши очки как можно скорее. Это может занять 1-3 дня.
+3.Если ваши близкие друзья выполнят задание, вы получите дополнительные 50% очков и дополнительные 25% от незнакомых друзей.</t>
+  </si>
+  <si>
+    <t>1.スポンサーのタスクを完了し、多くのポイントを獲得します。
+2.タスクの完了後、スポンサーは結果を確認し、できるだけ早くポイントを増やします。 1〜3日かかる場合があります。
+3.親しい友人がタスクを完了すると、50％のポイントが追加され、見知らぬ友人からは25％の追加ポイントが獲得されます。</t>
   </si>
 </sst>
 </file>
@@ -1515,12 +1695,12 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
-  <fonts count="21">
+  <fonts count="22">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1530,14 +1710,13 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="0"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
+      <color theme="1"/>
+      <name val="微软雅黑"/>
+      <charset val="134"/>
     </font>
     <font>
       <sz val="11"/>
-      <color theme="1"/>
+      <color theme="0"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1551,11 +1730,33 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="宋体"/>
-      <charset val="134"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="宋体"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -1566,23 +1767,17 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color rgb="FF3F3F76"/>
+      <color theme="3"/>
       <name val="宋体"/>
-      <charset val="0"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
       <sz val="11"/>
-      <color theme="1"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
+      <color rgb="FFFA7D00"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1603,33 +1798,8 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
+      <color rgb="FF3F3F76"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1637,14 +1807,6 @@
     <font>
       <sz val="11"/>
       <color rgb="FF006100"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1666,6 +1828,22 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
       <name val="宋体"/>
@@ -1673,11 +1851,18 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
       <name val="宋体"/>
       <charset val="134"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="微软雅黑"/>
+      <charset val="134"/>
     </font>
   </fonts>
   <fills count="33">
@@ -1686,6 +1871,126 @@
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -1701,49 +2006,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
+        <fgColor theme="7"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
+        <fgColor rgb="FFC6EFCE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
+        <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1755,13 +2030,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4"/>
+        <fgColor theme="4" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
+        <fgColor theme="4" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1773,103 +2048,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
+        <fgColor rgb="FFFFFFCC"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1927,30 +2112,6 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thin">
         <color rgb="FF7F7F7F"/>
       </left>
@@ -1968,10 +2129,8 @@
     <border>
       <left/>
       <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
+      <top/>
+      <bottom style="medium">
         <color theme="4"/>
       </bottom>
       <diagonal/>
@@ -2003,12 +2162,38 @@
     <border>
       <left/>
       <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
       <top/>
       <bottom style="double">
         <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
@@ -2017,10 +2202,10 @@
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="14" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="21" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -2029,137 +2214,137 @@
     <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="6" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="32" borderId="11" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="24" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="24" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="18" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="18" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -2175,26 +2360,41 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="center"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="49">
@@ -2280,7 +2480,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="330835" y="12065"/>
-          <a:ext cx="1914525" cy="523875"/>
+          <a:ext cx="1914525" cy="638175"/>
         </a:xfrm>
         <a:prstGeom prst="line">
           <a:avLst/>
@@ -2323,8 +2523,8 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="5715" y="176530"/>
-          <a:ext cx="2242185" cy="356870"/>
+          <a:off x="5715" y="214630"/>
+          <a:ext cx="2242185" cy="433070"/>
         </a:xfrm>
         <a:prstGeom prst="line">
           <a:avLst/>
@@ -2637,1741 +2837,1900 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:E124"/>
+  <dimension ref="A1:E135"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A109" activePane="bottomLeft" state="frozen"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" topLeftCell="C1" workbookViewId="0">
+      <pane ySplit="3" topLeftCell="A34" activePane="bottomLeft" state="frozen"/>
       <selection/>
-      <selection pane="bottomLeft" activeCell="C112" sqref="C112:D124"/>
+      <selection pane="bottomLeft" activeCell="D59" sqref="D59"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelCol="4"/>
   <cols>
     <col min="1" max="1" width="29.375" style="2" customWidth="1"/>
-    <col min="2" max="2" width="92.625" style="3" customWidth="1"/>
+    <col min="2" max="2" width="158.916666666667" style="3" customWidth="1"/>
     <col min="3" max="3" width="104.458333333333" style="4" customWidth="1"/>
     <col min="4" max="4" width="72.4916666666667" style="4" customWidth="1"/>
     <col min="5" max="5" width="16.8583333333333" style="4" customWidth="1"/>
     <col min="6" max="16384" width="9" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" ht="16.5" spans="1:4">
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="B1" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="C1" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="D1" s="6" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:2">
+    <row r="2" ht="16.5" spans="1:4">
       <c r="A2" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="4"/>
-    </row>
-    <row r="3" s="1" customFormat="1" ht="14.25" spans="1:1">
-      <c r="A3" s="6" t="s">
+      <c r="B2" s="6"/>
+      <c r="C2" s="6"/>
+      <c r="D2" s="6"/>
+    </row>
+    <row r="3" s="1" customFormat="1" ht="17.25" spans="1:4">
+      <c r="A3" s="7" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="4" spans="1:4">
-      <c r="A4" s="2" t="s">
+      <c r="B3" s="8"/>
+      <c r="C3" s="8"/>
+      <c r="D3" s="8"/>
+    </row>
+    <row r="4" ht="16.5" spans="1:4">
+      <c r="A4" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="3" t="s">
+      <c r="B4" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="C4" s="7" t="s">
+      <c r="C4" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="D4" s="7" t="s">
+      <c r="D4" s="11" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="5" spans="1:4">
-      <c r="A5" s="2" t="s">
+    <row r="5" ht="16.5" spans="1:4">
+      <c r="A5" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="B5" s="3" t="s">
+      <c r="B5" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="C5" s="7" t="s">
+      <c r="C5" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="D5" s="7" t="s">
+      <c r="D5" s="11" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="6" spans="1:4">
-      <c r="A6" s="2" t="s">
+    <row r="6" ht="16.5" spans="1:4">
+      <c r="A6" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="B6" s="3" t="s">
+      <c r="B6" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="C6" s="7" t="s">
+      <c r="C6" s="11" t="s">
         <v>16</v>
       </c>
-      <c r="D6" s="7" t="s">
+      <c r="D6" s="11" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="7" spans="1:4">
-      <c r="A7" s="2" t="s">
+    <row r="7" ht="16.5" spans="1:4">
+      <c r="A7" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="B7" s="8" t="s">
+      <c r="B7" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="C7" s="7" t="s">
+      <c r="C7" s="11" t="s">
         <v>20</v>
       </c>
-      <c r="D7" s="7" t="s">
+      <c r="D7" s="11" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="8" spans="1:4">
-      <c r="A8" s="2" t="s">
+    <row r="8" ht="16.5" spans="1:4">
+      <c r="A8" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="B8" s="3" t="s">
+      <c r="B8" s="10" t="s">
         <v>23</v>
       </c>
-      <c r="C8" s="7" t="s">
+      <c r="C8" s="11" t="s">
         <v>24</v>
       </c>
-      <c r="D8" s="7" t="s">
+      <c r="D8" s="11" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="9" spans="1:4">
-      <c r="A9" s="2" t="s">
+    <row r="9" ht="16.5" spans="1:4">
+      <c r="A9" s="9" t="s">
         <v>26</v>
       </c>
-      <c r="B9" s="8" t="s">
+      <c r="B9" s="10" t="s">
         <v>27</v>
       </c>
-      <c r="C9" s="7" t="s">
+      <c r="C9" s="11" t="s">
         <v>28</v>
       </c>
-      <c r="D9" s="7" t="s">
+      <c r="D9" s="11" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="10" spans="1:4">
-      <c r="A10" s="2" t="s">
+    <row r="10" ht="16.5" spans="1:4">
+      <c r="A10" s="9" t="s">
         <v>30</v>
       </c>
-      <c r="B10" s="8" t="s">
+      <c r="B10" s="10" t="s">
         <v>31</v>
       </c>
-      <c r="C10" s="7" t="s">
+      <c r="C10" s="11" t="s">
         <v>32</v>
       </c>
-      <c r="D10" s="7" t="s">
+      <c r="D10" s="11" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="11" spans="1:4">
-      <c r="A11" s="2" t="s">
+    <row r="11" ht="16.5" spans="1:4">
+      <c r="A11" s="9" t="s">
         <v>34</v>
       </c>
-      <c r="B11" s="3" t="s">
+      <c r="B11" s="10" t="s">
         <v>35</v>
       </c>
-      <c r="C11" s="7" t="s">
+      <c r="C11" s="11" t="s">
         <v>36</v>
       </c>
-      <c r="D11" s="7" t="s">
+      <c r="D11" s="11" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="12" spans="1:4">
-      <c r="A12" s="2" t="s">
+    <row r="12" ht="16.5" spans="1:4">
+      <c r="A12" s="9" t="s">
         <v>38</v>
       </c>
-      <c r="B12" s="3" t="s">
+      <c r="B12" s="10" t="s">
         <v>39</v>
       </c>
-      <c r="C12" s="7" t="s">
+      <c r="C12" s="11" t="s">
         <v>40</v>
       </c>
-      <c r="D12" s="7" t="s">
+      <c r="D12" s="11" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="13" spans="1:4">
-      <c r="A13" s="2" t="s">
+    <row r="13" ht="16.5" spans="1:4">
+      <c r="A13" s="9" t="s">
         <v>42</v>
       </c>
-      <c r="B13" s="3" t="s">
+      <c r="B13" s="10" t="s">
         <v>43</v>
       </c>
-      <c r="C13" s="7" t="s">
+      <c r="C13" s="11" t="s">
         <v>44</v>
       </c>
-      <c r="D13" s="7" t="s">
+      <c r="D13" s="11" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="14" spans="1:4">
-      <c r="A14" s="2" t="s">
+    <row r="14" ht="16.5" spans="1:4">
+      <c r="A14" s="9" t="s">
         <v>46</v>
       </c>
-      <c r="B14" s="3" t="s">
+      <c r="B14" s="10" t="s">
         <v>47</v>
       </c>
-      <c r="C14" s="7" t="s">
+      <c r="C14" s="11" t="s">
         <v>48</v>
       </c>
-      <c r="D14" s="7" t="s">
+      <c r="D14" s="11" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="15" spans="1:4">
-      <c r="A15" s="2" t="s">
+    <row r="15" ht="16.5" spans="1:4">
+      <c r="A15" s="9" t="s">
         <v>50</v>
       </c>
-      <c r="B15" s="3" t="s">
+      <c r="B15" s="10" t="s">
         <v>50</v>
       </c>
-      <c r="C15" s="7" t="s">
+      <c r="C15" s="11" t="s">
         <v>51</v>
       </c>
-      <c r="D15" s="7" t="s">
+      <c r="D15" s="11" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="16" spans="1:4">
-      <c r="A16" s="2" t="s">
+    <row r="16" ht="16.5" spans="1:4">
+      <c r="A16" s="9" t="s">
         <v>53</v>
       </c>
-      <c r="B16" s="3" t="s">
+      <c r="B16" s="10" t="s">
         <v>54</v>
       </c>
-      <c r="C16" s="7" t="s">
+      <c r="C16" s="11" t="s">
         <v>54</v>
       </c>
-      <c r="D16" s="7" t="s">
+      <c r="D16" s="11" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="17" spans="1:4">
-      <c r="A17" s="2" t="s">
+    <row r="17" ht="16.5" spans="1:4">
+      <c r="A17" s="9" t="s">
         <v>55</v>
       </c>
-      <c r="B17" s="3" t="s">
+      <c r="B17" s="10" t="s">
         <v>56</v>
       </c>
-      <c r="C17" s="7" t="s">
+      <c r="C17" s="11" t="s">
         <v>56</v>
       </c>
-      <c r="D17" s="7" t="s">
+      <c r="D17" s="11" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="18" spans="1:4">
-      <c r="A18" s="2" t="s">
+    <row r="18" ht="16.5" spans="1:4">
+      <c r="A18" s="9" t="s">
         <v>57</v>
       </c>
-      <c r="B18" s="3" t="s">
+      <c r="B18" s="10" t="s">
         <v>58</v>
       </c>
-      <c r="C18" s="7" t="s">
+      <c r="C18" s="11" t="s">
         <v>59</v>
       </c>
-      <c r="D18" s="7" t="s">
+      <c r="D18" s="11" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="19" spans="1:4">
-      <c r="A19" s="2" t="s">
+    <row r="19" ht="16.5" spans="1:4">
+      <c r="A19" s="9" t="s">
         <v>61</v>
       </c>
-      <c r="B19" s="3" t="s">
+      <c r="B19" s="10" t="s">
         <v>62</v>
       </c>
-      <c r="C19" s="7" t="s">
+      <c r="C19" s="11" t="s">
         <v>63</v>
       </c>
-      <c r="D19" s="7" t="s">
+      <c r="D19" s="11" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="20" spans="1:4">
-      <c r="A20" s="2" t="s">
+    <row r="20" ht="16.5" spans="1:4">
+      <c r="A20" s="9" t="s">
         <v>65</v>
       </c>
-      <c r="B20" s="3" t="s">
+      <c r="B20" s="10" t="s">
         <v>66</v>
       </c>
-      <c r="C20" s="7" t="s">
+      <c r="C20" s="11" t="s">
         <v>67</v>
       </c>
-      <c r="D20" s="7" t="s">
+      <c r="D20" s="11" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="21" spans="1:4">
-      <c r="A21" s="2" t="s">
+    <row r="21" ht="16.5" spans="1:4">
+      <c r="A21" s="9" t="s">
         <v>69</v>
       </c>
-      <c r="B21" s="3" t="s">
+      <c r="B21" s="10" t="s">
         <v>70</v>
       </c>
-      <c r="C21" s="7" t="s">
+      <c r="C21" s="11" t="s">
         <v>71</v>
       </c>
-      <c r="D21" s="7" t="s">
+      <c r="D21" s="11" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="22" spans="1:4">
-      <c r="A22" s="2" t="s">
+    <row r="22" ht="16.5" spans="1:4">
+      <c r="A22" s="9" t="s">
         <v>73</v>
       </c>
-      <c r="B22" s="3" t="s">
+      <c r="B22" s="10" t="s">
         <v>74</v>
       </c>
-      <c r="C22" s="7" t="s">
+      <c r="C22" s="11" t="s">
         <v>75</v>
       </c>
-      <c r="D22" s="7" t="s">
+      <c r="D22" s="11" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="23" spans="1:4">
-      <c r="A23" s="2" t="s">
+    <row r="23" ht="16.5" spans="1:4">
+      <c r="A23" s="9" t="s">
         <v>77</v>
       </c>
-      <c r="B23" s="3" t="s">
+      <c r="B23" s="10" t="s">
         <v>77</v>
       </c>
-      <c r="C23" s="7" t="s">
+      <c r="C23" s="11" t="s">
         <v>78</v>
       </c>
-      <c r="D23" s="7" t="s">
+      <c r="D23" s="11" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="24" spans="1:4">
-      <c r="A24" s="2" t="s">
+    <row r="24" ht="16.5" spans="1:4">
+      <c r="A24" s="9" t="s">
         <v>80</v>
       </c>
-      <c r="B24" s="3" t="s">
+      <c r="B24" s="10" t="s">
         <v>81</v>
       </c>
-      <c r="C24" s="7" t="s">
+      <c r="C24" s="11" t="s">
         <v>82</v>
       </c>
-      <c r="D24" s="7" t="s">
+      <c r="D24" s="11" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="25" spans="1:4">
-      <c r="A25" s="2" t="s">
+    <row r="25" ht="16.5" spans="1:4">
+      <c r="A25" s="9" t="s">
         <v>84</v>
       </c>
-      <c r="B25" s="3" t="s">
+      <c r="B25" s="10" t="s">
         <v>85</v>
       </c>
-      <c r="C25" s="7" t="s">
+      <c r="C25" s="11" t="s">
         <v>86</v>
       </c>
-      <c r="D25" s="7" t="s">
+      <c r="D25" s="11" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="26" spans="1:4">
-      <c r="A26" s="2" t="s">
+    <row r="26" ht="16.5" spans="1:4">
+      <c r="A26" s="9" t="s">
         <v>88</v>
       </c>
-      <c r="B26" s="3" t="s">
+      <c r="B26" s="10" t="s">
         <v>89</v>
       </c>
-      <c r="C26" s="7" t="s">
+      <c r="C26" s="11" t="s">
         <v>90</v>
       </c>
-      <c r="D26" s="7" t="s">
+      <c r="D26" s="11" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="27" spans="1:4">
-      <c r="A27" s="2" t="s">
+    <row r="27" ht="16.5" spans="1:4">
+      <c r="A27" s="9" t="s">
         <v>92</v>
       </c>
-      <c r="B27" s="3" t="s">
+      <c r="B27" s="10" t="s">
         <v>93</v>
       </c>
-      <c r="C27" s="7" t="s">
+      <c r="C27" s="11" t="s">
         <v>94</v>
       </c>
-      <c r="D27" s="7" t="s">
+      <c r="D27" s="11" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="28" spans="1:4">
-      <c r="A28" s="2" t="s">
+    <row r="28" ht="16.5" spans="1:4">
+      <c r="A28" s="9" t="s">
         <v>96</v>
       </c>
-      <c r="B28" s="3" t="s">
+      <c r="B28" s="10" t="s">
         <v>97</v>
       </c>
-      <c r="C28" s="7" t="s">
+      <c r="C28" s="11" t="s">
         <v>98</v>
       </c>
-      <c r="D28" s="7" t="s">
+      <c r="D28" s="11" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="29" spans="1:4">
-      <c r="A29" s="2" t="s">
+    <row r="29" ht="16.5" spans="1:4">
+      <c r="A29" s="9" t="s">
         <v>100</v>
       </c>
-      <c r="B29" s="3" t="s">
+      <c r="B29" s="10" t="s">
         <v>101</v>
       </c>
-      <c r="C29" s="7" t="s">
+      <c r="C29" s="11" t="s">
         <v>102</v>
       </c>
-      <c r="D29" s="7" t="s">
+      <c r="D29" s="11" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="30" spans="1:4">
-      <c r="A30" s="2" t="s">
+    <row r="30" ht="16.5" spans="1:4">
+      <c r="A30" s="9" t="s">
         <v>104</v>
       </c>
-      <c r="B30" s="3" t="s">
+      <c r="B30" s="10" t="s">
         <v>105</v>
       </c>
-      <c r="C30" s="7" t="s">
+      <c r="C30" s="11" t="s">
         <v>106</v>
       </c>
-      <c r="D30" s="7" t="s">
+      <c r="D30" s="11" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="31" spans="1:4">
-      <c r="A31" s="2" t="s">
+    <row r="31" ht="16.5" spans="1:4">
+      <c r="A31" s="9" t="s">
         <v>108</v>
       </c>
-      <c r="B31" s="3" t="s">
+      <c r="B31" s="10" t="s">
         <v>109</v>
       </c>
-      <c r="C31" s="7" t="s">
+      <c r="C31" s="11" t="s">
         <v>110</v>
       </c>
-      <c r="D31" s="7" t="s">
+      <c r="D31" s="11" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="32" spans="1:4">
-      <c r="A32" s="2" t="s">
+    <row r="32" ht="16.5" spans="1:4">
+      <c r="A32" s="9" t="s">
         <v>112</v>
       </c>
-      <c r="B32" s="3" t="s">
+      <c r="B32" s="10" t="s">
         <v>113</v>
       </c>
-      <c r="C32" s="7" t="s">
+      <c r="C32" s="11" t="s">
         <v>114</v>
       </c>
-      <c r="D32" s="7" t="s">
+      <c r="D32" s="11" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="33" ht="40.5" spans="1:4">
-      <c r="A33" s="2" t="s">
+    <row r="33" ht="33" spans="1:4">
+      <c r="A33" s="9" t="s">
         <v>116</v>
       </c>
-      <c r="B33" s="9" t="s">
+      <c r="B33" s="12" t="s">
         <v>117</v>
       </c>
-      <c r="C33" s="10" t="s">
+      <c r="C33" s="13" t="s">
         <v>118</v>
       </c>
-      <c r="D33" s="10" t="s">
+      <c r="D33" s="13" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="34" spans="1:4">
-      <c r="A34" s="2" t="s">
+    <row r="34" ht="16.5" spans="1:4">
+      <c r="A34" s="9" t="s">
         <v>120</v>
       </c>
-      <c r="B34" s="3" t="s">
+      <c r="B34" s="10" t="s">
         <v>121</v>
       </c>
-      <c r="C34" s="7" t="s">
+      <c r="C34" s="11" t="s">
         <v>122</v>
       </c>
-      <c r="D34" s="7" t="s">
+      <c r="D34" s="11" t="s">
         <v>123</v>
       </c>
     </row>
-    <row r="35" spans="1:4">
-      <c r="A35" s="2" t="s">
+    <row r="35" ht="16.5" spans="1:4">
+      <c r="A35" s="9" t="s">
         <v>124</v>
       </c>
-      <c r="B35" s="3" t="s">
+      <c r="B35" s="10" t="s">
         <v>125</v>
       </c>
-      <c r="C35" s="7" t="s">
+      <c r="C35" s="11" t="s">
         <v>126</v>
       </c>
-      <c r="D35" s="7" t="s">
+      <c r="D35" s="11" t="s">
         <v>127</v>
       </c>
     </row>
-    <row r="36" spans="1:4">
-      <c r="A36" s="2" t="s">
+    <row r="36" ht="16.5" spans="1:4">
+      <c r="A36" s="9" t="s">
         <v>128</v>
       </c>
-      <c r="B36" s="3" t="s">
+      <c r="B36" s="10" t="s">
         <v>129</v>
       </c>
-      <c r="C36" s="7" t="s">
+      <c r="C36" s="11" t="s">
         <v>130</v>
       </c>
-      <c r="D36" s="7" t="s">
+      <c r="D36" s="11" t="s">
         <v>131</v>
       </c>
     </row>
-    <row r="37" spans="1:4">
-      <c r="A37" s="2" t="s">
+    <row r="37" ht="16.5" spans="1:4">
+      <c r="A37" s="9" t="s">
         <v>132</v>
       </c>
-      <c r="B37" s="3" t="s">
+      <c r="B37" s="10" t="s">
         <v>133</v>
       </c>
-      <c r="C37" s="7" t="s">
+      <c r="C37" s="11" t="s">
         <v>134</v>
       </c>
-      <c r="D37" s="7" t="s">
+      <c r="D37" s="11" t="s">
         <v>135</v>
       </c>
     </row>
-    <row r="38" spans="1:4">
-      <c r="A38" s="2" t="s">
+    <row r="38" ht="16.5" spans="1:4">
+      <c r="A38" s="9" t="s">
         <v>136</v>
       </c>
-      <c r="B38" s="3" t="s">
+      <c r="B38" s="10" t="s">
         <v>136</v>
       </c>
-      <c r="C38" s="7" t="s">
+      <c r="C38" s="11" t="s">
         <v>137</v>
       </c>
-      <c r="D38" s="7" t="s">
+      <c r="D38" s="11" t="s">
         <v>138</v>
       </c>
     </row>
-    <row r="39" spans="1:4">
-      <c r="A39" s="2" t="s">
+    <row r="39" ht="16.5" spans="1:4">
+      <c r="A39" s="9" t="s">
         <v>139</v>
       </c>
-      <c r="B39" s="3" t="s">
+      <c r="B39" s="10" t="s">
         <v>140</v>
       </c>
-      <c r="C39" s="7" t="s">
+      <c r="C39" s="11" t="s">
         <v>141</v>
       </c>
-      <c r="D39" s="7" t="s">
+      <c r="D39" s="11" t="s">
         <v>142</v>
       </c>
     </row>
-    <row r="40" spans="1:4">
-      <c r="A40" s="2" t="s">
+    <row r="40" ht="16.5" spans="1:4">
+      <c r="A40" s="9" t="s">
         <v>143</v>
       </c>
-      <c r="B40" s="3" t="s">
+      <c r="B40" s="10" t="s">
         <v>144</v>
       </c>
-      <c r="C40" s="7" t="s">
+      <c r="C40" s="11" t="s">
         <v>145</v>
       </c>
-      <c r="D40" s="7" t="s">
+      <c r="D40" s="11" t="s">
         <v>146</v>
       </c>
     </row>
-    <row r="41" spans="1:4">
-      <c r="A41" s="2" t="s">
+    <row r="41" ht="16.5" spans="1:4">
+      <c r="A41" s="9" t="s">
         <v>147</v>
       </c>
-      <c r="B41" s="3" t="s">
+      <c r="B41" s="10" t="s">
         <v>148</v>
       </c>
-      <c r="C41" s="7" t="s">
+      <c r="C41" s="11" t="s">
         <v>149</v>
       </c>
-      <c r="D41" s="7" t="s">
+      <c r="D41" s="11" t="s">
         <v>150</v>
       </c>
     </row>
-    <row r="42" spans="1:4">
-      <c r="A42" s="2" t="s">
+    <row r="42" ht="16.5" spans="1:4">
+      <c r="A42" s="9" t="s">
         <v>151</v>
       </c>
-      <c r="B42" s="3" t="s">
+      <c r="B42" s="10" t="s">
         <v>152</v>
       </c>
-      <c r="C42" s="7" t="s">
+      <c r="C42" s="14" t="s">
         <v>153</v>
       </c>
-      <c r="D42" s="7" t="s">
+      <c r="D42" s="14" t="s">
         <v>154</v>
       </c>
     </row>
-    <row r="43" spans="1:4">
-      <c r="A43" s="2" t="s">
+    <row r="43" ht="16.5" spans="1:4">
+      <c r="A43" s="9" t="s">
         <v>155</v>
       </c>
-      <c r="B43" s="3" t="s">
+      <c r="B43" s="10" t="s">
         <v>156</v>
       </c>
-      <c r="C43" s="7" t="s">
+      <c r="C43" s="11" t="s">
         <v>157</v>
       </c>
-      <c r="D43" s="7" t="s">
+      <c r="D43" s="11" t="s">
         <v>158</v>
       </c>
     </row>
-    <row r="44" spans="1:4">
-      <c r="A44" s="2" t="s">
+    <row r="44" ht="16.5" spans="1:4">
+      <c r="A44" s="9" t="s">
         <v>159</v>
       </c>
-      <c r="B44" s="3" t="s">
+      <c r="B44" s="10" t="s">
         <v>160</v>
       </c>
-      <c r="C44" s="7" t="s">
+      <c r="C44" s="11" t="s">
         <v>161</v>
       </c>
-      <c r="D44" s="7" t="s">
+      <c r="D44" s="11" t="s">
         <v>162</v>
       </c>
     </row>
-    <row r="45" spans="1:4">
-      <c r="A45" s="2" t="s">
+    <row r="45" ht="16.5" spans="1:4">
+      <c r="A45" s="9" t="s">
         <v>163</v>
       </c>
-      <c r="B45" s="3" t="s">
+      <c r="B45" s="10" t="s">
         <v>164</v>
       </c>
-      <c r="C45" s="7" t="s">
+      <c r="C45" s="11" t="s">
         <v>165</v>
       </c>
-      <c r="D45" s="7" t="s">
+      <c r="D45" s="11" t="s">
         <v>166</v>
       </c>
     </row>
-    <row r="46" spans="1:4">
-      <c r="A46" s="2" t="s">
+    <row r="46" ht="16.5" spans="1:4">
+      <c r="A46" s="9" t="s">
         <v>167</v>
       </c>
-      <c r="B46" s="3" t="s">
+      <c r="B46" s="10" t="s">
         <v>168</v>
       </c>
-      <c r="C46" s="7" t="s">
+      <c r="C46" s="11" t="s">
         <v>169</v>
       </c>
-      <c r="D46" s="7" t="s">
+      <c r="D46" s="11" t="s">
         <v>170</v>
       </c>
     </row>
-    <row r="47" spans="1:4">
-      <c r="A47" s="2" t="s">
+    <row r="47" ht="16.5" spans="1:4">
+      <c r="A47" s="9" t="s">
         <v>171</v>
       </c>
-      <c r="B47" s="3" t="s">
+      <c r="B47" s="10" t="s">
         <v>172</v>
       </c>
-      <c r="C47" s="7" t="s">
+      <c r="C47" s="11" t="s">
         <v>173</v>
       </c>
-      <c r="D47" s="7" t="s">
+      <c r="D47" s="11" t="s">
         <v>174</v>
       </c>
     </row>
-    <row r="48" spans="1:4">
-      <c r="A48" s="2" t="s">
+    <row r="48" ht="16.5" spans="1:4">
+      <c r="A48" s="9" t="s">
         <v>175</v>
       </c>
-      <c r="B48" s="3" t="s">
+      <c r="B48" s="10" t="s">
         <v>176</v>
       </c>
-      <c r="C48" t="s">
+      <c r="C48" s="11" t="s">
         <v>177</v>
       </c>
-      <c r="D48" t="s">
+      <c r="D48" s="11" t="s">
         <v>178</v>
       </c>
     </row>
-    <row r="49" spans="1:4">
-      <c r="A49" s="2" t="s">
+    <row r="49" ht="16.5" spans="1:4">
+      <c r="A49" s="9" t="s">
         <v>179</v>
       </c>
-      <c r="B49" s="3" t="s">
+      <c r="B49" s="10" t="s">
         <v>180</v>
       </c>
-      <c r="C49" s="7" t="s">
+      <c r="C49" s="14" t="s">
         <v>181</v>
       </c>
-      <c r="D49" s="7" t="s">
+      <c r="D49" s="14" t="s">
         <v>182</v>
       </c>
     </row>
-    <row r="50" spans="1:4">
-      <c r="A50" s="2" t="s">
+    <row r="50" ht="16.5" spans="1:4">
+      <c r="A50" s="9" t="s">
         <v>183</v>
       </c>
-      <c r="B50" s="3" t="s">
+      <c r="B50" s="10" t="s">
         <v>184</v>
       </c>
-      <c r="C50" s="7" t="s">
+      <c r="C50" s="11" t="s">
         <v>185</v>
       </c>
-      <c r="D50" s="7" t="s">
-        <v>166</v>
-      </c>
-    </row>
-    <row r="51" spans="1:4">
-      <c r="A51" s="2" t="s">
+      <c r="D50" s="11" t="s">
         <v>186</v>
       </c>
-      <c r="B51" s="3" t="s">
+    </row>
+    <row r="51" ht="16.5" spans="1:4">
+      <c r="A51" s="9" t="s">
         <v>187</v>
       </c>
-      <c r="C51" s="7" t="s">
+      <c r="B51" s="10" t="s">
         <v>188</v>
       </c>
-      <c r="D51" s="7" t="s">
+      <c r="C51" s="11" t="s">
         <v>189</v>
       </c>
-    </row>
-    <row r="52" spans="1:4">
-      <c r="A52" s="2" t="s">
+      <c r="D51" s="11" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="52" ht="16.5" spans="1:4">
+      <c r="A52" s="9" t="s">
         <v>190</v>
       </c>
-      <c r="B52" s="3" t="s">
+      <c r="B52" s="10" t="s">
         <v>191</v>
       </c>
-      <c r="C52" t="s">
+      <c r="C52" s="11" t="s">
         <v>192</v>
       </c>
-      <c r="D52" t="s">
+      <c r="D52" s="11" t="s">
         <v>193</v>
       </c>
     </row>
-    <row r="53" spans="1:4">
-      <c r="A53" s="2" t="s">
+    <row r="53" ht="16.5" spans="1:4">
+      <c r="A53" s="9" t="s">
         <v>194</v>
       </c>
-      <c r="B53" s="3" t="s">
+      <c r="B53" s="10" t="s">
         <v>195</v>
       </c>
-      <c r="C53" s="7" t="s">
+      <c r="C53" s="14" t="s">
         <v>196</v>
       </c>
-      <c r="D53" s="7" t="s">
+      <c r="D53" s="14" t="s">
         <v>197</v>
       </c>
     </row>
-    <row r="54" spans="1:4">
-      <c r="A54" s="2" t="s">
+    <row r="54" ht="16.5" spans="1:4">
+      <c r="A54" s="9" t="s">
         <v>198</v>
       </c>
-      <c r="B54" s="3" t="s">
+      <c r="B54" s="10" t="s">
         <v>199</v>
       </c>
-      <c r="C54" s="7" t="s">
+      <c r="C54" s="11" t="s">
         <v>200</v>
       </c>
-      <c r="D54" s="7" t="s">
+      <c r="D54" s="11" t="s">
         <v>201</v>
       </c>
     </row>
-    <row r="55" spans="1:4">
-      <c r="A55" s="2" t="s">
+    <row r="55" ht="16.5" spans="1:4">
+      <c r="A55" s="9" t="s">
         <v>202</v>
       </c>
-      <c r="B55" s="11" t="s">
+      <c r="B55" s="10" t="s">
         <v>203</v>
       </c>
-      <c r="C55" s="7" t="s">
+      <c r="C55" s="11" t="s">
         <v>204</v>
       </c>
-      <c r="D55" s="7" t="s">
+      <c r="D55" s="11" t="s">
         <v>205</v>
       </c>
     </row>
-    <row r="56" spans="1:4">
-      <c r="A56" s="2" t="s">
+    <row r="56" ht="16.5" spans="1:4">
+      <c r="A56" s="9" t="s">
         <v>206</v>
       </c>
-      <c r="B56" s="11" t="s">
+      <c r="B56" s="15" t="s">
         <v>207</v>
       </c>
-      <c r="C56" s="7" t="s">
+      <c r="C56" s="11" t="s">
         <v>208</v>
       </c>
-      <c r="D56" s="7" t="s">
+      <c r="D56" s="11" t="s">
         <v>209</v>
       </c>
     </row>
-    <row r="57" spans="1:4">
-      <c r="A57" s="2" t="s">
+    <row r="57" ht="16.5" spans="1:4">
+      <c r="A57" s="9" t="s">
         <v>210</v>
       </c>
-      <c r="B57" s="11" t="s">
+      <c r="B57" s="15" t="s">
         <v>211</v>
       </c>
-      <c r="C57" s="7" t="s">
+      <c r="C57" s="11" t="s">
         <v>212</v>
       </c>
-      <c r="D57" s="7" t="s">
+      <c r="D57" s="11" t="s">
         <v>213</v>
       </c>
     </row>
-    <row r="58" spans="1:4">
-      <c r="A58" s="2" t="s">
+    <row r="58" ht="16.5" spans="1:4">
+      <c r="A58" s="9" t="s">
         <v>214</v>
       </c>
-      <c r="B58" s="3" t="s">
+      <c r="B58" s="15" t="s">
         <v>215</v>
       </c>
-      <c r="C58" s="7" t="s">
+      <c r="C58" s="11" t="s">
         <v>216</v>
       </c>
-      <c r="D58" s="7" t="s">
+      <c r="D58" s="11" t="s">
         <v>217</v>
       </c>
     </row>
-    <row r="59" spans="1:4">
-      <c r="A59" s="2" t="s">
+    <row r="59" ht="16.5" spans="1:4">
+      <c r="A59" s="9" t="s">
         <v>218</v>
       </c>
-      <c r="B59" s="3" t="s">
+      <c r="B59" s="10" t="s">
         <v>219</v>
       </c>
-      <c r="C59" s="7" t="s">
+      <c r="C59" s="11" t="s">
         <v>220</v>
       </c>
-      <c r="D59" s="7" t="s">
+      <c r="D59" s="11" t="s">
         <v>221</v>
       </c>
     </row>
-    <row r="60" spans="1:4">
-      <c r="A60" s="2" t="s">
+    <row r="60" ht="16.5" spans="1:4">
+      <c r="A60" s="9" t="s">
         <v>222</v>
       </c>
-      <c r="B60" s="3" t="s">
+      <c r="B60" s="10" t="s">
         <v>223</v>
       </c>
-      <c r="C60" s="7" t="s">
+      <c r="C60" s="11" t="s">
         <v>224</v>
       </c>
-      <c r="D60" s="7" t="s">
+      <c r="D60" s="11" t="s">
         <v>225</v>
       </c>
     </row>
-    <row r="61" spans="1:4">
-      <c r="A61" s="2" t="s">
+    <row r="61" ht="16.5" spans="1:4">
+      <c r="A61" s="9" t="s">
         <v>226</v>
       </c>
-      <c r="B61" s="11" t="s">
+      <c r="B61" s="10" t="s">
         <v>227</v>
       </c>
-      <c r="C61" s="7" t="s">
+      <c r="C61" s="11" t="s">
         <v>228</v>
       </c>
-      <c r="D61" s="7" t="s">
+      <c r="D61" s="11" t="s">
         <v>229</v>
       </c>
     </row>
-    <row r="62" spans="1:4">
-      <c r="A62" s="2" t="s">
+    <row r="62" ht="16.5" spans="1:4">
+      <c r="A62" s="9" t="s">
         <v>230</v>
       </c>
-      <c r="B62" s="3" t="s">
+      <c r="B62" s="15" t="s">
         <v>231</v>
       </c>
-      <c r="C62" s="7" t="s">
+      <c r="C62" s="11" t="s">
         <v>232</v>
       </c>
-      <c r="D62" s="7" t="s">
+      <c r="D62" s="11" t="s">
         <v>233</v>
       </c>
     </row>
-    <row r="63" spans="1:4">
-      <c r="A63" s="2" t="s">
+    <row r="63" ht="16.5" spans="1:4">
+      <c r="A63" s="9" t="s">
         <v>234</v>
       </c>
-      <c r="B63" s="3" t="s">
+      <c r="B63" s="10" t="s">
         <v>235</v>
       </c>
-      <c r="C63" s="7" t="s">
+      <c r="C63" s="11" t="s">
         <v>236</v>
       </c>
-      <c r="D63" s="7" t="s">
+      <c r="D63" s="11" t="s">
         <v>237</v>
       </c>
     </row>
-    <row r="64" spans="1:4">
-      <c r="A64" s="2" t="s">
+    <row r="64" ht="16.5" spans="1:4">
+      <c r="A64" s="9" t="s">
         <v>238</v>
       </c>
-      <c r="B64" s="3" t="s">
+      <c r="B64" s="10" t="s">
         <v>239</v>
       </c>
-      <c r="C64" s="7" t="s">
+      <c r="C64" s="11" t="s">
         <v>240</v>
       </c>
-      <c r="D64" s="7" t="s">
+      <c r="D64" s="11" t="s">
         <v>241</v>
       </c>
     </row>
-    <row r="65" spans="1:4">
-      <c r="A65" s="2" t="s">
+    <row r="65" ht="16.5" spans="1:4">
+      <c r="A65" s="9" t="s">
         <v>242</v>
       </c>
-      <c r="B65" s="3" t="s">
-        <v>242</v>
-      </c>
-      <c r="C65" s="7" t="s">
+      <c r="B65" s="10" t="s">
         <v>243</v>
       </c>
-      <c r="D65" s="7" t="s">
+      <c r="C65" s="11" t="s">
         <v>244</v>
       </c>
-    </row>
-    <row r="66" spans="1:4">
-      <c r="A66" s="2" t="s">
+      <c r="D65" s="11" t="s">
         <v>245</v>
       </c>
-      <c r="B66" s="3" t="s">
-        <v>245</v>
-      </c>
-      <c r="C66" s="7" t="s">
+    </row>
+    <row r="66" ht="16.5" spans="1:4">
+      <c r="A66" s="9" t="s">
         <v>246</v>
       </c>
-      <c r="D66" s="7" t="s">
+      <c r="B66" s="10" t="s">
+        <v>246</v>
+      </c>
+      <c r="C66" s="11" t="s">
         <v>247</v>
       </c>
-    </row>
-    <row r="67" spans="1:4">
-      <c r="A67" s="2" t="s">
+      <c r="D66" s="11" t="s">
         <v>248</v>
       </c>
-      <c r="B67" s="3" t="s">
+    </row>
+    <row r="67" ht="16.5" spans="1:4">
+      <c r="A67" s="9" t="s">
         <v>249</v>
       </c>
-      <c r="C67" s="7" t="s">
+      <c r="B67" s="10" t="s">
+        <v>249</v>
+      </c>
+      <c r="C67" s="11" t="s">
         <v>250</v>
       </c>
-      <c r="D67" s="7" t="s">
+      <c r="D67" s="11" t="s">
         <v>251</v>
       </c>
     </row>
-    <row r="68" spans="1:4">
-      <c r="A68" s="2" t="s">
+    <row r="68" ht="16.5" spans="1:4">
+      <c r="A68" s="9" t="s">
         <v>252</v>
       </c>
-      <c r="B68" s="3" t="s">
-        <v>252</v>
-      </c>
-      <c r="C68" s="7" t="s">
+      <c r="B68" s="10" t="s">
         <v>253</v>
       </c>
-      <c r="D68" s="7" t="s">
+      <c r="C68" s="11" t="s">
         <v>254</v>
       </c>
-    </row>
-    <row r="69" spans="1:4">
-      <c r="A69" s="2" t="s">
+      <c r="D68" s="11" t="s">
         <v>255</v>
       </c>
-      <c r="B69" s="3" t="s">
-        <v>255</v>
-      </c>
-      <c r="C69" s="7" t="s">
+    </row>
+    <row r="69" ht="16.5" spans="1:4">
+      <c r="A69" s="9" t="s">
         <v>256</v>
       </c>
-      <c r="D69" s="7" t="s">
+      <c r="B69" s="10" t="s">
+        <v>256</v>
+      </c>
+      <c r="C69" s="11" t="s">
         <v>257</v>
       </c>
-    </row>
-    <row r="70" spans="1:4">
-      <c r="A70" s="2" t="s">
+      <c r="D69" s="11" t="s">
         <v>258</v>
       </c>
-      <c r="B70" s="3" t="s">
+    </row>
+    <row r="70" ht="16.5" spans="1:4">
+      <c r="A70" s="9" t="s">
         <v>259</v>
       </c>
-      <c r="C70" s="7" t="s">
+      <c r="B70" s="10" t="s">
         <v>259</v>
       </c>
-      <c r="D70" s="7" t="s">
+      <c r="C70" s="11" t="s">
         <v>260</v>
       </c>
-    </row>
-    <row r="71" spans="1:4">
-      <c r="A71" s="2" t="s">
+      <c r="D70" s="11" t="s">
         <v>261</v>
       </c>
-      <c r="B71" s="3" t="s">
+    </row>
+    <row r="71" ht="16.5" spans="1:4">
+      <c r="A71" s="9" t="s">
         <v>262</v>
       </c>
-      <c r="C71" s="7" t="s">
+      <c r="B71" s="10" t="s">
         <v>263</v>
       </c>
-      <c r="D71" s="7" t="s">
+      <c r="C71" s="11" t="s">
+        <v>263</v>
+      </c>
+      <c r="D71" s="11" t="s">
         <v>264</v>
       </c>
     </row>
-    <row r="72" spans="1:4">
-      <c r="A72" s="2" t="s">
+    <row r="72" ht="16.5" spans="1:4">
+      <c r="A72" s="9" t="s">
         <v>265</v>
       </c>
-      <c r="B72" s="3" t="s">
+      <c r="B72" s="10" t="s">
         <v>266</v>
       </c>
-      <c r="C72" s="7" t="s">
+      <c r="C72" s="11" t="s">
         <v>267</v>
       </c>
-      <c r="D72" s="7" t="s">
+      <c r="D72" s="11" t="s">
         <v>268</v>
       </c>
     </row>
-    <row r="73" spans="1:4">
-      <c r="A73" s="2" t="s">
+    <row r="73" ht="16.5" spans="1:4">
+      <c r="A73" s="9" t="s">
         <v>269</v>
       </c>
-      <c r="B73" s="3" t="s">
+      <c r="B73" s="10" t="s">
         <v>270</v>
       </c>
-      <c r="C73" s="7" t="s">
+      <c r="C73" s="11" t="s">
         <v>271</v>
       </c>
-      <c r="D73" s="7" t="s">
+      <c r="D73" s="11" t="s">
         <v>272</v>
       </c>
     </row>
-    <row r="74" spans="1:4">
-      <c r="A74" s="2" t="s">
+    <row r="74" ht="16.5" spans="1:4">
+      <c r="A74" s="9" t="s">
         <v>273</v>
       </c>
-      <c r="B74" s="3" t="s">
+      <c r="B74" s="10" t="s">
         <v>274</v>
       </c>
-      <c r="C74" s="7" t="s">
+      <c r="C74" s="11" t="s">
         <v>275</v>
       </c>
-      <c r="D74" s="7" t="s">
-        <v>197</v>
-      </c>
-    </row>
-    <row r="75" spans="1:4">
-      <c r="A75" s="2" t="s">
+      <c r="D74" s="11" t="s">
         <v>276</v>
       </c>
-      <c r="B75" s="3" t="s">
+    </row>
+    <row r="75" ht="16.5" spans="1:4">
+      <c r="A75" s="9" t="s">
         <v>277</v>
       </c>
-      <c r="C75" s="7" t="s">
+      <c r="B75" s="10" t="s">
         <v>278</v>
       </c>
-      <c r="D75" s="7" t="s">
+      <c r="C75" s="11" t="s">
         <v>279</v>
       </c>
-    </row>
-    <row r="76" spans="1:4">
-      <c r="A76" s="2" t="s">
+      <c r="D75" s="11" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="76" ht="16.5" spans="1:4">
+      <c r="A76" s="9" t="s">
         <v>280</v>
       </c>
-      <c r="B76" s="3" t="s">
+      <c r="B76" s="10" t="s">
         <v>281</v>
       </c>
-      <c r="C76" s="7" t="s">
+      <c r="C76" s="11" t="s">
         <v>282</v>
       </c>
-      <c r="D76" s="7" t="s">
-        <v>281</v>
-      </c>
-    </row>
-    <row r="77" spans="1:4">
-      <c r="A77" s="2" t="s">
+      <c r="D76" s="11" t="s">
         <v>283</v>
       </c>
-      <c r="B77" s="3" t="s">
+    </row>
+    <row r="77" ht="16.5" spans="1:4">
+      <c r="A77" s="9" t="s">
         <v>284</v>
       </c>
-      <c r="C77" s="7" t="s">
+      <c r="B77" s="10" t="s">
         <v>285</v>
       </c>
-      <c r="D77" s="7" t="s">
+      <c r="C77" s="11" t="s">
         <v>286</v>
       </c>
-    </row>
-    <row r="78" spans="1:4">
-      <c r="A78" s="2" t="s">
+      <c r="D77" s="11" t="s">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="78" ht="16.5" spans="1:4">
+      <c r="A78" s="9" t="s">
         <v>287</v>
       </c>
-      <c r="B78" s="3" t="s">
+      <c r="B78" s="10" t="s">
         <v>288</v>
       </c>
-      <c r="C78" s="7" t="s">
+      <c r="C78" s="11" t="s">
         <v>289</v>
       </c>
-      <c r="D78" s="7" t="s">
+      <c r="D78" s="11" t="s">
         <v>290</v>
       </c>
     </row>
-    <row r="79" spans="1:4">
-      <c r="A79" s="2" t="s">
+    <row r="79" ht="16.5" spans="1:4">
+      <c r="A79" s="9" t="s">
         <v>291</v>
       </c>
-      <c r="B79" s="3" t="s">
+      <c r="B79" s="10" t="s">
         <v>292</v>
       </c>
-      <c r="C79" s="7" t="s">
+      <c r="C79" s="11" t="s">
         <v>293</v>
       </c>
-      <c r="D79" s="7" t="s">
+      <c r="D79" s="11" t="s">
         <v>294</v>
       </c>
     </row>
-    <row r="80" spans="1:4">
-      <c r="A80" s="2" t="s">
+    <row r="80" ht="16.5" spans="1:4">
+      <c r="A80" s="9" t="s">
         <v>295</v>
       </c>
-      <c r="B80" s="3" t="s">
+      <c r="B80" s="10" t="s">
         <v>296</v>
       </c>
-      <c r="C80" s="7" t="s">
+      <c r="C80" s="11" t="s">
         <v>297</v>
       </c>
-      <c r="D80" s="7" t="s">
+      <c r="D80" s="11" t="s">
         <v>298</v>
       </c>
     </row>
-    <row r="81" spans="1:4">
-      <c r="A81" s="2" t="s">
+    <row r="81" ht="16.5" spans="1:4">
+      <c r="A81" s="9" t="s">
         <v>299</v>
       </c>
-      <c r="B81" s="3" t="s">
-        <v>299</v>
-      </c>
-      <c r="C81" s="7" t="s">
+      <c r="B81" s="10" t="s">
         <v>300</v>
       </c>
-      <c r="D81" s="7" t="s">
+      <c r="C81" s="11" t="s">
         <v>301</v>
       </c>
-    </row>
-    <row r="82" spans="1:4">
-      <c r="A82" s="2" t="s">
+      <c r="D81" s="11" t="s">
         <v>302</v>
       </c>
-      <c r="B82" s="3" t="s">
+    </row>
+    <row r="82" ht="16.5" spans="1:4">
+      <c r="A82" s="9" t="s">
         <v>303</v>
       </c>
-      <c r="C82" s="7" t="s">
+      <c r="B82" s="10" t="s">
+        <v>303</v>
+      </c>
+      <c r="C82" s="11" t="s">
         <v>304</v>
       </c>
-      <c r="D82" s="7" t="s">
+      <c r="D82" s="11" t="s">
         <v>305</v>
       </c>
     </row>
-    <row r="83" ht="54" spans="1:4">
-      <c r="A83" s="2" t="s">
+    <row r="83" ht="16.5" spans="1:4">
+      <c r="A83" s="9" t="s">
         <v>306</v>
       </c>
-      <c r="B83" s="9" t="s">
+      <c r="B83" s="10" t="s">
         <v>307</v>
       </c>
-      <c r="C83" s="10" t="s">
+      <c r="C83" s="11" t="s">
         <v>308</v>
       </c>
-      <c r="D83" s="10" t="s">
+      <c r="D83" s="11" t="s">
         <v>309</v>
       </c>
     </row>
-    <row r="84" ht="27" spans="1:4">
-      <c r="A84" s="2" t="s">
+    <row r="84" ht="66" spans="1:4">
+      <c r="A84" s="9" t="s">
         <v>310</v>
       </c>
-      <c r="B84" s="9" t="s">
+      <c r="B84" s="12" t="s">
         <v>311</v>
       </c>
-      <c r="C84" s="10" t="s">
+      <c r="C84" s="13" t="s">
         <v>312</v>
       </c>
-      <c r="D84" s="10" t="s">
+      <c r="D84" s="13" t="s">
         <v>313</v>
       </c>
     </row>
-    <row r="85" spans="1:4">
-      <c r="A85" s="2" t="s">
+    <row r="85" ht="33" spans="1:4">
+      <c r="A85" s="9" t="s">
         <v>314</v>
       </c>
-      <c r="B85" s="3" t="s">
+      <c r="B85" s="12" t="s">
         <v>315</v>
       </c>
-      <c r="C85" s="7" t="s">
+      <c r="C85" s="13" t="s">
         <v>316</v>
       </c>
-      <c r="D85" s="7" t="s">
+      <c r="D85" s="13" t="s">
         <v>317</v>
       </c>
     </row>
-    <row r="86" spans="1:4">
-      <c r="A86" s="2" t="s">
+    <row r="86" ht="16.5" spans="1:4">
+      <c r="A86" s="9" t="s">
         <v>318</v>
       </c>
-      <c r="B86" s="3" t="s">
+      <c r="B86" s="10" t="s">
         <v>319</v>
       </c>
-      <c r="C86" s="7" t="s">
+      <c r="C86" s="11" t="s">
         <v>320</v>
       </c>
-      <c r="D86" s="7" t="s">
+      <c r="D86" s="11" t="s">
         <v>321</v>
       </c>
     </row>
-    <row r="87" spans="1:4">
-      <c r="A87" s="2" t="s">
+    <row r="87" ht="16.5" spans="1:4">
+      <c r="A87" s="9" t="s">
         <v>322</v>
       </c>
-      <c r="B87" s="3" t="s">
+      <c r="B87" s="10" t="s">
         <v>323</v>
       </c>
-      <c r="C87" s="7" t="s">
+      <c r="C87" s="11" t="s">
         <v>324</v>
       </c>
-      <c r="D87" s="7" t="s">
+      <c r="D87" s="11" t="s">
         <v>325</v>
       </c>
     </row>
-    <row r="88" spans="1:4">
-      <c r="A88" s="2" t="s">
+    <row r="88" ht="16.5" spans="1:4">
+      <c r="A88" s="9" t="s">
         <v>326</v>
       </c>
-      <c r="B88" s="3" t="s">
-        <v>326</v>
-      </c>
-      <c r="C88" s="7" t="s">
+      <c r="B88" s="10" t="s">
         <v>327</v>
       </c>
-      <c r="D88" s="7" t="s">
+      <c r="C88" s="11" t="s">
         <v>328</v>
       </c>
-    </row>
-    <row r="89" spans="1:4">
-      <c r="A89" s="2" t="s">
+      <c r="D88" s="11" t="s">
         <v>329</v>
       </c>
-      <c r="B89" s="3" t="s">
+    </row>
+    <row r="89" ht="16.5" spans="1:4">
+      <c r="A89" s="9" t="s">
         <v>330</v>
       </c>
-      <c r="C89" s="7" t="s">
+      <c r="B89" s="10" t="s">
+        <v>330</v>
+      </c>
+      <c r="C89" s="11" t="s">
         <v>331</v>
       </c>
-      <c r="D89" s="7" t="s">
+      <c r="D89" s="11" t="s">
         <v>332</v>
       </c>
     </row>
-    <row r="90" spans="1:4">
-      <c r="A90" s="2" t="s">
+    <row r="90" ht="16.5" spans="1:4">
+      <c r="A90" s="9" t="s">
         <v>333</v>
       </c>
-      <c r="B90" s="3" t="s">
+      <c r="B90" s="10" t="s">
         <v>334</v>
       </c>
-      <c r="C90" t="s">
+      <c r="C90" s="11" t="s">
         <v>335</v>
       </c>
-      <c r="D90" t="s">
+      <c r="D90" s="11" t="s">
         <v>336</v>
       </c>
     </row>
-    <row r="91" ht="27" spans="1:4">
-      <c r="A91" s="2" t="s">
+    <row r="91" ht="16.5" spans="1:4">
+      <c r="A91" s="9" t="s">
         <v>337</v>
       </c>
-      <c r="B91" s="9" t="s">
+      <c r="B91" s="10" t="s">
         <v>338</v>
       </c>
-      <c r="C91" s="10" t="s">
+      <c r="C91" s="14" t="s">
         <v>339</v>
       </c>
-      <c r="D91" s="10" t="s">
+      <c r="D91" s="14" t="s">
         <v>340</v>
       </c>
     </row>
-    <row r="92" ht="27" spans="1:4">
-      <c r="A92" s="2" t="s">
+    <row r="92" ht="33" spans="1:4">
+      <c r="A92" s="9" t="s">
         <v>341</v>
       </c>
-      <c r="B92" s="9" t="s">
+      <c r="B92" s="12" t="s">
         <v>342</v>
       </c>
-      <c r="C92" s="10" t="s">
+      <c r="C92" s="13" t="s">
         <v>343</v>
       </c>
-      <c r="D92" s="10" t="s">
+      <c r="D92" s="13" t="s">
         <v>344</v>
       </c>
     </row>
-    <row r="93" ht="27" spans="1:4">
-      <c r="A93" s="2" t="s">
+    <row r="93" ht="33" spans="1:4">
+      <c r="A93" s="9" t="s">
         <v>345</v>
       </c>
-      <c r="B93" s="9" t="s">
+      <c r="B93" s="12" t="s">
         <v>346</v>
       </c>
-      <c r="C93" s="10" t="s">
+      <c r="C93" s="13" t="s">
         <v>347</v>
       </c>
-      <c r="D93" s="10" t="s">
+      <c r="D93" s="13" t="s">
         <v>348</v>
       </c>
     </row>
-    <row r="94" spans="1:4">
-      <c r="A94" s="2" t="s">
+    <row r="94" ht="33" spans="1:4">
+      <c r="A94" s="9" t="s">
         <v>349</v>
       </c>
-      <c r="B94" s="3" t="s">
+      <c r="B94" s="12" t="s">
         <v>350</v>
       </c>
-      <c r="C94" s="7" t="s">
+      <c r="C94" s="13" t="s">
         <v>351</v>
       </c>
-      <c r="D94" s="7" t="s">
+      <c r="D94" s="13" t="s">
         <v>352</v>
       </c>
     </row>
-    <row r="95" spans="1:4">
-      <c r="A95" s="2" t="s">
+    <row r="95" ht="16.5" spans="1:4">
+      <c r="A95" s="9" t="s">
         <v>353</v>
       </c>
-      <c r="B95" s="3" t="s">
+      <c r="B95" s="10" t="s">
         <v>354</v>
       </c>
-      <c r="C95" s="7" t="s">
+      <c r="C95" s="11" t="s">
         <v>355</v>
       </c>
-      <c r="D95" s="7" t="s">
+      <c r="D95" s="11" t="s">
         <v>356</v>
       </c>
     </row>
-    <row r="96" spans="1:4">
-      <c r="A96" s="2" t="s">
+    <row r="96" ht="16.5" spans="1:4">
+      <c r="A96" s="9" t="s">
         <v>357</v>
       </c>
-      <c r="B96" s="3" t="s">
+      <c r="B96" s="10" t="s">
         <v>358</v>
       </c>
-      <c r="C96" s="7" t="s">
+      <c r="C96" s="11" t="s">
         <v>359</v>
       </c>
-      <c r="D96" s="7" t="s">
+      <c r="D96" s="11" t="s">
         <v>360</v>
       </c>
     </row>
-    <row r="97" spans="1:4">
-      <c r="A97" s="2" t="s">
+    <row r="97" ht="16.5" spans="1:4">
+      <c r="A97" s="9" t="s">
         <v>361</v>
       </c>
-      <c r="B97" s="3" t="s">
+      <c r="B97" s="10" t="s">
         <v>362</v>
       </c>
-      <c r="C97" s="7" t="s">
+      <c r="C97" s="11" t="s">
         <v>363</v>
       </c>
-      <c r="D97" s="7" t="s">
+      <c r="D97" s="11" t="s">
         <v>364</v>
       </c>
     </row>
-    <row r="98" spans="1:4">
-      <c r="A98" s="2" t="s">
+    <row r="98" ht="16.5" spans="1:4">
+      <c r="A98" s="9" t="s">
         <v>365</v>
       </c>
-      <c r="B98" s="3" t="s">
-        <v>365</v>
-      </c>
-      <c r="C98" s="7" t="s">
+      <c r="B98" s="10" t="s">
         <v>366</v>
       </c>
-      <c r="D98" s="7" t="s">
+      <c r="C98" s="11" t="s">
         <v>367</v>
       </c>
-    </row>
-    <row r="99" spans="1:4">
-      <c r="A99" s="2" t="s">
+      <c r="D98" s="11" t="s">
         <v>368</v>
       </c>
-      <c r="B99" s="3" t="s">
+    </row>
+    <row r="99" ht="16.5" spans="1:4">
+      <c r="A99" s="9" t="s">
         <v>369</v>
       </c>
-      <c r="C99" s="7" t="s">
+      <c r="B99" s="10" t="s">
+        <v>369</v>
+      </c>
+      <c r="C99" s="11" t="s">
         <v>370</v>
       </c>
-      <c r="D99" s="7" t="s">
+      <c r="D99" s="11" t="s">
         <v>371</v>
       </c>
     </row>
-    <row r="100" spans="1:4">
-      <c r="A100" s="2" t="s">
+    <row r="100" ht="16.5" spans="1:4">
+      <c r="A100" s="9" t="s">
         <v>372</v>
       </c>
-      <c r="B100" s="3" t="s">
-        <v>372</v>
-      </c>
-      <c r="C100" s="7" t="s">
+      <c r="B100" s="10" t="s">
         <v>373</v>
       </c>
-      <c r="D100" s="7" t="s">
+      <c r="C100" s="11" t="s">
         <v>374</v>
       </c>
-    </row>
-    <row r="101" spans="1:4">
-      <c r="A101" s="2" t="s">
+      <c r="D100" s="11" t="s">
         <v>375</v>
       </c>
-      <c r="B101" s="3" t="s">
+    </row>
+    <row r="101" ht="16.5" spans="1:4">
+      <c r="A101" s="9" t="s">
         <v>376</v>
       </c>
-      <c r="C101" s="7" t="s">
+      <c r="B101" s="10" t="s">
+        <v>376</v>
+      </c>
+      <c r="C101" s="11" t="s">
         <v>377</v>
       </c>
-      <c r="D101" s="7" t="s">
+      <c r="D101" s="11" t="s">
         <v>378</v>
       </c>
     </row>
-    <row r="102" spans="1:4">
-      <c r="A102" s="2" t="s">
+    <row r="102" ht="16.5" spans="1:4">
+      <c r="A102" s="9" t="s">
         <v>379</v>
       </c>
-      <c r="B102" s="3" t="s">
+      <c r="B102" s="10" t="s">
         <v>380</v>
       </c>
-      <c r="C102" s="7" t="s">
+      <c r="C102" s="11" t="s">
         <v>381</v>
       </c>
-      <c r="D102" s="7" t="s">
+      <c r="D102" s="11" t="s">
         <v>382</v>
       </c>
     </row>
-    <row r="103" spans="1:4">
-      <c r="A103" s="2" t="s">
+    <row r="103" ht="16.5" spans="1:4">
+      <c r="A103" s="9" t="s">
         <v>383</v>
       </c>
-      <c r="B103" s="3" t="s">
+      <c r="B103" s="10" t="s">
         <v>384</v>
       </c>
-      <c r="C103" s="7" t="s">
+      <c r="C103" s="11" t="s">
         <v>385</v>
       </c>
-      <c r="D103" s="7" t="s">
+      <c r="D103" s="11" t="s">
         <v>386</v>
       </c>
     </row>
-    <row r="104" spans="1:4">
-      <c r="A104" s="2" t="s">
+    <row r="104" ht="16.5" spans="1:4">
+      <c r="A104" s="9" t="s">
         <v>387</v>
       </c>
-      <c r="B104" s="3" t="s">
+      <c r="B104" s="10" t="s">
         <v>388</v>
       </c>
-      <c r="C104" s="7" t="s">
+      <c r="C104" s="11" t="s">
         <v>389</v>
       </c>
-      <c r="D104" s="7" t="s">
+      <c r="D104" s="11" t="s">
         <v>390</v>
       </c>
     </row>
-    <row r="105" spans="1:4">
-      <c r="A105" s="2" t="s">
+    <row r="105" ht="16.5" spans="1:4">
+      <c r="A105" s="9" t="s">
         <v>391</v>
       </c>
-      <c r="B105" s="3" t="s">
+      <c r="B105" s="10" t="s">
         <v>392</v>
       </c>
-      <c r="C105" s="7" t="s">
+      <c r="C105" s="11" t="s">
         <v>393</v>
       </c>
-      <c r="D105" s="7" t="s">
+      <c r="D105" s="11" t="s">
         <v>394</v>
       </c>
     </row>
-    <row r="106" spans="1:4">
-      <c r="A106" s="2" t="s">
+    <row r="106" ht="16.5" spans="1:4">
+      <c r="A106" s="9" t="s">
         <v>395</v>
       </c>
-      <c r="B106" s="3" t="s">
+      <c r="B106" s="10" t="s">
         <v>396</v>
       </c>
-      <c r="C106" s="7" t="s">
+      <c r="C106" s="11" t="s">
         <v>397</v>
       </c>
-      <c r="D106" s="7" t="s">
+      <c r="D106" s="11" t="s">
         <v>398</v>
       </c>
     </row>
-    <row r="107" spans="1:4">
-      <c r="A107" s="2" t="s">
+    <row r="107" ht="16.5" spans="1:4">
+      <c r="A107" s="9" t="s">
         <v>399</v>
       </c>
-      <c r="B107" s="3" t="s">
+      <c r="B107" s="10" t="s">
         <v>400</v>
       </c>
-      <c r="C107" s="7" t="s">
+      <c r="C107" s="11" t="s">
         <v>401</v>
       </c>
-      <c r="D107" s="7" t="s">
+      <c r="D107" s="11" t="s">
         <v>402</v>
       </c>
     </row>
-    <row r="108" spans="1:4">
-      <c r="A108" s="2" t="s">
+    <row r="108" ht="16.5" spans="1:4">
+      <c r="A108" s="9" t="s">
         <v>403</v>
       </c>
-      <c r="B108" s="3" t="s">
+      <c r="B108" s="10" t="s">
         <v>404</v>
       </c>
-      <c r="C108" t="s">
+      <c r="C108" s="11" t="s">
         <v>405</v>
       </c>
-      <c r="D108" t="s">
+      <c r="D108" s="11" t="s">
         <v>406</v>
       </c>
     </row>
-    <row r="109" spans="1:4">
-      <c r="A109" s="2" t="s">
+    <row r="109" ht="16.5" spans="1:4">
+      <c r="A109" s="9" t="s">
         <v>407</v>
       </c>
-      <c r="B109" s="3" t="s">
+      <c r="B109" s="10" t="s">
         <v>408</v>
       </c>
-      <c r="C109" t="s">
+      <c r="C109" s="14" t="s">
         <v>409</v>
       </c>
-      <c r="D109" t="s">
+      <c r="D109" s="14" t="s">
         <v>410</v>
       </c>
     </row>
-    <row r="110" spans="1:4">
-      <c r="A110" s="2" t="s">
+    <row r="110" ht="16.5" spans="1:4">
+      <c r="A110" s="9" t="s">
         <v>411</v>
       </c>
-      <c r="B110" s="3" t="s">
+      <c r="B110" s="10" t="s">
         <v>412</v>
       </c>
-      <c r="C110" t="s">
+      <c r="C110" s="14" t="s">
         <v>413</v>
       </c>
-      <c r="D110" t="s">
+      <c r="D110" s="14" t="s">
         <v>414</v>
       </c>
     </row>
-    <row r="111" spans="1:4">
-      <c r="A111" s="2" t="s">
+    <row r="111" ht="16.5" spans="1:4">
+      <c r="A111" s="9" t="s">
         <v>415</v>
       </c>
-      <c r="B111" s="3" t="s">
+      <c r="B111" s="10" t="s">
         <v>416</v>
       </c>
-      <c r="C111" t="s">
+      <c r="C111" s="14" t="s">
         <v>417</v>
       </c>
-      <c r="D111" t="s">
+      <c r="D111" s="14" t="s">
         <v>418</v>
       </c>
     </row>
-    <row r="112" spans="1:4">
-      <c r="A112" s="2" t="s">
+    <row r="112" ht="16.5" spans="1:4">
+      <c r="A112" s="9" t="s">
         <v>419</v>
       </c>
-      <c r="B112" s="3" t="s">
+      <c r="B112" s="10" t="s">
         <v>420</v>
       </c>
-      <c r="C112" s="7" t="s">
+      <c r="C112" s="14" t="s">
         <v>421</v>
       </c>
-      <c r="D112" s="7" t="s">
+      <c r="D112" s="14" t="s">
         <v>422</v>
       </c>
     </row>
-    <row r="113" spans="1:4">
-      <c r="A113" s="2" t="s">
+    <row r="113" ht="16.5" spans="1:4">
+      <c r="A113" s="9" t="s">
         <v>423</v>
       </c>
-      <c r="B113" s="3" t="s">
+      <c r="B113" s="10" t="s">
         <v>424</v>
       </c>
-      <c r="C113" s="7" t="s">
+      <c r="C113" s="11" t="s">
         <v>425</v>
       </c>
-      <c r="D113" s="7" t="s">
+      <c r="D113" s="11" t="s">
         <v>426</v>
       </c>
     </row>
-    <row r="114" spans="1:4">
-      <c r="A114" s="2" t="s">
+    <row r="114" ht="16.5" spans="1:4">
+      <c r="A114" s="9" t="s">
         <v>427</v>
       </c>
-      <c r="B114" s="3" t="s">
+      <c r="B114" s="10" t="s">
         <v>428</v>
       </c>
-      <c r="C114" s="7" t="s">
+      <c r="C114" s="11" t="s">
         <v>429</v>
       </c>
-      <c r="D114" s="7" t="s">
+      <c r="D114" s="11" t="s">
         <v>430</v>
       </c>
     </row>
-    <row r="115" spans="1:4">
-      <c r="A115" s="2" t="s">
+    <row r="115" ht="16.5" spans="1:4">
+      <c r="A115" s="9" t="s">
         <v>431</v>
       </c>
-      <c r="B115" s="3" t="s">
+      <c r="B115" s="10" t="s">
         <v>432</v>
       </c>
-      <c r="C115" s="7" t="s">
+      <c r="C115" s="11" t="s">
         <v>433</v>
       </c>
-      <c r="D115" s="7" t="s">
+      <c r="D115" s="11" t="s">
         <v>434</v>
       </c>
     </row>
-    <row r="116" spans="1:4">
-      <c r="A116" s="2" t="s">
+    <row r="116" ht="16.5" spans="1:4">
+      <c r="A116" s="9" t="s">
         <v>435</v>
       </c>
-      <c r="B116" s="3" t="s">
+      <c r="B116" s="10" t="s">
         <v>436</v>
       </c>
-      <c r="C116" s="7" t="s">
+      <c r="C116" s="11" t="s">
         <v>437</v>
       </c>
-      <c r="D116" s="7" t="s">
+      <c r="D116" s="11" t="s">
         <v>438</v>
       </c>
     </row>
-    <row r="117" spans="1:4">
-      <c r="A117" s="2" t="s">
+    <row r="117" ht="16.5" spans="1:4">
+      <c r="A117" s="9" t="s">
         <v>439</v>
       </c>
-      <c r="B117" s="3" t="s">
+      <c r="B117" s="10" t="s">
         <v>440</v>
       </c>
-      <c r="C117" s="7" t="s">
+      <c r="C117" s="11" t="s">
         <v>441</v>
       </c>
-      <c r="D117" s="7" t="s">
+      <c r="D117" s="11" t="s">
         <v>442</v>
       </c>
     </row>
-    <row r="118" spans="1:4">
-      <c r="A118" s="2" t="s">
+    <row r="118" ht="16.5" spans="1:4">
+      <c r="A118" s="9" t="s">
         <v>443</v>
       </c>
-      <c r="B118" s="3" t="s">
+      <c r="B118" s="10" t="s">
         <v>444</v>
       </c>
-      <c r="C118" s="7" t="s">
+      <c r="C118" s="11" t="s">
         <v>445</v>
       </c>
-      <c r="D118" s="7" t="s">
+      <c r="D118" s="11" t="s">
         <v>446</v>
       </c>
     </row>
-    <row r="119" spans="1:4">
-      <c r="A119" s="2" t="s">
+    <row r="119" ht="16.5" spans="1:4">
+      <c r="A119" s="9" t="s">
         <v>447</v>
       </c>
-      <c r="B119" s="3" t="s">
+      <c r="B119" s="10" t="s">
         <v>448</v>
       </c>
-      <c r="C119" s="7" t="s">
+      <c r="C119" s="11" t="s">
         <v>449</v>
       </c>
-      <c r="D119" s="7" t="s">
-        <v>448</v>
-      </c>
-    </row>
-    <row r="120" spans="1:4">
-      <c r="A120" s="2" t="s">
+      <c r="D119" s="11" t="s">
         <v>450</v>
       </c>
-      <c r="B120" s="3" t="s">
+    </row>
+    <row r="120" ht="16.5" spans="1:4">
+      <c r="A120" s="9" t="s">
         <v>451</v>
       </c>
-      <c r="C120" s="7" t="s">
+      <c r="B120" s="10" t="s">
         <v>452</v>
       </c>
-      <c r="D120" s="7" t="s">
+      <c r="C120" s="11" t="s">
         <v>453</v>
       </c>
-    </row>
-    <row r="121" spans="1:4">
-      <c r="A121" s="2" t="s">
+      <c r="D120" s="11" t="s">
+        <v>452</v>
+      </c>
+    </row>
+    <row r="121" ht="16.5" spans="1:4">
+      <c r="A121" s="9" t="s">
         <v>454</v>
       </c>
-      <c r="B121" s="3" t="s">
+      <c r="B121" s="10" t="s">
         <v>455</v>
       </c>
-      <c r="C121" s="7" t="s">
+      <c r="C121" s="11" t="s">
         <v>456</v>
       </c>
-      <c r="D121" s="7" t="s">
+      <c r="D121" s="11" t="s">
         <v>457</v>
       </c>
     </row>
-    <row r="122" spans="1:4">
-      <c r="A122" s="2" t="s">
+    <row r="122" ht="16.5" spans="1:4">
+      <c r="A122" s="9" t="s">
         <v>458</v>
       </c>
-      <c r="B122" s="3" t="s">
+      <c r="B122" s="10" t="s">
         <v>459</v>
       </c>
-      <c r="C122" s="7" t="s">
+      <c r="C122" s="11" t="s">
         <v>460</v>
       </c>
-      <c r="D122" s="7" t="s">
+      <c r="D122" s="11" t="s">
         <v>461</v>
       </c>
     </row>
-    <row r="123" spans="1:4">
-      <c r="A123" s="2" t="s">
+    <row r="123" ht="16.5" spans="1:4">
+      <c r="A123" s="9" t="s">
         <v>462</v>
       </c>
-      <c r="B123" s="3" t="s">
+      <c r="B123" s="10" t="s">
         <v>463</v>
       </c>
-      <c r="C123" s="7" t="s">
+      <c r="C123" s="11" t="s">
         <v>464</v>
       </c>
-      <c r="D123" s="7" t="s">
+      <c r="D123" s="11" t="s">
         <v>465</v>
       </c>
     </row>
-    <row r="124" spans="1:4">
-      <c r="A124" s="2" t="s">
+    <row r="124" ht="16.5" spans="1:4">
+      <c r="A124" s="9" t="s">
         <v>466</v>
       </c>
-      <c r="B124" s="3" t="s">
+      <c r="B124" s="10" t="s">
         <v>467</v>
       </c>
-      <c r="C124" s="7" t="s">
+      <c r="C124" s="11" t="s">
         <v>468</v>
       </c>
-      <c r="D124" s="7" t="s">
+      <c r="D124" s="11" t="s">
         <v>469</v>
+      </c>
+    </row>
+    <row r="125" ht="16.5" spans="1:4">
+      <c r="A125" s="9" t="s">
+        <v>470</v>
+      </c>
+      <c r="B125" s="10" t="s">
+        <v>471</v>
+      </c>
+      <c r="C125" s="11" t="s">
+        <v>472</v>
+      </c>
+      <c r="D125" s="11" t="s">
+        <v>473</v>
+      </c>
+    </row>
+    <row r="126" ht="66" spans="1:4">
+      <c r="A126" s="9" t="s">
+        <v>474</v>
+      </c>
+      <c r="B126" s="12" t="s">
+        <v>475</v>
+      </c>
+      <c r="C126" s="13" t="s">
+        <v>476</v>
+      </c>
+      <c r="D126" s="13" t="s">
+        <v>477</v>
+      </c>
+    </row>
+    <row r="127" ht="16.5" spans="1:4">
+      <c r="A127" s="9" t="s">
+        <v>478</v>
+      </c>
+      <c r="B127" s="10" t="s">
+        <v>479</v>
+      </c>
+      <c r="C127" s="11" t="s">
+        <v>480</v>
+      </c>
+      <c r="D127" s="11" t="s">
+        <v>481</v>
+      </c>
+    </row>
+    <row r="128" ht="16.5" spans="1:4">
+      <c r="A128" s="9" t="s">
+        <v>482</v>
+      </c>
+      <c r="B128" s="10" t="s">
+        <v>483</v>
+      </c>
+      <c r="C128" s="11" t="s">
+        <v>484</v>
+      </c>
+      <c r="D128" s="11" t="s">
+        <v>386</v>
+      </c>
+    </row>
+    <row r="129" ht="99" spans="1:4">
+      <c r="A129" s="9" t="s">
+        <v>485</v>
+      </c>
+      <c r="B129" s="12" t="s">
+        <v>486</v>
+      </c>
+      <c r="C129" s="13" t="s">
+        <v>487</v>
+      </c>
+      <c r="D129" s="13" t="s">
+        <v>488</v>
+      </c>
+    </row>
+    <row r="130" ht="66" spans="1:4">
+      <c r="A130" s="9" t="s">
+        <v>489</v>
+      </c>
+      <c r="B130" s="12" t="s">
+        <v>490</v>
+      </c>
+      <c r="C130" s="13" t="s">
+        <v>491</v>
+      </c>
+      <c r="D130" s="13" t="s">
+        <v>492</v>
+      </c>
+    </row>
+    <row r="131" ht="148.5" spans="1:4">
+      <c r="A131" s="9" t="s">
+        <v>493</v>
+      </c>
+      <c r="B131" s="12" t="s">
+        <v>494</v>
+      </c>
+      <c r="C131" s="16" t="s">
+        <v>495</v>
+      </c>
+      <c r="D131" s="13" t="s">
+        <v>496</v>
+      </c>
+    </row>
+    <row r="132" ht="82.5" spans="1:4">
+      <c r="A132" s="9" t="s">
+        <v>497</v>
+      </c>
+      <c r="B132" s="12" t="s">
+        <v>498</v>
+      </c>
+      <c r="C132" s="13" t="s">
+        <v>499</v>
+      </c>
+      <c r="D132" s="13" t="s">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="133" ht="82.5" spans="1:4">
+      <c r="A133" s="9" t="s">
+        <v>501</v>
+      </c>
+      <c r="B133" s="12" t="s">
+        <v>502</v>
+      </c>
+      <c r="C133" s="13" t="s">
+        <v>503</v>
+      </c>
+      <c r="D133" s="13" t="s">
+        <v>504</v>
+      </c>
+    </row>
+    <row r="134" ht="16.5" spans="1:4">
+      <c r="A134" s="9" t="s">
+        <v>505</v>
+      </c>
+      <c r="B134" s="12" t="s">
+        <v>506</v>
+      </c>
+      <c r="C134" s="14" t="s">
+        <v>507</v>
+      </c>
+      <c r="D134" s="14" t="s">
+        <v>508</v>
+      </c>
+    </row>
+    <row r="135" ht="82.5" spans="1:4">
+      <c r="A135" s="9" t="s">
+        <v>509</v>
+      </c>
+      <c r="B135" s="12" t="s">
+        <v>510</v>
+      </c>
+      <c r="C135" s="13" t="s">
+        <v>511</v>
+      </c>
+      <c r="D135" s="13" t="s">
+        <v>512</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
change invite friend reward icon
</commit_message>
<xml_diff>
--- a/Assets/Language.xlsx
+++ b/Assets/Language.xlsx
@@ -2597,19 +2597,48 @@
     <t>Slots_NextSlotsIn</t>
   </si>
   <si>
-    <t>FREE SLOTS :</t>
-  </si>
-  <si>
-    <t>БЕСПЛАТНЫЕ СЛОТЫ:</t>
-  </si>
-  <si>
-    <t>無料スロット：</t>
-  </si>
-  <si>
-    <t>무료 슬롯 :</t>
-  </si>
-  <si>
-    <t>FREI SLOTS :</t>
+    <t>FREE SLOTS</t>
+  </si>
+  <si>
+    <t>БЕСПЛАТНЫЕ СЛОТЫ</t>
+  </si>
+  <si>
+    <t>無料スロット</t>
+  </si>
+  <si>
+    <r>
+      <t>무료</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="微软雅黑"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="MS Gothic"/>
+        <charset val="134"/>
+      </rPr>
+      <t>슬롯</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="微软雅黑"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+  </si>
+  <si>
+    <t>FREI SLOTS</t>
   </si>
   <si>
     <t>Slots_Win</t>
@@ -6526,13 +6555,13 @@
     <t>Tips_ClickUnlockOfferwall</t>
   </si>
   <si>
-    <t>Unlock at level 4.</t>
-  </si>
-  <si>
-    <t>Разблокируется на уровне 4.</t>
-  </si>
-  <si>
-    <t>レベル4でロック解除。</t>
+    <t>Unlock at level 2.</t>
+  </si>
+  <si>
+    <t>Разблокируется на уровне 2.</t>
+  </si>
+  <si>
+    <t>レベル2でロック解除。</t>
   </si>
   <si>
     <r>
@@ -6551,7 +6580,7 @@
         <rFont val="微软雅黑"/>
         <charset val="134"/>
       </rPr>
-      <t xml:space="preserve"> 4</t>
+      <t xml:space="preserve"> 2</t>
     </r>
     <r>
       <rPr>
@@ -6609,7 +6638,7 @@
     </r>
   </si>
   <si>
-    <t>Unlock auf Ebene 4.</t>
+    <t>Unlock auf Ebene 2.</t>
   </si>
   <si>
     <t>Tips_EmptyEmail</t>
@@ -11528,28 +11557,28 @@
     </font>
     <font>
       <sz val="11"/>
-      <name val="微软雅黑"/>
+      <color theme="1"/>
+      <name val="MS Gothic"/>
       <charset val="134"/>
     </font>
     <font>
       <sz val="11"/>
-      <color theme="1"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
+      <name val="微软雅黑"/>
+      <charset val="134"/>
     </font>
     <font>
       <sz val="11"/>
       <color theme="0"/>
       <name val="宋体"/>
       <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -11561,7 +11590,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF3F3F76"/>
+      <color theme="1"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -11569,7 +11598,7 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color rgb="FFFFFFFF"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -11594,6 +11623,37 @@
       <u/>
       <sz val="11"/>
       <color rgb="FF0000FF"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -11629,25 +11689,9 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
+      <color rgb="FFFA7D00"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -11660,26 +11704,11 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
+      <color rgb="FFFA7D00"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="MS Gothic"/>
-      <charset val="134"/>
     </font>
     <font>
       <sz val="11"/>
@@ -11709,19 +11738,121 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
+        <fgColor theme="6"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -11739,31 +11870,31 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
+        <fgColor theme="9" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
+        <fgColor theme="7" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
+        <fgColor theme="8" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
+        <fgColor theme="8"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
+        <fgColor theme="8" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -11775,43 +11906,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
+        <fgColor theme="8" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -11823,73 +11918,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -11935,8 +11964,62 @@
       <left/>
       <right/>
       <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
       <bottom style="double">
-        <color rgb="FFFF8001"/>
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -11958,15 +12041,6 @@
     <border>
       <left/>
       <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
       <top style="thin">
         <color theme="4"/>
       </top>
@@ -11979,53 +12053,8 @@
       <left/>
       <right/>
       <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
       <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
+        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
@@ -12037,10 +12066,10 @@
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="12" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="18" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -12049,16 +12078,16 @@
     <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -12067,119 +12096,119 @@
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="33" borderId="11" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="15" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="13" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="15" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="13" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="32" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="9" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -12240,10 +12269,13 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -12783,10 +12815,10 @@
   <sheetPr/>
   <dimension ref="A1:F138"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" topLeftCell="A121" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="C1" activePane="topRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" topLeftCell="A40" workbookViewId="0">
+      <pane xSplit="1" topLeftCell="E1" activePane="topRight" state="frozen"/>
       <selection/>
-      <selection pane="topRight" activeCell="E136" sqref="E136"/>
+      <selection pane="topRight" activeCell="F52" sqref="F52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="16.5" outlineLevelCol="5"/>
@@ -13813,7 +13845,7 @@
       <c r="D52" s="8" t="s">
         <v>281</v>
       </c>
-      <c r="E52" s="8" t="s">
+      <c r="E52" s="20" t="s">
         <v>282</v>
       </c>
       <c r="F52" s="8" t="s">
@@ -13884,7 +13916,7 @@
       <c r="A56" s="13" t="s">
         <v>301</v>
       </c>
-      <c r="B56" s="20" t="s">
+      <c r="B56" s="21" t="s">
         <v>302</v>
       </c>
       <c r="C56" s="8" t="s">
@@ -13904,7 +13936,7 @@
       <c r="A57" s="13" t="s">
         <v>307</v>
       </c>
-      <c r="B57" s="20" t="s">
+      <c r="B57" s="21" t="s">
         <v>308</v>
       </c>
       <c r="C57" s="8" t="s">
@@ -13924,7 +13956,7 @@
       <c r="A58" s="13" t="s">
         <v>313</v>
       </c>
-      <c r="B58" s="20" t="s">
+      <c r="B58" s="21" t="s">
         <v>314</v>
       </c>
       <c r="C58" s="8" t="s">
@@ -14004,7 +14036,7 @@
       <c r="A62" s="13" t="s">
         <v>337</v>
       </c>
-      <c r="B62" s="20" t="s">
+      <c r="B62" s="21" t="s">
         <v>338</v>
       </c>
       <c r="C62" s="8" t="s">
@@ -14164,7 +14196,7 @@
       <c r="A70" s="13" t="s">
         <v>382</v>
       </c>
-      <c r="B70" s="21" t="s">
+      <c r="B70" s="22" t="s">
         <v>382</v>
       </c>
       <c r="C70" s="8" t="s">
@@ -14344,19 +14376,19 @@
       <c r="A79" s="13" t="s">
         <v>430</v>
       </c>
-      <c r="B79" s="22" t="s">
+      <c r="B79" s="23" t="s">
         <v>431</v>
       </c>
-      <c r="C79" s="22" t="s">
+      <c r="C79" s="23" t="s">
         <v>432</v>
       </c>
-      <c r="D79" s="22" t="s">
+      <c r="D79" s="23" t="s">
         <v>433</v>
       </c>
-      <c r="E79" s="22" t="s">
+      <c r="E79" s="23" t="s">
         <v>434</v>
       </c>
-      <c r="F79" s="22" t="s">
+      <c r="F79" s="23" t="s">
         <v>435</v>
       </c>
     </row>
@@ -14364,19 +14396,19 @@
       <c r="A80" s="13" t="s">
         <v>436</v>
       </c>
-      <c r="B80" s="22" t="s">
+      <c r="B80" s="23" t="s">
         <v>437</v>
       </c>
-      <c r="C80" s="22" t="s">
+      <c r="C80" s="23" t="s">
         <v>438</v>
       </c>
-      <c r="D80" s="22" t="s">
+      <c r="D80" s="23" t="s">
         <v>439</v>
       </c>
-      <c r="E80" s="22" t="s">
+      <c r="E80" s="23" t="s">
         <v>440</v>
       </c>
-      <c r="F80" s="22" t="s">
+      <c r="F80" s="23" t="s">
         <v>441</v>
       </c>
     </row>
@@ -14384,19 +14416,19 @@
       <c r="A81" s="13" t="s">
         <v>442</v>
       </c>
-      <c r="B81" s="22" t="s">
+      <c r="B81" s="23" t="s">
         <v>443</v>
       </c>
-      <c r="C81" s="22" t="s">
+      <c r="C81" s="23" t="s">
         <v>444</v>
       </c>
-      <c r="D81" s="22" t="s">
+      <c r="D81" s="23" t="s">
         <v>445</v>
       </c>
-      <c r="E81" s="22" t="s">
+      <c r="E81" s="23" t="s">
         <v>446</v>
       </c>
-      <c r="F81" s="22" t="s">
+      <c r="F81" s="23" t="s">
         <v>447</v>
       </c>
     </row>
@@ -15173,7 +15205,7 @@
       <c r="D120" s="8" t="s">
         <v>674</v>
       </c>
-      <c r="E120" s="8" t="s">
+      <c r="E120" s="20" t="s">
         <v>675</v>
       </c>
       <c r="F120" s="8" t="s">
@@ -15407,7 +15439,7 @@
       <c r="B132" s="14" t="s">
         <v>742</v>
       </c>
-      <c r="C132" s="23" t="s">
+      <c r="C132" s="24" t="s">
         <v>743</v>
       </c>
       <c r="D132" s="15" t="s">
@@ -15504,7 +15536,7 @@
       <c r="A137" s="13" t="s">
         <v>771</v>
       </c>
-      <c r="B137" s="22" t="s">
+      <c r="B137" s="23" t="s">
         <v>772</v>
       </c>
       <c r="C137" s="8" t="s">
@@ -15524,7 +15556,7 @@
       <c r="A138" s="13" t="s">
         <v>777</v>
       </c>
-      <c r="B138" s="22" t="s">
+      <c r="B138" s="23" t="s">
         <v>778</v>
       </c>
       <c r="C138" s="16" t="s">

</xml_diff>

<commit_message>
fix sign guide image
</commit_message>
<xml_diff>
--- a/Assets/Language.xlsx
+++ b/Assets/Language.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="818" uniqueCount="783">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="820" uniqueCount="785">
   <si>
     <t xml:space="preserve">内                                     国 </t>
   </si>
@@ -2607,6 +2607,12 @@
   </si>
   <si>
     <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="MS Gothic"/>
+        <charset val="134"/>
+      </rPr>
       <t>무료</t>
     </r>
     <r>
@@ -5158,6 +5164,12 @@
   </si>
   <si>
     <t>Spiele Lucy mit Tickets Draw Geld zu verdienen. Gute Lucy!</t>
+  </si>
+  <si>
+    <t>Guide4</t>
+  </si>
+  <si>
+    <t>Check in 15 days, you can receive the money!</t>
   </si>
   <si>
     <t>InviteOk_Tip</t>
@@ -11536,12 +11548,12 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
-  <fonts count="25">
+  <fonts count="26">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -11568,17 +11580,29 @@
     </font>
     <font>
       <sz val="11"/>
+      <color rgb="FF333333"/>
+      <name val="微软雅黑"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color theme="0"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
       <name val="宋体"/>
-      <charset val="134"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -11589,8 +11613,16 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FFFF0000"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -11598,7 +11630,7 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
+      <color rgb="FF3F3F3F"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -11628,9 +11660,31 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
+      <color theme="1"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -11653,13 +11707,6 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
       <color rgb="FF006100"/>
       <name val="宋体"/>
       <charset val="0"/>
@@ -11667,43 +11714,14 @@
     </font>
     <font>
       <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
+      <sz val="15"/>
       <color theme="3"/>
       <name val="宋体"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
       <name val="宋体"/>
@@ -11723,12 +11741,18 @@
       <charset val="134"/>
     </font>
   </fonts>
-  <fills count="34">
+  <fills count="35">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -11738,97 +11762,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
+        <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -11846,7 +11780,133 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -11858,13 +11918,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
+        <fgColor theme="5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -11876,19 +11930,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
+        <fgColor rgb="FFFFFFCC"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -11900,25 +11942,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
+        <fgColor theme="5" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -11971,30 +11995,15 @@
     </border>
     <border>
       <left style="thin">
-        <color rgb="FFB2B2B2"/>
+        <color rgb="FF3F3F3F"/>
       </left>
       <right style="thin">
-        <color rgb="FFB2B2B2"/>
+        <color rgb="FF3F3F3F"/>
       </right>
       <top style="thin">
-        <color rgb="FFB2B2B2"/>
+        <color rgb="FF3F3F3F"/>
       </top>
       <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
         <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
@@ -12005,21 +12014,6 @@
       <top/>
       <bottom style="medium">
         <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -12041,6 +12035,15 @@
     <border>
       <left/>
       <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
       <top style="thin">
         <color theme="4"/>
       </top>
@@ -12050,11 +12053,32 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
       <bottom style="double">
-        <color rgb="FFFF8001"/>
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
       </bottom>
       <diagonal/>
     </border>
@@ -12066,10 +12090,10 @@
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="18" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="18" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -12078,37 +12102,34 @@
     <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="32" borderId="11" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -12117,98 +12138,101 @@
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="13" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="13" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="14" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="9" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="23" fillId="14" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="26" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -12219,6 +12243,9 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -12260,7 +12287,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -12279,6 +12306,15 @@
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -12813,18 +12849,18 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:F138"/>
+  <dimension ref="A1:F139"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" topLeftCell="A40" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="E1" activePane="topRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" topLeftCell="A79" workbookViewId="0">
+      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
       <selection/>
-      <selection pane="topRight" activeCell="F52" sqref="F52"/>
+      <selection pane="topRight" activeCell="B93" sqref="B93"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="16.5" outlineLevelCol="5"/>
   <cols>
-    <col min="1" max="1" width="29.375" style="4" customWidth="1"/>
-    <col min="2" max="2" width="158.916666666667" style="5" customWidth="1"/>
+    <col min="1" max="1" width="29.375" style="5" customWidth="1"/>
+    <col min="2" max="2" width="158.916666666667" style="6" customWidth="1"/>
     <col min="3" max="3" width="104.458333333333" style="2" customWidth="1"/>
     <col min="4" max="4" width="105.541666666667" style="2" customWidth="1"/>
     <col min="5" max="5" width="118.583333333333" style="2" customWidth="1"/>
@@ -12833,10 +12869,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
-      <c r="A1" s="6" t="s">
+      <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="7" t="s">
+      <c r="B1" s="8" t="s">
         <v>1</v>
       </c>
       <c r="C1" s="3" t="s">
@@ -12845,2731 +12881,2743 @@
       <c r="D1" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="8" t="s">
+      <c r="E1" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="8" t="s">
+      <c r="F1" s="9" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="2" spans="1:6">
-      <c r="A2" s="6" t="s">
+      <c r="A2" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="B2" s="7"/>
+      <c r="B2" s="8"/>
       <c r="C2" s="3"/>
       <c r="D2" s="3"/>
-      <c r="E2" s="8"/>
-      <c r="F2" s="8"/>
+      <c r="E2" s="9"/>
+      <c r="F2" s="9"/>
     </row>
     <row r="3" s="1" customFormat="1" ht="17.25" spans="1:6">
-      <c r="A3" s="9" t="s">
+      <c r="A3" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="B3" s="10"/>
-      <c r="C3" s="11"/>
-      <c r="D3" s="11"/>
-      <c r="E3" s="12"/>
-      <c r="F3" s="12"/>
+      <c r="B3" s="11"/>
+      <c r="C3" s="12"/>
+      <c r="D3" s="12"/>
+      <c r="E3" s="13"/>
+      <c r="F3" s="13"/>
     </row>
     <row r="4" spans="1:6">
-      <c r="A4" s="13" t="s">
+      <c r="A4" s="14" t="s">
         <v>8</v>
       </c>
-      <c r="B4" s="14" t="s">
+      <c r="B4" s="15" t="s">
         <v>9</v>
       </c>
-      <c r="C4" s="8" t="s">
+      <c r="C4" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="D4" s="8" t="s">
+      <c r="D4" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="E4" s="8" t="s">
+      <c r="E4" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="F4" s="8" t="s">
+      <c r="F4" s="9" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="5" spans="1:6">
-      <c r="A5" s="13" t="s">
+      <c r="A5" s="14" t="s">
         <v>14</v>
       </c>
-      <c r="B5" s="14" t="s">
+      <c r="B5" s="15" t="s">
         <v>15</v>
       </c>
-      <c r="C5" s="8" t="s">
+      <c r="C5" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="D5" s="8" t="s">
+      <c r="D5" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="E5" s="8" t="s">
+      <c r="E5" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="F5" s="8" t="s">
+      <c r="F5" s="9" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="6" spans="1:6">
-      <c r="A6" s="13" t="s">
+      <c r="A6" s="14" t="s">
         <v>20</v>
       </c>
-      <c r="B6" s="14" t="s">
+      <c r="B6" s="15" t="s">
         <v>21</v>
       </c>
-      <c r="C6" s="8" t="s">
+      <c r="C6" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="D6" s="8" t="s">
+      <c r="D6" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="E6" s="8" t="s">
+      <c r="E6" s="9" t="s">
         <v>24</v>
       </c>
-      <c r="F6" s="8" t="s">
+      <c r="F6" s="9" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="7" spans="1:6">
-      <c r="A7" s="13" t="s">
+      <c r="A7" s="14" t="s">
         <v>26</v>
       </c>
-      <c r="B7" s="14" t="s">
+      <c r="B7" s="15" t="s">
         <v>27</v>
       </c>
-      <c r="C7" s="8" t="s">
+      <c r="C7" s="9" t="s">
         <v>28</v>
       </c>
-      <c r="D7" s="8" t="s">
+      <c r="D7" s="9" t="s">
         <v>29</v>
       </c>
-      <c r="E7" s="8" t="s">
+      <c r="E7" s="9" t="s">
         <v>30</v>
       </c>
-      <c r="F7" s="8" t="s">
+      <c r="F7" s="9" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="8" spans="1:6">
-      <c r="A8" s="13" t="s">
+      <c r="A8" s="14" t="s">
         <v>32</v>
       </c>
-      <c r="B8" s="14" t="s">
+      <c r="B8" s="15" t="s">
         <v>33</v>
       </c>
-      <c r="C8" s="8" t="s">
+      <c r="C8" s="9" t="s">
         <v>34</v>
       </c>
-      <c r="D8" s="8" t="s">
+      <c r="D8" s="9" t="s">
         <v>35</v>
       </c>
-      <c r="E8" s="8" t="s">
+      <c r="E8" s="9" t="s">
         <v>36</v>
       </c>
-      <c r="F8" s="8" t="s">
+      <c r="F8" s="9" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="9" spans="1:6">
-      <c r="A9" s="13" t="s">
+      <c r="A9" s="14" t="s">
         <v>38</v>
       </c>
-      <c r="B9" s="14" t="s">
+      <c r="B9" s="15" t="s">
         <v>39</v>
       </c>
-      <c r="C9" s="8" t="s">
+      <c r="C9" s="9" t="s">
         <v>40</v>
       </c>
-      <c r="D9" s="8" t="s">
+      <c r="D9" s="9" t="s">
         <v>41</v>
       </c>
-      <c r="E9" s="8" t="s">
+      <c r="E9" s="9" t="s">
         <v>42</v>
       </c>
-      <c r="F9" s="8" t="s">
+      <c r="F9" s="9" t="s">
         <v>43</v>
       </c>
     </row>
     <row r="10" spans="1:6">
-      <c r="A10" s="13" t="s">
+      <c r="A10" s="14" t="s">
         <v>44</v>
       </c>
-      <c r="B10" s="14" t="s">
+      <c r="B10" s="15" t="s">
         <v>45</v>
       </c>
-      <c r="C10" s="8" t="s">
+      <c r="C10" s="9" t="s">
         <v>46</v>
       </c>
-      <c r="D10" s="8" t="s">
+      <c r="D10" s="9" t="s">
         <v>47</v>
       </c>
-      <c r="E10" s="8" t="s">
+      <c r="E10" s="9" t="s">
         <v>48</v>
       </c>
-      <c r="F10" s="8" t="s">
+      <c r="F10" s="9" t="s">
         <v>49</v>
       </c>
     </row>
     <row r="11" spans="1:6">
-      <c r="A11" s="13" t="s">
+      <c r="A11" s="14" t="s">
         <v>50</v>
       </c>
-      <c r="B11" s="14" t="s">
+      <c r="B11" s="15" t="s">
         <v>51</v>
       </c>
-      <c r="C11" s="8" t="s">
+      <c r="C11" s="9" t="s">
         <v>52</v>
       </c>
-      <c r="D11" s="8" t="s">
+      <c r="D11" s="9" t="s">
         <v>53</v>
       </c>
-      <c r="E11" s="8" t="s">
+      <c r="E11" s="9" t="s">
         <v>54</v>
       </c>
-      <c r="F11" s="8" t="s">
+      <c r="F11" s="9" t="s">
         <v>55</v>
       </c>
     </row>
     <row r="12" spans="1:6">
-      <c r="A12" s="13" t="s">
+      <c r="A12" s="14" t="s">
         <v>56</v>
       </c>
-      <c r="B12" s="14" t="s">
+      <c r="B12" s="15" t="s">
         <v>57</v>
       </c>
-      <c r="C12" s="8" t="s">
+      <c r="C12" s="9" t="s">
         <v>58</v>
       </c>
-      <c r="D12" s="8" t="s">
+      <c r="D12" s="9" t="s">
         <v>59</v>
       </c>
-      <c r="E12" s="8" t="s">
+      <c r="E12" s="9" t="s">
         <v>60</v>
       </c>
-      <c r="F12" s="8" t="s">
+      <c r="F12" s="9" t="s">
         <v>61</v>
       </c>
     </row>
     <row r="13" spans="1:6">
-      <c r="A13" s="13" t="s">
+      <c r="A13" s="14" t="s">
         <v>62</v>
       </c>
-      <c r="B13" s="14" t="s">
+      <c r="B13" s="15" t="s">
         <v>63</v>
       </c>
-      <c r="C13" s="8" t="s">
+      <c r="C13" s="9" t="s">
         <v>64</v>
       </c>
-      <c r="D13" s="8" t="s">
+      <c r="D13" s="9" t="s">
         <v>65</v>
       </c>
-      <c r="E13" s="8" t="s">
+      <c r="E13" s="9" t="s">
         <v>66</v>
       </c>
-      <c r="F13" s="8" t="s">
+      <c r="F13" s="9" t="s">
         <v>63</v>
       </c>
     </row>
     <row r="14" spans="1:6">
-      <c r="A14" s="13" t="s">
+      <c r="A14" s="14" t="s">
         <v>67</v>
       </c>
-      <c r="B14" s="14" t="s">
+      <c r="B14" s="15" t="s">
         <v>68</v>
       </c>
-      <c r="C14" s="8" t="s">
+      <c r="C14" s="9" t="s">
         <v>69</v>
       </c>
-      <c r="D14" s="8" t="s">
+      <c r="D14" s="9" t="s">
         <v>70</v>
       </c>
-      <c r="E14" s="8" t="s">
+      <c r="E14" s="9" t="s">
         <v>71</v>
       </c>
-      <c r="F14" s="8" t="s">
+      <c r="F14" s="9" t="s">
         <v>72</v>
       </c>
     </row>
     <row r="15" spans="1:6">
-      <c r="A15" s="13" t="s">
+      <c r="A15" s="14" t="s">
         <v>73</v>
       </c>
-      <c r="B15" s="14" t="s">
+      <c r="B15" s="15" t="s">
         <v>73</v>
       </c>
-      <c r="C15" s="8" t="s">
+      <c r="C15" s="9" t="s">
         <v>74</v>
       </c>
-      <c r="D15" s="8" t="s">
+      <c r="D15" s="9" t="s">
         <v>75</v>
       </c>
-      <c r="E15" s="8" t="s">
+      <c r="E15" s="9" t="s">
         <v>76</v>
       </c>
-      <c r="F15" s="8" t="s">
+      <c r="F15" s="9" t="s">
         <v>77</v>
       </c>
     </row>
     <row r="16" spans="1:6">
-      <c r="A16" s="13" t="s">
+      <c r="A16" s="14" t="s">
         <v>78</v>
       </c>
-      <c r="B16" s="14" t="s">
+      <c r="B16" s="15" t="s">
         <v>79</v>
       </c>
-      <c r="C16" s="8" t="s">
+      <c r="C16" s="9" t="s">
         <v>79</v>
       </c>
-      <c r="D16" s="8" t="s">
+      <c r="D16" s="9" t="s">
         <v>79</v>
       </c>
-      <c r="E16" s="14" t="s">
+      <c r="E16" s="15" t="s">
         <v>79</v>
       </c>
-      <c r="F16" s="14" t="s">
+      <c r="F16" s="15" t="s">
         <v>79</v>
       </c>
     </row>
     <row r="17" spans="1:6">
-      <c r="A17" s="13" t="s">
+      <c r="A17" s="14" t="s">
         <v>80</v>
       </c>
-      <c r="B17" s="14" t="s">
+      <c r="B17" s="15" t="s">
         <v>81</v>
       </c>
-      <c r="C17" s="8" t="s">
+      <c r="C17" s="9" t="s">
         <v>81</v>
       </c>
-      <c r="D17" s="8" t="s">
+      <c r="D17" s="9" t="s">
         <v>81</v>
       </c>
-      <c r="E17" s="14" t="s">
+      <c r="E17" s="15" t="s">
         <v>81</v>
       </c>
-      <c r="F17" s="14" t="s">
+      <c r="F17" s="15" t="s">
         <v>81</v>
       </c>
     </row>
     <row r="18" spans="1:6">
-      <c r="A18" s="13" t="s">
+      <c r="A18" s="14" t="s">
         <v>82</v>
       </c>
-      <c r="B18" s="14" t="s">
+      <c r="B18" s="15" t="s">
         <v>83</v>
       </c>
-      <c r="C18" s="8" t="s">
+      <c r="C18" s="9" t="s">
         <v>84</v>
       </c>
-      <c r="D18" s="8" t="s">
+      <c r="D18" s="9" t="s">
         <v>85</v>
       </c>
-      <c r="E18" s="8" t="s">
+      <c r="E18" s="9" t="s">
         <v>86</v>
       </c>
-      <c r="F18" s="8" t="s">
+      <c r="F18" s="9" t="s">
         <v>87</v>
       </c>
     </row>
     <row r="19" spans="1:6">
-      <c r="A19" s="13" t="s">
+      <c r="A19" s="14" t="s">
         <v>88</v>
       </c>
-      <c r="B19" s="14" t="s">
+      <c r="B19" s="15" t="s">
         <v>89</v>
       </c>
-      <c r="C19" s="8" t="s">
+      <c r="C19" s="9" t="s">
         <v>90</v>
       </c>
-      <c r="D19" s="8" t="s">
+      <c r="D19" s="9" t="s">
         <v>91</v>
       </c>
-      <c r="E19" s="8" t="s">
+      <c r="E19" s="9" t="s">
         <v>92</v>
       </c>
-      <c r="F19" s="8" t="s">
+      <c r="F19" s="9" t="s">
         <v>93</v>
       </c>
     </row>
     <row r="20" spans="1:6">
-      <c r="A20" s="13" t="s">
+      <c r="A20" s="14" t="s">
         <v>94</v>
       </c>
-      <c r="B20" s="14" t="s">
+      <c r="B20" s="15" t="s">
         <v>95</v>
       </c>
-      <c r="C20" s="8" t="s">
+      <c r="C20" s="9" t="s">
         <v>96</v>
       </c>
-      <c r="D20" s="8" t="s">
+      <c r="D20" s="9" t="s">
         <v>97</v>
       </c>
-      <c r="E20" s="8" t="s">
+      <c r="E20" s="9" t="s">
         <v>98</v>
       </c>
-      <c r="F20" s="8" t="s">
+      <c r="F20" s="9" t="s">
         <v>99</v>
       </c>
     </row>
     <row r="21" spans="1:6">
-      <c r="A21" s="13" t="s">
+      <c r="A21" s="14" t="s">
         <v>100</v>
       </c>
-      <c r="B21" s="14" t="s">
+      <c r="B21" s="15" t="s">
         <v>101</v>
       </c>
-      <c r="C21" s="8" t="s">
+      <c r="C21" s="9" t="s">
         <v>102</v>
       </c>
-      <c r="D21" s="8" t="s">
+      <c r="D21" s="9" t="s">
         <v>103</v>
       </c>
-      <c r="E21" s="8" t="s">
+      <c r="E21" s="9" t="s">
         <v>104</v>
       </c>
-      <c r="F21" s="8" t="s">
+      <c r="F21" s="9" t="s">
         <v>105</v>
       </c>
     </row>
     <row r="22" spans="1:6">
-      <c r="A22" s="13" t="s">
+      <c r="A22" s="14" t="s">
         <v>106</v>
       </c>
-      <c r="B22" s="14" t="s">
+      <c r="B22" s="15" t="s">
         <v>107</v>
       </c>
-      <c r="C22" s="8" t="s">
+      <c r="C22" s="9" t="s">
         <v>108</v>
       </c>
-      <c r="D22" s="8" t="s">
+      <c r="D22" s="9" t="s">
         <v>109</v>
       </c>
-      <c r="E22" s="8" t="s">
+      <c r="E22" s="9" t="s">
         <v>110</v>
       </c>
-      <c r="F22" s="8" t="s">
+      <c r="F22" s="9" t="s">
         <v>111</v>
       </c>
     </row>
     <row r="23" spans="1:6">
-      <c r="A23" s="13" t="s">
+      <c r="A23" s="14" t="s">
         <v>112</v>
       </c>
-      <c r="B23" s="14" t="s">
+      <c r="B23" s="15" t="s">
         <v>112</v>
       </c>
-      <c r="C23" s="8" t="s">
+      <c r="C23" s="9" t="s">
         <v>113</v>
       </c>
-      <c r="D23" s="8" t="s">
+      <c r="D23" s="9" t="s">
         <v>114</v>
       </c>
-      <c r="E23" s="8" t="s">
+      <c r="E23" s="9" t="s">
         <v>115</v>
       </c>
-      <c r="F23" s="8" t="s">
+      <c r="F23" s="9" t="s">
         <v>116</v>
       </c>
     </row>
     <row r="24" spans="1:6">
-      <c r="A24" s="13" t="s">
+      <c r="A24" s="14" t="s">
         <v>117</v>
       </c>
-      <c r="B24" s="14" t="s">
+      <c r="B24" s="15" t="s">
         <v>118</v>
       </c>
-      <c r="C24" s="8" t="s">
+      <c r="C24" s="9" t="s">
         <v>119</v>
       </c>
-      <c r="D24" s="8" t="s">
+      <c r="D24" s="9" t="s">
         <v>120</v>
       </c>
-      <c r="E24" s="8" t="s">
+      <c r="E24" s="9" t="s">
         <v>121</v>
       </c>
-      <c r="F24" s="8" t="s">
+      <c r="F24" s="9" t="s">
         <v>118</v>
       </c>
     </row>
     <row r="25" spans="1:6">
-      <c r="A25" s="13" t="s">
+      <c r="A25" s="14" t="s">
         <v>122</v>
       </c>
-      <c r="B25" s="14" t="s">
+      <c r="B25" s="15" t="s">
         <v>123</v>
       </c>
-      <c r="C25" s="8" t="s">
+      <c r="C25" s="9" t="s">
         <v>124</v>
       </c>
-      <c r="D25" s="8" t="s">
+      <c r="D25" s="9" t="s">
         <v>125</v>
       </c>
-      <c r="E25" s="8" t="s">
+      <c r="E25" s="9" t="s">
         <v>126</v>
       </c>
-      <c r="F25" s="8" t="s">
+      <c r="F25" s="9" t="s">
         <v>127</v>
       </c>
     </row>
     <row r="26" spans="1:6">
-      <c r="A26" s="13" t="s">
+      <c r="A26" s="14" t="s">
         <v>128</v>
       </c>
-      <c r="B26" s="14" t="s">
+      <c r="B26" s="15" t="s">
         <v>129</v>
       </c>
-      <c r="C26" s="8" t="s">
+      <c r="C26" s="9" t="s">
         <v>130</v>
       </c>
-      <c r="D26" s="8" t="s">
+      <c r="D26" s="9" t="s">
         <v>131</v>
       </c>
-      <c r="E26" s="8" t="s">
+      <c r="E26" s="9" t="s">
         <v>132</v>
       </c>
-      <c r="F26" s="8" t="s">
+      <c r="F26" s="9" t="s">
         <v>133</v>
       </c>
     </row>
     <row r="27" spans="1:6">
-      <c r="A27" s="13" t="s">
+      <c r="A27" s="14" t="s">
         <v>134</v>
       </c>
-      <c r="B27" s="14" t="s">
+      <c r="B27" s="15" t="s">
         <v>135</v>
       </c>
-      <c r="C27" s="8" t="s">
+      <c r="C27" s="9" t="s">
         <v>136</v>
       </c>
-      <c r="D27" s="8" t="s">
+      <c r="D27" s="9" t="s">
         <v>137</v>
       </c>
-      <c r="E27" s="8" t="s">
+      <c r="E27" s="9" t="s">
         <v>138</v>
       </c>
-      <c r="F27" s="8" t="s">
+      <c r="F27" s="9" t="s">
         <v>139</v>
       </c>
     </row>
     <row r="28" spans="1:6">
-      <c r="A28" s="13" t="s">
+      <c r="A28" s="14" t="s">
         <v>140</v>
       </c>
-      <c r="B28" s="14" t="s">
+      <c r="B28" s="15" t="s">
         <v>141</v>
       </c>
-      <c r="C28" s="8" t="s">
+      <c r="C28" s="9" t="s">
         <v>142</v>
       </c>
-      <c r="D28" s="8" t="s">
+      <c r="D28" s="9" t="s">
         <v>143</v>
       </c>
-      <c r="E28" s="8" t="s">
+      <c r="E28" s="9" t="s">
         <v>144</v>
       </c>
-      <c r="F28" s="8" t="s">
+      <c r="F28" s="9" t="s">
         <v>145</v>
       </c>
     </row>
     <row r="29" spans="1:6">
-      <c r="A29" s="13" t="s">
+      <c r="A29" s="14" t="s">
         <v>146</v>
       </c>
-      <c r="B29" s="14" t="s">
+      <c r="B29" s="15" t="s">
         <v>147</v>
       </c>
-      <c r="C29" s="8" t="s">
+      <c r="C29" s="9" t="s">
         <v>148</v>
       </c>
-      <c r="D29" s="8" t="s">
+      <c r="D29" s="9" t="s">
         <v>149</v>
       </c>
-      <c r="E29" s="8" t="s">
+      <c r="E29" s="9" t="s">
         <v>150</v>
       </c>
-      <c r="F29" s="8" t="s">
+      <c r="F29" s="9" t="s">
         <v>151</v>
       </c>
     </row>
     <row r="30" spans="1:6">
-      <c r="A30" s="13" t="s">
+      <c r="A30" s="14" t="s">
         <v>152</v>
       </c>
-      <c r="B30" s="14" t="s">
+      <c r="B30" s="15" t="s">
         <v>153</v>
       </c>
-      <c r="C30" s="8" t="s">
+      <c r="C30" s="9" t="s">
         <v>154</v>
       </c>
-      <c r="D30" s="8" t="s">
+      <c r="D30" s="9" t="s">
         <v>155</v>
       </c>
-      <c r="E30" s="8" t="s">
+      <c r="E30" s="9" t="s">
         <v>156</v>
       </c>
-      <c r="F30" s="8" t="s">
+      <c r="F30" s="9" t="s">
         <v>157</v>
       </c>
     </row>
     <row r="31" spans="1:6">
-      <c r="A31" s="13" t="s">
+      <c r="A31" s="14" t="s">
         <v>158</v>
       </c>
-      <c r="B31" s="14" t="s">
+      <c r="B31" s="15" t="s">
         <v>159</v>
       </c>
-      <c r="C31" s="8" t="s">
+      <c r="C31" s="9" t="s">
         <v>160</v>
       </c>
-      <c r="D31" s="8" t="s">
+      <c r="D31" s="9" t="s">
         <v>161</v>
       </c>
-      <c r="E31" s="8" t="s">
+      <c r="E31" s="9" t="s">
         <v>162</v>
       </c>
-      <c r="F31" s="8" t="s">
+      <c r="F31" s="9" t="s">
         <v>163</v>
       </c>
     </row>
     <row r="32" spans="1:6">
-      <c r="A32" s="13" t="s">
+      <c r="A32" s="14" t="s">
         <v>164</v>
       </c>
-      <c r="B32" s="14" t="s">
+      <c r="B32" s="15" t="s">
         <v>165</v>
       </c>
-      <c r="C32" s="8" t="s">
+      <c r="C32" s="9" t="s">
         <v>166</v>
       </c>
-      <c r="D32" s="8" t="s">
+      <c r="D32" s="9" t="s">
         <v>167</v>
       </c>
-      <c r="E32" s="8" t="s">
+      <c r="E32" s="9" t="s">
         <v>168</v>
       </c>
-      <c r="F32" s="8" t="s">
+      <c r="F32" s="9" t="s">
         <v>169</v>
       </c>
     </row>
     <row r="33" ht="33" spans="1:6">
-      <c r="A33" s="13" t="s">
+      <c r="A33" s="14" t="s">
         <v>170</v>
       </c>
-      <c r="B33" s="14" t="s">
+      <c r="B33" s="15" t="s">
         <v>171</v>
       </c>
-      <c r="C33" s="15" t="s">
+      <c r="C33" s="16" t="s">
         <v>172</v>
       </c>
-      <c r="D33" s="15" t="s">
+      <c r="D33" s="16" t="s">
         <v>173</v>
       </c>
-      <c r="E33" s="15" t="s">
+      <c r="E33" s="16" t="s">
         <v>174</v>
       </c>
-      <c r="F33" s="15" t="s">
+      <c r="F33" s="16" t="s">
         <v>175</v>
       </c>
     </row>
     <row r="34" spans="1:6">
-      <c r="A34" s="13" t="s">
+      <c r="A34" s="14" t="s">
         <v>176</v>
       </c>
-      <c r="B34" s="14" t="s">
+      <c r="B34" s="15" t="s">
         <v>177</v>
       </c>
-      <c r="C34" s="8" t="s">
+      <c r="C34" s="9" t="s">
         <v>178</v>
       </c>
-      <c r="D34" s="8" t="s">
+      <c r="D34" s="9" t="s">
         <v>179</v>
       </c>
-      <c r="E34" s="8" t="s">
+      <c r="E34" s="9" t="s">
         <v>180</v>
       </c>
-      <c r="F34" s="8" t="s">
+      <c r="F34" s="9" t="s">
         <v>181</v>
       </c>
     </row>
     <row r="35" spans="1:6">
-      <c r="A35" s="13" t="s">
+      <c r="A35" s="14" t="s">
         <v>182</v>
       </c>
-      <c r="B35" s="14" t="s">
+      <c r="B35" s="15" t="s">
         <v>183</v>
       </c>
-      <c r="C35" s="8" t="s">
+      <c r="C35" s="9" t="s">
         <v>184</v>
       </c>
-      <c r="D35" s="8" t="s">
+      <c r="D35" s="9" t="s">
         <v>185</v>
       </c>
-      <c r="E35" s="8" t="s">
+      <c r="E35" s="9" t="s">
         <v>186</v>
       </c>
-      <c r="F35" s="8" t="s">
+      <c r="F35" s="9" t="s">
         <v>187</v>
       </c>
     </row>
     <row r="36" spans="1:6">
-      <c r="A36" s="13" t="s">
+      <c r="A36" s="14" t="s">
         <v>188</v>
       </c>
-      <c r="B36" s="14" t="s">
+      <c r="B36" s="15" t="s">
         <v>189</v>
       </c>
-      <c r="C36" s="8" t="s">
+      <c r="C36" s="9" t="s">
         <v>190</v>
       </c>
-      <c r="D36" s="8" t="s">
+      <c r="D36" s="9" t="s">
         <v>191</v>
       </c>
-      <c r="E36" s="8" t="s">
+      <c r="E36" s="9" t="s">
         <v>192</v>
       </c>
-      <c r="F36" s="8" t="s">
+      <c r="F36" s="9" t="s">
         <v>193</v>
       </c>
     </row>
     <row r="37" spans="1:6">
-      <c r="A37" s="13" t="s">
+      <c r="A37" s="14" t="s">
         <v>194</v>
       </c>
-      <c r="B37" s="14" t="s">
+      <c r="B37" s="15" t="s">
         <v>195</v>
       </c>
-      <c r="C37" s="8" t="s">
+      <c r="C37" s="9" t="s">
         <v>196</v>
       </c>
-      <c r="D37" s="8" t="s">
+      <c r="D37" s="9" t="s">
         <v>197</v>
       </c>
-      <c r="E37" s="8" t="s">
+      <c r="E37" s="9" t="s">
         <v>198</v>
       </c>
-      <c r="F37" s="8" t="s">
+      <c r="F37" s="9" t="s">
         <v>199</v>
       </c>
     </row>
     <row r="38" spans="1:6">
-      <c r="A38" s="13" t="s">
+      <c r="A38" s="14" t="s">
         <v>200</v>
       </c>
-      <c r="B38" s="14" t="s">
+      <c r="B38" s="15" t="s">
         <v>200</v>
       </c>
-      <c r="C38" s="8" t="s">
+      <c r="C38" s="9" t="s">
         <v>201</v>
       </c>
-      <c r="D38" s="8" t="s">
+      <c r="D38" s="9" t="s">
         <v>202</v>
       </c>
-      <c r="E38" s="8" t="s">
+      <c r="E38" s="9" t="s">
         <v>203</v>
       </c>
-      <c r="F38" s="8" t="s">
+      <c r="F38" s="9" t="s">
         <v>204</v>
       </c>
     </row>
     <row r="39" spans="1:6">
-      <c r="A39" s="13" t="s">
+      <c r="A39" s="14" t="s">
         <v>205</v>
       </c>
-      <c r="B39" s="14" t="s">
+      <c r="B39" s="15" t="s">
         <v>206</v>
       </c>
-      <c r="C39" s="8" t="s">
+      <c r="C39" s="9" t="s">
         <v>207</v>
       </c>
-      <c r="D39" s="8" t="s">
+      <c r="D39" s="9" t="s">
         <v>208</v>
       </c>
-      <c r="E39" s="8" t="s">
+      <c r="E39" s="9" t="s">
         <v>209</v>
       </c>
-      <c r="F39" s="8" t="s">
+      <c r="F39" s="9" t="s">
         <v>210</v>
       </c>
     </row>
     <row r="40" spans="1:6">
-      <c r="A40" s="13" t="s">
+      <c r="A40" s="14" t="s">
         <v>211</v>
       </c>
-      <c r="B40" s="14" t="s">
+      <c r="B40" s="15" t="s">
         <v>212</v>
       </c>
-      <c r="C40" s="8" t="s">
+      <c r="C40" s="9" t="s">
         <v>213</v>
       </c>
-      <c r="D40" s="8" t="s">
+      <c r="D40" s="9" t="s">
         <v>214</v>
       </c>
-      <c r="E40" s="8" t="s">
+      <c r="E40" s="9" t="s">
         <v>215</v>
       </c>
-      <c r="F40" s="8" t="s">
+      <c r="F40" s="9" t="s">
         <v>212</v>
       </c>
     </row>
     <row r="41" spans="1:6">
-      <c r="A41" s="13" t="s">
+      <c r="A41" s="14" t="s">
         <v>216</v>
       </c>
-      <c r="B41" s="14" t="s">
+      <c r="B41" s="15" t="s">
         <v>217</v>
       </c>
-      <c r="C41" s="8" t="s">
+      <c r="C41" s="9" t="s">
         <v>218</v>
       </c>
-      <c r="D41" s="8" t="s">
+      <c r="D41" s="9" t="s">
         <v>219</v>
       </c>
-      <c r="E41" s="8" t="s">
+      <c r="E41" s="9" t="s">
         <v>220</v>
       </c>
-      <c r="F41" s="8" t="s">
+      <c r="F41" s="9" t="s">
         <v>221</v>
       </c>
     </row>
     <row r="42" spans="1:6">
-      <c r="A42" s="13" t="s">
+      <c r="A42" s="14" t="s">
         <v>222</v>
       </c>
-      <c r="B42" s="14" t="s">
+      <c r="B42" s="15" t="s">
         <v>223</v>
       </c>
-      <c r="C42" s="16" t="s">
+      <c r="C42" s="17" t="s">
         <v>224</v>
       </c>
-      <c r="D42" s="16" t="s">
+      <c r="D42" s="17" t="s">
         <v>225</v>
       </c>
-      <c r="E42" s="8" t="s">
+      <c r="E42" s="9" t="s">
         <v>226</v>
       </c>
-      <c r="F42" s="8" t="s">
+      <c r="F42" s="9" t="s">
         <v>227</v>
       </c>
     </row>
     <row r="43" s="2" customFormat="1" spans="1:6">
-      <c r="A43" s="4" t="s">
+      <c r="A43" s="5" t="s">
         <v>228</v>
       </c>
-      <c r="B43" s="17" t="s">
+      <c r="B43" s="18" t="s">
         <v>229</v>
       </c>
-      <c r="C43" s="18" t="s">
+      <c r="C43" s="19" t="s">
         <v>230</v>
       </c>
-      <c r="D43" s="18" t="s">
+      <c r="D43" s="19" t="s">
         <v>231</v>
       </c>
-      <c r="E43" s="18" t="s">
+      <c r="E43" s="19" t="s">
         <v>232</v>
       </c>
-      <c r="F43" s="19" t="s">
+      <c r="F43" s="20" t="s">
         <v>233</v>
       </c>
     </row>
     <row r="44" spans="1:6">
-      <c r="A44" s="13" t="s">
+      <c r="A44" s="14" t="s">
         <v>234</v>
       </c>
-      <c r="B44" s="14" t="s">
+      <c r="B44" s="15" t="s">
         <v>235</v>
       </c>
-      <c r="C44" s="8" t="s">
+      <c r="C44" s="9" t="s">
         <v>236</v>
       </c>
-      <c r="D44" s="8" t="s">
+      <c r="D44" s="9" t="s">
         <v>237</v>
       </c>
-      <c r="E44" s="8" t="s">
+      <c r="E44" s="9" t="s">
         <v>238</v>
       </c>
-      <c r="F44" s="8" t="s">
+      <c r="F44" s="9" t="s">
         <v>235</v>
       </c>
     </row>
     <row r="45" spans="1:6">
-      <c r="A45" s="13" t="s">
+      <c r="A45" s="14" t="s">
         <v>239</v>
       </c>
-      <c r="B45" s="14" t="s">
+      <c r="B45" s="15" t="s">
         <v>240</v>
       </c>
-      <c r="C45" s="8" t="s">
+      <c r="C45" s="9" t="s">
         <v>241</v>
       </c>
-      <c r="D45" s="8" t="s">
+      <c r="D45" s="9" t="s">
         <v>242</v>
       </c>
-      <c r="E45" s="8" t="s">
+      <c r="E45" s="9" t="s">
         <v>243</v>
       </c>
-      <c r="F45" s="8" t="s">
+      <c r="F45" s="9" t="s">
         <v>244</v>
       </c>
     </row>
     <row r="46" spans="1:6">
-      <c r="A46" s="13" t="s">
+      <c r="A46" s="14" t="s">
         <v>245</v>
       </c>
-      <c r="B46" s="14" t="s">
+      <c r="B46" s="15" t="s">
         <v>246</v>
       </c>
-      <c r="C46" s="8" t="s">
+      <c r="C46" s="9" t="s">
         <v>247</v>
       </c>
-      <c r="D46" s="8" t="s">
+      <c r="D46" s="9" t="s">
         <v>248</v>
       </c>
-      <c r="E46" s="8" t="s">
+      <c r="E46" s="9" t="s">
         <v>249</v>
       </c>
-      <c r="F46" s="8" t="s">
+      <c r="F46" s="9" t="s">
         <v>250</v>
       </c>
     </row>
     <row r="47" spans="1:6">
-      <c r="A47" s="13" t="s">
+      <c r="A47" s="14" t="s">
         <v>251</v>
       </c>
-      <c r="B47" s="14" t="s">
+      <c r="B47" s="15" t="s">
         <v>252</v>
       </c>
-      <c r="C47" s="8" t="s">
+      <c r="C47" s="9" t="s">
         <v>253</v>
       </c>
-      <c r="D47" s="8" t="s">
+      <c r="D47" s="9" t="s">
         <v>254</v>
       </c>
-      <c r="E47" s="8" t="s">
+      <c r="E47" s="9" t="s">
         <v>255</v>
       </c>
-      <c r="F47" s="8" t="s">
+      <c r="F47" s="9" t="s">
         <v>256</v>
       </c>
     </row>
     <row r="48" spans="1:6">
-      <c r="A48" s="13" t="s">
+      <c r="A48" s="14" t="s">
         <v>257</v>
       </c>
-      <c r="B48" s="14" t="s">
+      <c r="B48" s="15" t="s">
         <v>258</v>
       </c>
-      <c r="C48" s="8" t="s">
+      <c r="C48" s="9" t="s">
         <v>259</v>
       </c>
-      <c r="D48" s="8" t="s">
+      <c r="D48" s="9" t="s">
         <v>260</v>
       </c>
-      <c r="E48" s="8" t="s">
+      <c r="E48" s="9" t="s">
         <v>261</v>
       </c>
-      <c r="F48" s="8" t="s">
+      <c r="F48" s="9" t="s">
         <v>262</v>
       </c>
     </row>
     <row r="49" spans="1:6">
-      <c r="A49" s="13" t="s">
+      <c r="A49" s="14" t="s">
         <v>263</v>
       </c>
-      <c r="B49" s="14" t="s">
+      <c r="B49" s="15" t="s">
         <v>264</v>
       </c>
-      <c r="C49" s="16" t="s">
+      <c r="C49" s="17" t="s">
         <v>265</v>
       </c>
-      <c r="D49" s="16" t="s">
+      <c r="D49" s="17" t="s">
         <v>266</v>
       </c>
-      <c r="E49" s="8" t="s">
+      <c r="E49" s="9" t="s">
         <v>267</v>
       </c>
-      <c r="F49" s="8" t="s">
+      <c r="F49" s="9" t="s">
         <v>268</v>
       </c>
     </row>
     <row r="50" spans="1:6">
-      <c r="A50" s="13" t="s">
+      <c r="A50" s="14" t="s">
         <v>269</v>
       </c>
-      <c r="B50" s="14" t="s">
+      <c r="B50" s="15" t="s">
         <v>270</v>
       </c>
-      <c r="C50" s="8" t="s">
+      <c r="C50" s="9" t="s">
         <v>271</v>
       </c>
-      <c r="D50" s="8" t="s">
+      <c r="D50" s="9" t="s">
         <v>272</v>
       </c>
-      <c r="E50" s="8" t="s">
+      <c r="E50" s="9" t="s">
         <v>273</v>
       </c>
-      <c r="F50" s="8" t="s">
+      <c r="F50" s="9" t="s">
         <v>274</v>
       </c>
     </row>
     <row r="51" spans="1:6">
-      <c r="A51" s="13" t="s">
+      <c r="A51" s="14" t="s">
         <v>275</v>
       </c>
-      <c r="B51" s="14" t="s">
+      <c r="B51" s="15" t="s">
         <v>276</v>
       </c>
-      <c r="C51" s="8" t="s">
+      <c r="C51" s="9" t="s">
         <v>277</v>
       </c>
-      <c r="D51" s="8" t="s">
+      <c r="D51" s="9" t="s">
         <v>248</v>
       </c>
-      <c r="E51" s="8" t="s">
+      <c r="E51" s="9" t="s">
         <v>249</v>
       </c>
-      <c r="F51" s="8" t="s">
+      <c r="F51" s="9" t="s">
         <v>276</v>
       </c>
     </row>
     <row r="52" s="2" customFormat="1" spans="1:6">
-      <c r="A52" s="13" t="s">
+      <c r="A52" s="14" t="s">
         <v>278</v>
       </c>
-      <c r="B52" s="14" t="s">
+      <c r="B52" s="15" t="s">
         <v>279</v>
       </c>
-      <c r="C52" s="8" t="s">
+      <c r="C52" s="9" t="s">
         <v>280</v>
       </c>
-      <c r="D52" s="8" t="s">
+      <c r="D52" s="9" t="s">
         <v>281</v>
       </c>
-      <c r="E52" s="20" t="s">
+      <c r="E52" s="21" t="s">
         <v>282</v>
       </c>
-      <c r="F52" s="8" t="s">
+      <c r="F52" s="9" t="s">
         <v>283</v>
       </c>
     </row>
     <row r="53" spans="1:6">
-      <c r="A53" s="13" t="s">
+      <c r="A53" s="14" t="s">
         <v>284</v>
       </c>
-      <c r="B53" s="14" t="s">
+      <c r="B53" s="15" t="s">
         <v>285</v>
       </c>
-      <c r="C53" s="16" t="s">
+      <c r="C53" s="17" t="s">
         <v>286</v>
       </c>
-      <c r="D53" s="16" t="s">
+      <c r="D53" s="17" t="s">
         <v>231</v>
       </c>
-      <c r="E53" s="8" t="s">
+      <c r="E53" s="9" t="s">
         <v>287</v>
       </c>
-      <c r="F53" s="8" t="s">
+      <c r="F53" s="9" t="s">
         <v>288</v>
       </c>
     </row>
     <row r="54" spans="1:6">
-      <c r="A54" s="13" t="s">
+      <c r="A54" s="14" t="s">
         <v>289</v>
       </c>
-      <c r="B54" s="14" t="s">
+      <c r="B54" s="15" t="s">
         <v>290</v>
       </c>
-      <c r="C54" s="8" t="s">
+      <c r="C54" s="9" t="s">
         <v>291</v>
       </c>
-      <c r="D54" s="8" t="s">
+      <c r="D54" s="9" t="s">
         <v>292</v>
       </c>
-      <c r="E54" s="8" t="s">
+      <c r="E54" s="9" t="s">
         <v>293</v>
       </c>
-      <c r="F54" s="8" t="s">
+      <c r="F54" s="9" t="s">
         <v>294</v>
       </c>
     </row>
     <row r="55" spans="1:6">
-      <c r="A55" s="13" t="s">
+      <c r="A55" s="14" t="s">
         <v>295</v>
       </c>
-      <c r="B55" s="14" t="s">
+      <c r="B55" s="15" t="s">
         <v>296</v>
       </c>
-      <c r="C55" s="8" t="s">
+      <c r="C55" s="9" t="s">
         <v>297</v>
       </c>
-      <c r="D55" s="8" t="s">
+      <c r="D55" s="9" t="s">
         <v>298</v>
       </c>
-      <c r="E55" s="8" t="s">
+      <c r="E55" s="9" t="s">
         <v>299</v>
       </c>
-      <c r="F55" s="8" t="s">
+      <c r="F55" s="9" t="s">
         <v>300</v>
       </c>
     </row>
     <row r="56" spans="1:6">
-      <c r="A56" s="13" t="s">
+      <c r="A56" s="14" t="s">
         <v>301</v>
       </c>
-      <c r="B56" s="21" t="s">
+      <c r="B56" s="22" t="s">
         <v>302</v>
       </c>
-      <c r="C56" s="8" t="s">
+      <c r="C56" s="9" t="s">
         <v>303</v>
       </c>
-      <c r="D56" s="8" t="s">
+      <c r="D56" s="9" t="s">
         <v>304</v>
       </c>
-      <c r="E56" s="8" t="s">
+      <c r="E56" s="9" t="s">
         <v>305</v>
       </c>
-      <c r="F56" s="8" t="s">
+      <c r="F56" s="9" t="s">
         <v>306</v>
       </c>
     </row>
     <row r="57" spans="1:6">
-      <c r="A57" s="13" t="s">
+      <c r="A57" s="14" t="s">
         <v>307</v>
       </c>
-      <c r="B57" s="21" t="s">
+      <c r="B57" s="22" t="s">
         <v>308</v>
       </c>
-      <c r="C57" s="8" t="s">
+      <c r="C57" s="9" t="s">
         <v>309</v>
       </c>
-      <c r="D57" s="8" t="s">
+      <c r="D57" s="9" t="s">
         <v>310</v>
       </c>
-      <c r="E57" s="8" t="s">
+      <c r="E57" s="9" t="s">
         <v>311</v>
       </c>
-      <c r="F57" s="8" t="s">
+      <c r="F57" s="9" t="s">
         <v>312</v>
       </c>
     </row>
     <row r="58" spans="1:6">
-      <c r="A58" s="13" t="s">
+      <c r="A58" s="14" t="s">
         <v>313</v>
       </c>
-      <c r="B58" s="21" t="s">
+      <c r="B58" s="22" t="s">
         <v>314</v>
       </c>
-      <c r="C58" s="8" t="s">
+      <c r="C58" s="9" t="s">
         <v>315</v>
       </c>
-      <c r="D58" s="8" t="s">
+      <c r="D58" s="9" t="s">
         <v>316</v>
       </c>
-      <c r="E58" s="8" t="s">
+      <c r="E58" s="9" t="s">
         <v>317</v>
       </c>
-      <c r="F58" s="8" t="s">
+      <c r="F58" s="9" t="s">
         <v>318</v>
       </c>
     </row>
     <row r="59" spans="1:6">
-      <c r="A59" s="13" t="s">
+      <c r="A59" s="14" t="s">
         <v>319</v>
       </c>
-      <c r="B59" s="14" t="s">
+      <c r="B59" s="15" t="s">
         <v>320</v>
       </c>
-      <c r="C59" s="8" t="s">
+      <c r="C59" s="9" t="s">
         <v>321</v>
       </c>
-      <c r="D59" s="8" t="s">
+      <c r="D59" s="9" t="s">
         <v>322</v>
       </c>
-      <c r="E59" s="8" t="s">
+      <c r="E59" s="9" t="s">
         <v>323</v>
       </c>
-      <c r="F59" s="8" t="s">
+      <c r="F59" s="9" t="s">
         <v>324</v>
       </c>
     </row>
     <row r="60" spans="1:6">
-      <c r="A60" s="13" t="s">
+      <c r="A60" s="14" t="s">
         <v>325</v>
       </c>
-      <c r="B60" s="14" t="s">
+      <c r="B60" s="15" t="s">
         <v>326</v>
       </c>
-      <c r="C60" s="8" t="s">
+      <c r="C60" s="9" t="s">
         <v>327</v>
       </c>
-      <c r="D60" s="8" t="s">
+      <c r="D60" s="9" t="s">
         <v>328</v>
       </c>
-      <c r="E60" s="8" t="s">
+      <c r="E60" s="9" t="s">
         <v>329</v>
       </c>
-      <c r="F60" s="8" t="s">
+      <c r="F60" s="9" t="s">
         <v>330</v>
       </c>
     </row>
     <row r="61" spans="1:6">
-      <c r="A61" s="13" t="s">
+      <c r="A61" s="14" t="s">
         <v>331</v>
       </c>
-      <c r="B61" s="14" t="s">
+      <c r="B61" s="15" t="s">
         <v>332</v>
       </c>
-      <c r="C61" s="8" t="s">
+      <c r="C61" s="9" t="s">
         <v>333</v>
       </c>
-      <c r="D61" s="8" t="s">
+      <c r="D61" s="9" t="s">
         <v>334</v>
       </c>
-      <c r="E61" s="8" t="s">
+      <c r="E61" s="9" t="s">
         <v>335</v>
       </c>
-      <c r="F61" s="8" t="s">
+      <c r="F61" s="9" t="s">
         <v>336</v>
       </c>
     </row>
     <row r="62" spans="1:6">
-      <c r="A62" s="13" t="s">
+      <c r="A62" s="14" t="s">
         <v>337</v>
       </c>
-      <c r="B62" s="21" t="s">
+      <c r="B62" s="22" t="s">
         <v>338</v>
       </c>
-      <c r="C62" s="8" t="s">
+      <c r="C62" s="9" t="s">
         <v>339</v>
       </c>
-      <c r="D62" s="8" t="s">
+      <c r="D62" s="9" t="s">
         <v>340</v>
       </c>
-      <c r="E62" s="8" t="s">
+      <c r="E62" s="9" t="s">
         <v>341</v>
       </c>
-      <c r="F62" s="8" t="s">
+      <c r="F62" s="9" t="s">
         <v>342</v>
       </c>
     </row>
     <row r="63" spans="1:6">
-      <c r="A63" s="13" t="s">
+      <c r="A63" s="14" t="s">
         <v>343</v>
       </c>
-      <c r="B63" s="14" t="s">
+      <c r="B63" s="15" t="s">
         <v>344</v>
       </c>
-      <c r="C63" s="8" t="s">
+      <c r="C63" s="9" t="s">
         <v>345</v>
       </c>
-      <c r="D63" s="8" t="s">
+      <c r="D63" s="9" t="s">
         <v>346</v>
       </c>
-      <c r="E63" s="8" t="s">
+      <c r="E63" s="9" t="s">
         <v>347</v>
       </c>
-      <c r="F63" s="8" t="s">
+      <c r="F63" s="9" t="s">
         <v>348</v>
       </c>
     </row>
     <row r="64" spans="1:6">
-      <c r="A64" s="13" t="s">
+      <c r="A64" s="14" t="s">
         <v>349</v>
       </c>
-      <c r="B64" s="14" t="s">
+      <c r="B64" s="15" t="s">
         <v>350</v>
       </c>
-      <c r="C64" s="8" t="s">
+      <c r="C64" s="9" t="s">
         <v>351</v>
       </c>
-      <c r="D64" s="8" t="s">
+      <c r="D64" s="9" t="s">
         <v>352</v>
       </c>
-      <c r="E64" s="8" t="s">
+      <c r="E64" s="9" t="s">
         <v>353</v>
       </c>
-      <c r="F64" s="8" t="s">
+      <c r="F64" s="9" t="s">
         <v>354</v>
       </c>
     </row>
     <row r="65" spans="1:6">
-      <c r="A65" s="13" t="s">
+      <c r="A65" s="14" t="s">
         <v>355</v>
       </c>
-      <c r="B65" s="14" t="s">
+      <c r="B65" s="15" t="s">
         <v>356</v>
       </c>
-      <c r="C65" s="8" t="s">
+      <c r="C65" s="9" t="s">
         <v>357</v>
       </c>
-      <c r="D65" s="8" t="s">
+      <c r="D65" s="9" t="s">
         <v>358</v>
       </c>
-      <c r="E65" s="8" t="s">
+      <c r="E65" s="9" t="s">
         <v>359</v>
       </c>
-      <c r="F65" s="8" t="s">
+      <c r="F65" s="9" t="s">
         <v>360</v>
       </c>
     </row>
     <row r="66" spans="1:6">
-      <c r="A66" s="13" t="s">
+      <c r="A66" s="14" t="s">
         <v>361</v>
       </c>
-      <c r="B66" s="14" t="s">
+      <c r="B66" s="15" t="s">
         <v>361</v>
       </c>
-      <c r="C66" s="8" t="s">
+      <c r="C66" s="9" t="s">
         <v>362</v>
       </c>
-      <c r="D66" s="8" t="s">
+      <c r="D66" s="9" t="s">
         <v>363</v>
       </c>
-      <c r="E66" s="8" t="s">
+      <c r="E66" s="9" t="s">
         <v>364</v>
       </c>
-      <c r="F66" s="8" t="s">
+      <c r="F66" s="9" t="s">
         <v>365</v>
       </c>
     </row>
     <row r="67" spans="1:6">
-      <c r="A67" s="13" t="s">
+      <c r="A67" s="14" t="s">
         <v>366</v>
       </c>
-      <c r="B67" s="14" t="s">
+      <c r="B67" s="15" t="s">
         <v>366</v>
       </c>
-      <c r="C67" s="8" t="s">
+      <c r="C67" s="9" t="s">
         <v>367</v>
       </c>
-      <c r="D67" s="8" t="s">
+      <c r="D67" s="9" t="s">
         <v>368</v>
       </c>
-      <c r="E67" s="8" t="s">
+      <c r="E67" s="9" t="s">
         <v>369</v>
       </c>
-      <c r="F67" s="8" t="s">
+      <c r="F67" s="9" t="s">
         <v>370</v>
       </c>
     </row>
     <row r="68" spans="1:6">
-      <c r="A68" s="13" t="s">
+      <c r="A68" s="14" t="s">
         <v>371</v>
       </c>
-      <c r="B68" s="14" t="s">
+      <c r="B68" s="15" t="s">
         <v>372</v>
       </c>
-      <c r="C68" s="8" t="s">
+      <c r="C68" s="9" t="s">
         <v>373</v>
       </c>
-      <c r="D68" s="8" t="s">
+      <c r="D68" s="9" t="s">
         <v>374</v>
       </c>
-      <c r="E68" s="8" t="s">
+      <c r="E68" s="9" t="s">
         <v>375</v>
       </c>
-      <c r="F68" s="8" t="s">
+      <c r="F68" s="9" t="s">
         <v>376</v>
       </c>
     </row>
     <row r="69" spans="1:6">
-      <c r="A69" s="13" t="s">
+      <c r="A69" s="14" t="s">
         <v>377</v>
       </c>
-      <c r="B69" s="14" t="s">
+      <c r="B69" s="15" t="s">
         <v>377</v>
       </c>
-      <c r="C69" s="8" t="s">
+      <c r="C69" s="9" t="s">
         <v>378</v>
       </c>
-      <c r="D69" s="8" t="s">
+      <c r="D69" s="9" t="s">
         <v>379</v>
       </c>
-      <c r="E69" s="8" t="s">
+      <c r="E69" s="9" t="s">
         <v>380</v>
       </c>
-      <c r="F69" s="8" t="s">
+      <c r="F69" s="9" t="s">
         <v>381</v>
       </c>
     </row>
     <row r="70" spans="1:6">
-      <c r="A70" s="13" t="s">
+      <c r="A70" s="14" t="s">
         <v>382</v>
       </c>
-      <c r="B70" s="22" t="s">
+      <c r="B70" s="23" t="s">
         <v>382</v>
       </c>
-      <c r="C70" s="8" t="s">
+      <c r="C70" s="9" t="s">
         <v>383</v>
       </c>
-      <c r="D70" s="8" t="s">
+      <c r="D70" s="9" t="s">
         <v>384</v>
       </c>
-      <c r="E70" s="8" t="s">
+      <c r="E70" s="9" t="s">
         <v>385</v>
       </c>
-      <c r="F70" s="8" t="s">
+      <c r="F70" s="9" t="s">
         <v>386</v>
       </c>
     </row>
     <row r="71" spans="1:6">
-      <c r="A71" s="13" t="s">
+      <c r="A71" s="14" t="s">
         <v>387</v>
       </c>
-      <c r="B71" s="14" t="s">
+      <c r="B71" s="15" t="s">
         <v>388</v>
       </c>
-      <c r="C71" s="8" t="s">
+      <c r="C71" s="9" t="s">
         <v>388</v>
       </c>
-      <c r="D71" s="8" t="s">
+      <c r="D71" s="9" t="s">
         <v>389</v>
       </c>
-      <c r="E71" s="8" t="s">
+      <c r="E71" s="9" t="s">
         <v>388</v>
       </c>
-      <c r="F71" s="8" t="s">
+      <c r="F71" s="9" t="s">
         <v>388</v>
       </c>
     </row>
     <row r="72" spans="1:6">
-      <c r="A72" s="13" t="s">
+      <c r="A72" s="14" t="s">
         <v>390</v>
       </c>
-      <c r="B72" s="14" t="s">
+      <c r="B72" s="15" t="s">
         <v>391</v>
       </c>
-      <c r="C72" s="8" t="s">
+      <c r="C72" s="9" t="s">
         <v>392</v>
       </c>
-      <c r="D72" s="8" t="s">
+      <c r="D72" s="9" t="s">
         <v>393</v>
       </c>
-      <c r="E72" s="8" t="s">
+      <c r="E72" s="9" t="s">
         <v>394</v>
       </c>
-      <c r="F72" s="8" t="s">
+      <c r="F72" s="9" t="s">
         <v>395</v>
       </c>
     </row>
     <row r="73" spans="1:6">
-      <c r="A73" s="13" t="s">
+      <c r="A73" s="14" t="s">
         <v>396</v>
       </c>
-      <c r="B73" s="14" t="s">
+      <c r="B73" s="15" t="s">
         <v>397</v>
       </c>
-      <c r="C73" s="8" t="s">
+      <c r="C73" s="9" t="s">
         <v>398</v>
       </c>
-      <c r="D73" s="8" t="s">
+      <c r="D73" s="9" t="s">
         <v>399</v>
       </c>
-      <c r="E73" s="8" t="s">
+      <c r="E73" s="9" t="s">
         <v>400</v>
       </c>
-      <c r="F73" s="8" t="s">
+      <c r="F73" s="9" t="s">
         <v>401</v>
       </c>
     </row>
     <row r="74" spans="1:6">
-      <c r="A74" s="13" t="s">
+      <c r="A74" s="14" t="s">
         <v>402</v>
       </c>
-      <c r="B74" s="14" t="s">
+      <c r="B74" s="15" t="s">
         <v>403</v>
       </c>
-      <c r="C74" s="8" t="s">
+      <c r="C74" s="9" t="s">
         <v>404</v>
       </c>
-      <c r="D74" s="8" t="s">
+      <c r="D74" s="9" t="s">
         <v>405</v>
       </c>
-      <c r="E74" s="8" t="s">
+      <c r="E74" s="9" t="s">
         <v>406</v>
       </c>
-      <c r="F74" s="8" t="s">
+      <c r="F74" s="9" t="s">
         <v>407</v>
       </c>
     </row>
     <row r="75" spans="1:6">
-      <c r="A75" s="13" t="s">
+      <c r="A75" s="14" t="s">
         <v>408</v>
       </c>
-      <c r="B75" s="14" t="s">
+      <c r="B75" s="15" t="s">
         <v>409</v>
       </c>
-      <c r="C75" s="8" t="s">
+      <c r="C75" s="9" t="s">
         <v>410</v>
       </c>
-      <c r="D75" s="8" t="s">
+      <c r="D75" s="9" t="s">
         <v>292</v>
       </c>
-      <c r="E75" s="8" t="s">
+      <c r="E75" s="9" t="s">
         <v>411</v>
       </c>
-      <c r="F75" s="8" t="s">
+      <c r="F75" s="9" t="s">
         <v>412</v>
       </c>
     </row>
     <row r="76" spans="1:6">
-      <c r="A76" s="13" t="s">
+      <c r="A76" s="14" t="s">
         <v>413</v>
       </c>
-      <c r="B76" s="14" t="s">
+      <c r="B76" s="15" t="s">
         <v>414</v>
       </c>
-      <c r="C76" s="8" t="s">
+      <c r="C76" s="9" t="s">
         <v>415</v>
       </c>
-      <c r="D76" s="8" t="s">
+      <c r="D76" s="9" t="s">
         <v>416</v>
       </c>
-      <c r="E76" s="8" t="s">
+      <c r="E76" s="9" t="s">
         <v>417</v>
       </c>
-      <c r="F76" s="8" t="s">
+      <c r="F76" s="9" t="s">
         <v>418</v>
       </c>
     </row>
     <row r="77" spans="1:6">
-      <c r="A77" s="13" t="s">
+      <c r="A77" s="14" t="s">
         <v>419</v>
       </c>
-      <c r="B77" s="14" t="s">
+      <c r="B77" s="15" t="s">
         <v>420</v>
       </c>
-      <c r="C77" s="8" t="s">
+      <c r="C77" s="9" t="s">
         <v>421</v>
       </c>
-      <c r="D77" s="8" t="s">
+      <c r="D77" s="9" t="s">
         <v>420</v>
       </c>
-      <c r="E77" s="8" t="s">
+      <c r="E77" s="9" t="s">
         <v>422</v>
       </c>
-      <c r="F77" s="8" t="s">
+      <c r="F77" s="9" t="s">
         <v>423</v>
       </c>
     </row>
     <row r="78" spans="1:6">
-      <c r="A78" s="13" t="s">
+      <c r="A78" s="14" t="s">
         <v>424</v>
       </c>
-      <c r="B78" s="14" t="s">
+      <c r="B78" s="15" t="s">
         <v>425</v>
       </c>
-      <c r="C78" s="8" t="s">
+      <c r="C78" s="9" t="s">
         <v>426</v>
       </c>
-      <c r="D78" s="8" t="s">
+      <c r="D78" s="9" t="s">
         <v>427</v>
       </c>
-      <c r="E78" s="8" t="s">
+      <c r="E78" s="9" t="s">
         <v>428</v>
       </c>
-      <c r="F78" s="8" t="s">
+      <c r="F78" s="9" t="s">
         <v>429</v>
       </c>
     </row>
     <row r="79" s="3" customFormat="1" spans="1:6">
-      <c r="A79" s="13" t="s">
+      <c r="A79" s="14" t="s">
         <v>430</v>
       </c>
-      <c r="B79" s="23" t="s">
+      <c r="B79" s="24" t="s">
         <v>431</v>
       </c>
-      <c r="C79" s="23" t="s">
+      <c r="C79" s="24" t="s">
         <v>432</v>
       </c>
-      <c r="D79" s="23" t="s">
+      <c r="D79" s="24" t="s">
         <v>433</v>
       </c>
-      <c r="E79" s="23" t="s">
+      <c r="E79" s="24" t="s">
         <v>434</v>
       </c>
-      <c r="F79" s="23" t="s">
+      <c r="F79" s="24" t="s">
         <v>435</v>
       </c>
     </row>
     <row r="80" s="3" customFormat="1" spans="1:6">
-      <c r="A80" s="13" t="s">
+      <c r="A80" s="14" t="s">
         <v>436</v>
       </c>
-      <c r="B80" s="23" t="s">
+      <c r="B80" s="24" t="s">
         <v>437</v>
       </c>
-      <c r="C80" s="23" t="s">
+      <c r="C80" s="24" t="s">
         <v>438</v>
       </c>
-      <c r="D80" s="23" t="s">
+      <c r="D80" s="24" t="s">
         <v>439</v>
       </c>
-      <c r="E80" s="23" t="s">
+      <c r="E80" s="24" t="s">
         <v>440</v>
       </c>
-      <c r="F80" s="23" t="s">
+      <c r="F80" s="24" t="s">
         <v>441</v>
       </c>
     </row>
     <row r="81" s="3" customFormat="1" spans="1:6">
-      <c r="A81" s="13" t="s">
+      <c r="A81" s="14" t="s">
         <v>442</v>
       </c>
-      <c r="B81" s="23" t="s">
+      <c r="B81" s="24" t="s">
         <v>443</v>
       </c>
-      <c r="C81" s="23" t="s">
+      <c r="C81" s="24" t="s">
         <v>444</v>
       </c>
-      <c r="D81" s="23" t="s">
+      <c r="D81" s="24" t="s">
         <v>445</v>
       </c>
-      <c r="E81" s="23" t="s">
+      <c r="E81" s="24" t="s">
         <v>446</v>
       </c>
-      <c r="F81" s="23" t="s">
+      <c r="F81" s="24" t="s">
         <v>447</v>
       </c>
     </row>
     <row r="82" spans="1:6">
-      <c r="A82" s="13" t="s">
+      <c r="A82" s="14" t="s">
         <v>448</v>
       </c>
-      <c r="B82" s="14" t="s">
+      <c r="B82" s="15" t="s">
         <v>449</v>
       </c>
-      <c r="C82" s="8" t="s">
+      <c r="C82" s="9" t="s">
         <v>450</v>
       </c>
-      <c r="D82" s="8" t="s">
+      <c r="D82" s="9" t="s">
         <v>451</v>
       </c>
-      <c r="E82" s="8" t="s">
+      <c r="E82" s="9" t="s">
         <v>452</v>
       </c>
-      <c r="F82" s="8" t="s">
+      <c r="F82" s="9" t="s">
         <v>453</v>
       </c>
     </row>
     <row r="83" spans="1:6">
-      <c r="A83" s="13" t="s">
+      <c r="A83" s="14" t="s">
         <v>454</v>
       </c>
-      <c r="B83" s="14" t="s">
+      <c r="B83" s="15" t="s">
         <v>454</v>
       </c>
-      <c r="C83" s="8" t="s">
+      <c r="C83" s="9" t="s">
         <v>455</v>
       </c>
-      <c r="D83" s="8" t="s">
+      <c r="D83" s="9" t="s">
         <v>456</v>
       </c>
-      <c r="E83" s="8" t="s">
+      <c r="E83" s="9" t="s">
         <v>457</v>
       </c>
-      <c r="F83" s="8" t="s">
+      <c r="F83" s="9" t="s">
         <v>458</v>
       </c>
     </row>
     <row r="84" spans="1:6">
-      <c r="A84" s="13" t="s">
+      <c r="A84" s="14" t="s">
         <v>459</v>
       </c>
-      <c r="B84" s="14" t="s">
+      <c r="B84" s="15" t="s">
         <v>460</v>
       </c>
-      <c r="C84" s="8" t="s">
+      <c r="C84" s="9" t="s">
         <v>461</v>
       </c>
-      <c r="D84" s="8" t="s">
+      <c r="D84" s="9" t="s">
         <v>462</v>
       </c>
-      <c r="E84" s="8" t="s">
+      <c r="E84" s="9" t="s">
         <v>463</v>
       </c>
-      <c r="F84" s="8" t="s">
+      <c r="F84" s="9" t="s">
         <v>464</v>
       </c>
     </row>
     <row r="85" ht="66" spans="1:6">
-      <c r="A85" s="13" t="s">
+      <c r="A85" s="14" t="s">
         <v>465</v>
       </c>
-      <c r="B85" s="14" t="s">
+      <c r="B85" s="15" t="s">
         <v>466</v>
       </c>
-      <c r="C85" s="15" t="s">
+      <c r="C85" s="16" t="s">
         <v>467</v>
       </c>
-      <c r="D85" s="15" t="s">
+      <c r="D85" s="16" t="s">
         <v>468</v>
       </c>
-      <c r="E85" s="15" t="s">
+      <c r="E85" s="16" t="s">
         <v>469</v>
       </c>
-      <c r="F85" s="15" t="s">
+      <c r="F85" s="16" t="s">
         <v>470</v>
       </c>
     </row>
     <row r="86" ht="33" spans="1:6">
-      <c r="A86" s="13" t="s">
+      <c r="A86" s="14" t="s">
         <v>471</v>
       </c>
-      <c r="B86" s="14" t="s">
+      <c r="B86" s="15" t="s">
         <v>472</v>
       </c>
-      <c r="C86" s="15" t="s">
+      <c r="C86" s="16" t="s">
         <v>473</v>
       </c>
-      <c r="D86" s="15" t="s">
+      <c r="D86" s="16" t="s">
         <v>474</v>
       </c>
-      <c r="E86" s="15" t="s">
+      <c r="E86" s="16" t="s">
         <v>475</v>
       </c>
-      <c r="F86" s="15" t="s">
+      <c r="F86" s="16" t="s">
         <v>476</v>
       </c>
     </row>
     <row r="87" spans="1:6">
-      <c r="A87" s="13" t="s">
+      <c r="A87" s="14" t="s">
         <v>477</v>
       </c>
-      <c r="B87" s="14" t="s">
+      <c r="B87" s="15" t="s">
         <v>478</v>
       </c>
-      <c r="C87" s="8" t="s">
+      <c r="C87" s="9" t="s">
         <v>479</v>
       </c>
-      <c r="D87" s="8" t="s">
+      <c r="D87" s="9" t="s">
         <v>480</v>
       </c>
-      <c r="E87" s="8" t="s">
+      <c r="E87" s="9" t="s">
         <v>481</v>
       </c>
-      <c r="F87" s="8" t="s">
+      <c r="F87" s="9" t="s">
         <v>482</v>
       </c>
     </row>
     <row r="88" spans="1:6">
-      <c r="A88" s="13" t="s">
+      <c r="A88" s="14" t="s">
         <v>483</v>
       </c>
-      <c r="B88" s="14" t="s">
+      <c r="B88" s="15" t="s">
         <v>484</v>
       </c>
-      <c r="C88" s="8" t="s">
+      <c r="C88" s="9" t="s">
         <v>485</v>
       </c>
-      <c r="D88" s="8" t="s">
+      <c r="D88" s="9" t="s">
         <v>486</v>
       </c>
-      <c r="E88" s="8" t="s">
+      <c r="E88" s="9" t="s">
         <v>487</v>
       </c>
-      <c r="F88" s="8" t="s">
+      <c r="F88" s="9" t="s">
         <v>488</v>
       </c>
     </row>
     <row r="89" spans="1:6">
-      <c r="A89" s="13" t="s">
+      <c r="A89" s="14" t="s">
         <v>489</v>
       </c>
-      <c r="B89" s="14" t="s">
+      <c r="B89" s="15" t="s">
         <v>490</v>
       </c>
-      <c r="C89" s="8" t="s">
+      <c r="C89" s="9" t="s">
         <v>491</v>
       </c>
-      <c r="D89" s="8" t="s">
+      <c r="D89" s="9" t="s">
         <v>492</v>
       </c>
-      <c r="E89" s="8" t="s">
+      <c r="E89" s="9" t="s">
         <v>493</v>
       </c>
-      <c r="F89" s="8" t="s">
+      <c r="F89" s="9" t="s">
         <v>494</v>
       </c>
     </row>
     <row r="90" spans="1:6">
-      <c r="A90" s="13" t="s">
+      <c r="A90" s="14" t="s">
         <v>495</v>
       </c>
-      <c r="B90" s="14" t="s">
+      <c r="B90" s="15" t="s">
         <v>495</v>
       </c>
-      <c r="C90" s="8" t="s">
+      <c r="C90" s="9" t="s">
         <v>496</v>
       </c>
-      <c r="D90" s="8" t="s">
+      <c r="D90" s="9" t="s">
         <v>497</v>
       </c>
-      <c r="E90" s="8" t="s">
+      <c r="E90" s="9" t="s">
         <v>498</v>
       </c>
-      <c r="F90" s="8" t="s">
+      <c r="F90" s="9" t="s">
         <v>499</v>
       </c>
     </row>
     <row r="91" spans="1:6">
-      <c r="A91" s="13" t="s">
+      <c r="A91" s="14" t="s">
         <v>500</v>
       </c>
-      <c r="B91" s="14" t="s">
+      <c r="B91" s="15" t="s">
         <v>501</v>
       </c>
-      <c r="C91" s="8" t="s">
+      <c r="C91" s="9" t="s">
         <v>502</v>
       </c>
-      <c r="D91" s="8" t="s">
+      <c r="D91" s="9" t="s">
         <v>503</v>
       </c>
-      <c r="E91" s="8" t="s">
+      <c r="E91" s="9" t="s">
         <v>504</v>
       </c>
-      <c r="F91" s="8" t="s">
+      <c r="F91" s="9" t="s">
         <v>505</v>
       </c>
     </row>
     <row r="92" spans="1:6">
-      <c r="A92" s="13" t="s">
+      <c r="A92" s="14" t="s">
         <v>506</v>
       </c>
-      <c r="B92" s="14" t="s">
+      <c r="B92" s="15" t="s">
         <v>507</v>
       </c>
-      <c r="C92" s="16" t="s">
+      <c r="C92" s="17" t="s">
         <v>508</v>
       </c>
-      <c r="D92" s="16" t="s">
+      <c r="D92" s="17" t="s">
         <v>509</v>
       </c>
-      <c r="E92" s="8" t="s">
+      <c r="E92" s="9" t="s">
         <v>510</v>
       </c>
-      <c r="F92" s="8" t="s">
+      <c r="F92" s="9" t="s">
         <v>511</v>
       </c>
     </row>
     <row r="93" ht="33" spans="1:6">
-      <c r="A93" s="13" t="s">
+      <c r="A93" s="14" t="s">
         <v>512</v>
       </c>
-      <c r="B93" s="14" t="s">
+      <c r="B93" s="15" t="s">
         <v>513</v>
       </c>
-      <c r="C93" s="15" t="s">
+      <c r="C93" s="16" t="s">
         <v>514</v>
       </c>
-      <c r="D93" s="15" t="s">
+      <c r="D93" s="16" t="s">
         <v>515</v>
       </c>
-      <c r="E93" s="15" t="s">
+      <c r="E93" s="16" t="s">
         <v>516</v>
       </c>
-      <c r="F93" s="15" t="s">
+      <c r="F93" s="16" t="s">
         <v>517</v>
       </c>
     </row>
     <row r="94" ht="33" spans="1:6">
-      <c r="A94" s="13" t="s">
+      <c r="A94" s="14" t="s">
         <v>518</v>
       </c>
-      <c r="B94" s="14" t="s">
+      <c r="B94" s="15" t="s">
         <v>519</v>
       </c>
-      <c r="C94" s="15" t="s">
+      <c r="C94" s="16" t="s">
         <v>520</v>
       </c>
-      <c r="D94" s="15" t="s">
+      <c r="D94" s="16" t="s">
         <v>521</v>
       </c>
-      <c r="E94" s="15" t="s">
+      <c r="E94" s="16" t="s">
         <v>522</v>
       </c>
-      <c r="F94" s="15" t="s">
+      <c r="F94" s="16" t="s">
         <v>523</v>
       </c>
     </row>
     <row r="95" ht="33" spans="1:6">
-      <c r="A95" s="13" t="s">
+      <c r="A95" s="14" t="s">
         <v>524</v>
       </c>
-      <c r="B95" s="14" t="s">
+      <c r="B95" s="15" t="s">
         <v>525</v>
       </c>
-      <c r="C95" s="15" t="s">
+      <c r="C95" s="16" t="s">
         <v>526</v>
       </c>
-      <c r="D95" s="15" t="s">
+      <c r="D95" s="16" t="s">
         <v>527</v>
       </c>
-      <c r="E95" s="15" t="s">
+      <c r="E95" s="16" t="s">
         <v>528</v>
       </c>
-      <c r="F95" s="15" t="s">
+      <c r="F95" s="16" t="s">
         <v>529</v>
       </c>
     </row>
     <row r="96" spans="1:6">
-      <c r="A96" s="13" t="s">
+      <c r="A96" s="14" t="s">
         <v>530</v>
       </c>
-      <c r="B96" s="14" t="s">
+      <c r="B96" s="15" t="s">
         <v>531</v>
       </c>
-      <c r="C96" s="8" t="s">
+      <c r="C96" s="9" t="s">
         <v>532</v>
       </c>
-      <c r="D96" s="8" t="s">
+      <c r="D96" s="9" t="s">
         <v>533</v>
       </c>
-      <c r="E96" s="8" t="s">
+      <c r="E96" s="9" t="s">
         <v>534</v>
       </c>
-      <c r="F96" s="8" t="s">
+      <c r="F96" s="9" t="s">
         <v>535</v>
       </c>
     </row>
     <row r="97" spans="1:6">
-      <c r="A97" s="13" t="s">
+      <c r="A97" s="14" t="s">
         <v>536</v>
       </c>
-      <c r="B97" s="14" t="s">
+      <c r="B97" s="15" t="s">
         <v>537</v>
       </c>
-      <c r="C97" s="8" t="s">
+      <c r="C97" s="9" t="s">
         <v>538</v>
       </c>
-      <c r="D97" s="8" t="s">
+      <c r="D97" s="9" t="s">
         <v>539</v>
       </c>
-      <c r="E97" s="8" t="s">
+      <c r="E97" s="9" t="s">
         <v>540</v>
       </c>
-      <c r="F97" s="8" t="s">
+      <c r="F97" s="9" t="s">
         <v>541</v>
       </c>
     </row>
     <row r="98" spans="1:6">
-      <c r="A98" s="13" t="s">
+      <c r="A98" s="14" t="s">
         <v>542</v>
       </c>
-      <c r="B98" s="14" t="s">
+      <c r="B98" s="15" t="s">
         <v>543</v>
       </c>
-      <c r="C98" s="8" t="s">
+      <c r="C98" s="9" t="s">
         <v>544</v>
       </c>
-      <c r="D98" s="8" t="s">
+      <c r="D98" s="9" t="s">
         <v>545</v>
       </c>
-      <c r="E98" s="8" t="s">
+      <c r="E98" s="9" t="s">
         <v>546</v>
       </c>
-      <c r="F98" s="8" t="s">
+      <c r="F98" s="9" t="s">
         <v>547</v>
       </c>
     </row>
-    <row r="99" spans="1:6">
-      <c r="A99" s="13" t="s">
+    <row r="99" s="4" customFormat="1" spans="1:6">
+      <c r="A99" s="25" t="s">
         <v>548</v>
       </c>
-      <c r="B99" s="14" t="s">
+      <c r="B99" s="26" t="s">
         <v>549</v>
       </c>
-      <c r="C99" s="8" t="s">
-        <v>550</v>
-      </c>
-      <c r="D99" s="8" t="s">
-        <v>551</v>
-      </c>
-      <c r="E99" s="8" t="s">
-        <v>552</v>
-      </c>
-      <c r="F99" s="8" t="s">
-        <v>553</v>
-      </c>
+      <c r="C99" s="27"/>
+      <c r="D99" s="27"/>
+      <c r="E99" s="27"/>
+      <c r="F99" s="27"/>
     </row>
     <row r="100" spans="1:6">
-      <c r="A100" s="13" t="s">
+      <c r="A100" s="14" t="s">
+        <v>550</v>
+      </c>
+      <c r="B100" s="15" t="s">
+        <v>551</v>
+      </c>
+      <c r="C100" s="9" t="s">
+        <v>552</v>
+      </c>
+      <c r="D100" s="9" t="s">
+        <v>553</v>
+      </c>
+      <c r="E100" s="9" t="s">
         <v>554</v>
       </c>
-      <c r="B100" s="14" t="s">
-        <v>554</v>
-      </c>
-      <c r="C100" s="8" t="s">
+      <c r="F100" s="9" t="s">
         <v>555</v>
-      </c>
-      <c r="D100" s="8" t="s">
-        <v>556</v>
-      </c>
-      <c r="E100" s="8" t="s">
-        <v>557</v>
-      </c>
-      <c r="F100" s="8" t="s">
-        <v>558</v>
       </c>
     </row>
     <row r="101" spans="1:6">
-      <c r="A101" s="13" t="s">
+      <c r="A101" s="14" t="s">
+        <v>556</v>
+      </c>
+      <c r="B101" s="15" t="s">
+        <v>556</v>
+      </c>
+      <c r="C101" s="9" t="s">
+        <v>557</v>
+      </c>
+      <c r="D101" s="9" t="s">
+        <v>558</v>
+      </c>
+      <c r="E101" s="9" t="s">
         <v>559</v>
       </c>
-      <c r="B101" s="14" t="s">
+      <c r="F101" s="9" t="s">
         <v>560</v>
-      </c>
-      <c r="C101" s="8" t="s">
-        <v>561</v>
-      </c>
-      <c r="D101" s="8" t="s">
-        <v>562</v>
-      </c>
-      <c r="E101" s="8" t="s">
-        <v>563</v>
-      </c>
-      <c r="F101" s="8" t="s">
-        <v>564</v>
       </c>
     </row>
     <row r="102" spans="1:6">
-      <c r="A102" s="13" t="s">
+      <c r="A102" s="14" t="s">
+        <v>561</v>
+      </c>
+      <c r="B102" s="15" t="s">
+        <v>562</v>
+      </c>
+      <c r="C102" s="9" t="s">
+        <v>563</v>
+      </c>
+      <c r="D102" s="9" t="s">
+        <v>564</v>
+      </c>
+      <c r="E102" s="9" t="s">
         <v>565</v>
       </c>
-      <c r="B102" s="14" t="s">
-        <v>565</v>
-      </c>
-      <c r="C102" s="8" t="s">
+      <c r="F102" s="9" t="s">
         <v>566</v>
-      </c>
-      <c r="D102" s="8" t="s">
-        <v>567</v>
-      </c>
-      <c r="E102" s="8" t="s">
-        <v>568</v>
-      </c>
-      <c r="F102" s="8" t="s">
-        <v>569</v>
       </c>
     </row>
     <row r="103" spans="1:6">
-      <c r="A103" s="13" t="s">
+      <c r="A103" s="14" t="s">
+        <v>567</v>
+      </c>
+      <c r="B103" s="15" t="s">
+        <v>567</v>
+      </c>
+      <c r="C103" s="9" t="s">
+        <v>568</v>
+      </c>
+      <c r="D103" s="9" t="s">
+        <v>569</v>
+      </c>
+      <c r="E103" s="9" t="s">
         <v>570</v>
       </c>
-      <c r="B103" s="14" t="s">
+      <c r="F103" s="9" t="s">
         <v>571</v>
-      </c>
-      <c r="C103" s="8" t="s">
-        <v>572</v>
-      </c>
-      <c r="D103" s="8" t="s">
-        <v>573</v>
-      </c>
-      <c r="E103" s="8" t="s">
-        <v>574</v>
-      </c>
-      <c r="F103" s="8" t="s">
-        <v>575</v>
       </c>
     </row>
     <row r="104" spans="1:6">
-      <c r="A104" s="13" t="s">
+      <c r="A104" s="14" t="s">
+        <v>572</v>
+      </c>
+      <c r="B104" s="15" t="s">
+        <v>573</v>
+      </c>
+      <c r="C104" s="9" t="s">
+        <v>574</v>
+      </c>
+      <c r="D104" s="9" t="s">
+        <v>575</v>
+      </c>
+      <c r="E104" s="9" t="s">
         <v>576</v>
       </c>
-      <c r="B104" s="14" t="s">
+      <c r="F104" s="9" t="s">
         <v>577</v>
-      </c>
-      <c r="C104" s="8" t="s">
-        <v>578</v>
-      </c>
-      <c r="D104" s="8" t="s">
-        <v>579</v>
-      </c>
-      <c r="E104" s="8" t="s">
-        <v>580</v>
-      </c>
-      <c r="F104" s="8" t="s">
-        <v>581</v>
       </c>
     </row>
     <row r="105" spans="1:6">
-      <c r="A105" s="13" t="s">
+      <c r="A105" s="14" t="s">
+        <v>578</v>
+      </c>
+      <c r="B105" s="15" t="s">
+        <v>579</v>
+      </c>
+      <c r="C105" s="9" t="s">
+        <v>580</v>
+      </c>
+      <c r="D105" s="9" t="s">
+        <v>581</v>
+      </c>
+      <c r="E105" s="9" t="s">
         <v>582</v>
       </c>
-      <c r="B105" s="14" t="s">
+      <c r="F105" s="9" t="s">
         <v>583</v>
-      </c>
-      <c r="C105" s="8" t="s">
-        <v>584</v>
-      </c>
-      <c r="D105" s="8" t="s">
-        <v>585</v>
-      </c>
-      <c r="E105" s="8" t="s">
-        <v>586</v>
-      </c>
-      <c r="F105" s="8" t="s">
-        <v>587</v>
       </c>
     </row>
     <row r="106" spans="1:6">
-      <c r="A106" s="13" t="s">
+      <c r="A106" s="14" t="s">
+        <v>584</v>
+      </c>
+      <c r="B106" s="15" t="s">
+        <v>585</v>
+      </c>
+      <c r="C106" s="9" t="s">
+        <v>586</v>
+      </c>
+      <c r="D106" s="9" t="s">
+        <v>587</v>
+      </c>
+      <c r="E106" s="9" t="s">
         <v>588</v>
       </c>
-      <c r="B106" s="14" t="s">
+      <c r="F106" s="9" t="s">
         <v>589</v>
-      </c>
-      <c r="C106" s="8" t="s">
-        <v>590</v>
-      </c>
-      <c r="D106" s="8" t="s">
-        <v>591</v>
-      </c>
-      <c r="E106" s="8" t="s">
-        <v>592</v>
-      </c>
-      <c r="F106" s="8" t="s">
-        <v>43</v>
       </c>
     </row>
     <row r="107" spans="1:6">
-      <c r="A107" s="13" t="s">
+      <c r="A107" s="14" t="s">
+        <v>590</v>
+      </c>
+      <c r="B107" s="15" t="s">
+        <v>591</v>
+      </c>
+      <c r="C107" s="9" t="s">
+        <v>592</v>
+      </c>
+      <c r="D107" s="9" t="s">
         <v>593</v>
       </c>
-      <c r="B107" s="14" t="s">
+      <c r="E107" s="9" t="s">
         <v>594</v>
       </c>
-      <c r="C107" s="8" t="s">
-        <v>595</v>
-      </c>
-      <c r="D107" s="8" t="s">
-        <v>596</v>
-      </c>
-      <c r="E107" s="8" t="s">
-        <v>597</v>
-      </c>
-      <c r="F107" s="8" t="s">
-        <v>598</v>
+      <c r="F107" s="9" t="s">
+        <v>43</v>
       </c>
     </row>
     <row r="108" spans="1:6">
-      <c r="A108" s="13" t="s">
+      <c r="A108" s="14" t="s">
+        <v>595</v>
+      </c>
+      <c r="B108" s="15" t="s">
+        <v>596</v>
+      </c>
+      <c r="C108" s="9" t="s">
+        <v>597</v>
+      </c>
+      <c r="D108" s="9" t="s">
+        <v>598</v>
+      </c>
+      <c r="E108" s="9" t="s">
         <v>599</v>
       </c>
-      <c r="B108" s="14" t="s">
+      <c r="F108" s="9" t="s">
         <v>600</v>
-      </c>
-      <c r="C108" s="8" t="s">
-        <v>601</v>
-      </c>
-      <c r="D108" s="8" t="s">
-        <v>602</v>
-      </c>
-      <c r="E108" s="8" t="s">
-        <v>603</v>
-      </c>
-      <c r="F108" s="8" t="s">
-        <v>604</v>
       </c>
     </row>
     <row r="109" spans="1:6">
-      <c r="A109" s="13" t="s">
+      <c r="A109" s="14" t="s">
+        <v>601</v>
+      </c>
+      <c r="B109" s="15" t="s">
+        <v>602</v>
+      </c>
+      <c r="C109" s="9" t="s">
+        <v>603</v>
+      </c>
+      <c r="D109" s="9" t="s">
+        <v>604</v>
+      </c>
+      <c r="E109" s="9" t="s">
         <v>605</v>
       </c>
-      <c r="B109" s="14" t="s">
+      <c r="F109" s="9" t="s">
         <v>606</v>
-      </c>
-      <c r="C109" s="8" t="s">
-        <v>607</v>
-      </c>
-      <c r="D109" s="8" t="s">
-        <v>608</v>
-      </c>
-      <c r="E109" s="8" t="s">
-        <v>609</v>
-      </c>
-      <c r="F109" s="8" t="s">
-        <v>610</v>
       </c>
     </row>
     <row r="110" spans="1:6">
-      <c r="A110" s="13" t="s">
+      <c r="A110" s="14" t="s">
+        <v>607</v>
+      </c>
+      <c r="B110" s="15" t="s">
+        <v>608</v>
+      </c>
+      <c r="C110" s="9" t="s">
+        <v>609</v>
+      </c>
+      <c r="D110" s="9" t="s">
+        <v>610</v>
+      </c>
+      <c r="E110" s="9" t="s">
         <v>611</v>
       </c>
-      <c r="B110" s="14" t="s">
+      <c r="F110" s="9" t="s">
         <v>612</v>
-      </c>
-      <c r="C110" s="16" t="s">
-        <v>613</v>
-      </c>
-      <c r="D110" s="16" t="s">
-        <v>614</v>
-      </c>
-      <c r="E110" s="8" t="s">
-        <v>615</v>
-      </c>
-      <c r="F110" s="8" t="s">
-        <v>616</v>
       </c>
     </row>
     <row r="111" spans="1:6">
-      <c r="A111" s="13" t="s">
+      <c r="A111" s="14" t="s">
+        <v>613</v>
+      </c>
+      <c r="B111" s="15" t="s">
+        <v>614</v>
+      </c>
+      <c r="C111" s="17" t="s">
+        <v>615</v>
+      </c>
+      <c r="D111" s="17" t="s">
+        <v>616</v>
+      </c>
+      <c r="E111" s="9" t="s">
         <v>617</v>
       </c>
-      <c r="B111" s="14" t="s">
+      <c r="F111" s="9" t="s">
         <v>618</v>
-      </c>
-      <c r="C111" s="16" t="s">
-        <v>619</v>
-      </c>
-      <c r="D111" s="16" t="s">
-        <v>620</v>
-      </c>
-      <c r="E111" s="8" t="s">
-        <v>621</v>
-      </c>
-      <c r="F111" s="8" t="s">
-        <v>622</v>
       </c>
     </row>
     <row r="112" spans="1:6">
-      <c r="A112" s="13" t="s">
+      <c r="A112" s="14" t="s">
+        <v>619</v>
+      </c>
+      <c r="B112" s="15" t="s">
+        <v>620</v>
+      </c>
+      <c r="C112" s="17" t="s">
+        <v>621</v>
+      </c>
+      <c r="D112" s="17" t="s">
+        <v>622</v>
+      </c>
+      <c r="E112" s="9" t="s">
         <v>623</v>
       </c>
-      <c r="B112" s="14" t="s">
+      <c r="F112" s="9" t="s">
         <v>624</v>
-      </c>
-      <c r="C112" s="16" t="s">
-        <v>625</v>
-      </c>
-      <c r="D112" s="16" t="s">
-        <v>626</v>
-      </c>
-      <c r="E112" s="8" t="s">
-        <v>627</v>
-      </c>
-      <c r="F112" s="8" t="s">
-        <v>628</v>
       </c>
     </row>
     <row r="113" spans="1:6">
-      <c r="A113" s="13" t="s">
+      <c r="A113" s="14" t="s">
+        <v>625</v>
+      </c>
+      <c r="B113" s="15" t="s">
+        <v>626</v>
+      </c>
+      <c r="C113" s="17" t="s">
+        <v>627</v>
+      </c>
+      <c r="D113" s="17" t="s">
+        <v>628</v>
+      </c>
+      <c r="E113" s="9" t="s">
         <v>629</v>
       </c>
-      <c r="B113" s="14" t="s">
+      <c r="F113" s="9" t="s">
         <v>630</v>
-      </c>
-      <c r="C113" s="16" t="s">
-        <v>631</v>
-      </c>
-      <c r="D113" s="16" t="s">
-        <v>632</v>
-      </c>
-      <c r="E113" s="8" t="s">
-        <v>633</v>
-      </c>
-      <c r="F113" s="8" t="s">
-        <v>634</v>
       </c>
     </row>
     <row r="114" spans="1:6">
-      <c r="A114" s="13" t="s">
+      <c r="A114" s="14" t="s">
+        <v>631</v>
+      </c>
+      <c r="B114" s="15" t="s">
+        <v>632</v>
+      </c>
+      <c r="C114" s="17" t="s">
+        <v>633</v>
+      </c>
+      <c r="D114" s="17" t="s">
+        <v>634</v>
+      </c>
+      <c r="E114" s="9" t="s">
         <v>635</v>
       </c>
-      <c r="B114" s="14" t="s">
+      <c r="F114" s="9" t="s">
         <v>636</v>
-      </c>
-      <c r="C114" s="8" t="s">
-        <v>637</v>
-      </c>
-      <c r="D114" s="8" t="s">
-        <v>638</v>
-      </c>
-      <c r="E114" s="8" t="s">
-        <v>639</v>
-      </c>
-      <c r="F114" s="8" t="s">
-        <v>640</v>
       </c>
     </row>
     <row r="115" spans="1:6">
-      <c r="A115" s="13" t="s">
+      <c r="A115" s="14" t="s">
+        <v>637</v>
+      </c>
+      <c r="B115" s="15" t="s">
+        <v>638</v>
+      </c>
+      <c r="C115" s="9" t="s">
+        <v>639</v>
+      </c>
+      <c r="D115" s="9" t="s">
+        <v>640</v>
+      </c>
+      <c r="E115" s="9" t="s">
         <v>641</v>
       </c>
-      <c r="B115" s="14" t="s">
+      <c r="F115" s="9" t="s">
         <v>642</v>
-      </c>
-      <c r="C115" s="8" t="s">
-        <v>643</v>
-      </c>
-      <c r="D115" s="8" t="s">
-        <v>644</v>
-      </c>
-      <c r="E115" s="8" t="s">
-        <v>645</v>
-      </c>
-      <c r="F115" s="8" t="s">
-        <v>646</v>
       </c>
     </row>
     <row r="116" spans="1:6">
-      <c r="A116" s="13" t="s">
+      <c r="A116" s="14" t="s">
+        <v>643</v>
+      </c>
+      <c r="B116" s="15" t="s">
+        <v>644</v>
+      </c>
+      <c r="C116" s="9" t="s">
+        <v>645</v>
+      </c>
+      <c r="D116" s="9" t="s">
+        <v>646</v>
+      </c>
+      <c r="E116" s="9" t="s">
         <v>647</v>
       </c>
-      <c r="B116" s="14" t="s">
+      <c r="F116" s="9" t="s">
         <v>648</v>
-      </c>
-      <c r="C116" s="8" t="s">
-        <v>649</v>
-      </c>
-      <c r="D116" s="8" t="s">
-        <v>650</v>
-      </c>
-      <c r="E116" s="8" t="s">
-        <v>651</v>
-      </c>
-      <c r="F116" s="8" t="s">
-        <v>652</v>
       </c>
     </row>
     <row r="117" spans="1:6">
-      <c r="A117" s="13" t="s">
+      <c r="A117" s="14" t="s">
+        <v>649</v>
+      </c>
+      <c r="B117" s="15" t="s">
+        <v>650</v>
+      </c>
+      <c r="C117" s="9" t="s">
+        <v>651</v>
+      </c>
+      <c r="D117" s="9" t="s">
+        <v>652</v>
+      </c>
+      <c r="E117" s="9" t="s">
         <v>653</v>
       </c>
-      <c r="B117" s="14" t="s">
+      <c r="F117" s="9" t="s">
         <v>654</v>
-      </c>
-      <c r="C117" s="8" t="s">
-        <v>655</v>
-      </c>
-      <c r="D117" s="8" t="s">
-        <v>656</v>
-      </c>
-      <c r="E117" s="8" t="s">
-        <v>657</v>
-      </c>
-      <c r="F117" s="8" t="s">
-        <v>658</v>
       </c>
     </row>
     <row r="118" spans="1:6">
-      <c r="A118" s="13" t="s">
+      <c r="A118" s="14" t="s">
+        <v>655</v>
+      </c>
+      <c r="B118" s="15" t="s">
+        <v>656</v>
+      </c>
+      <c r="C118" s="9" t="s">
+        <v>657</v>
+      </c>
+      <c r="D118" s="9" t="s">
+        <v>658</v>
+      </c>
+      <c r="E118" s="9" t="s">
         <v>659</v>
       </c>
-      <c r="B118" s="14" t="s">
+      <c r="F118" s="9" t="s">
         <v>660</v>
-      </c>
-      <c r="C118" s="8" t="s">
-        <v>661</v>
-      </c>
-      <c r="D118" s="8" t="s">
-        <v>662</v>
-      </c>
-      <c r="E118" s="8" t="s">
-        <v>663</v>
-      </c>
-      <c r="F118" s="8" t="s">
-        <v>664</v>
       </c>
     </row>
     <row r="119" spans="1:6">
-      <c r="A119" s="13" t="s">
+      <c r="A119" s="14" t="s">
+        <v>661</v>
+      </c>
+      <c r="B119" s="15" t="s">
+        <v>662</v>
+      </c>
+      <c r="C119" s="9" t="s">
+        <v>663</v>
+      </c>
+      <c r="D119" s="9" t="s">
+        <v>664</v>
+      </c>
+      <c r="E119" s="9" t="s">
         <v>665</v>
       </c>
-      <c r="B119" s="14" t="s">
+      <c r="F119" s="9" t="s">
         <v>666</v>
-      </c>
-      <c r="C119" s="8" t="s">
-        <v>667</v>
-      </c>
-      <c r="D119" s="8" t="s">
-        <v>668</v>
-      </c>
-      <c r="E119" s="8" t="s">
-        <v>669</v>
-      </c>
-      <c r="F119" s="8" t="s">
-        <v>670</v>
       </c>
     </row>
     <row r="120" spans="1:6">
-      <c r="A120" s="13" t="s">
+      <c r="A120" s="14" t="s">
+        <v>667</v>
+      </c>
+      <c r="B120" s="15" t="s">
+        <v>668</v>
+      </c>
+      <c r="C120" s="9" t="s">
+        <v>669</v>
+      </c>
+      <c r="D120" s="9" t="s">
+        <v>670</v>
+      </c>
+      <c r="E120" s="9" t="s">
         <v>671</v>
       </c>
-      <c r="B120" s="14" t="s">
+      <c r="F120" s="9" t="s">
         <v>672</v>
-      </c>
-      <c r="C120" s="8" t="s">
-        <v>673</v>
-      </c>
-      <c r="D120" s="8" t="s">
-        <v>674</v>
-      </c>
-      <c r="E120" s="20" t="s">
-        <v>675</v>
-      </c>
-      <c r="F120" s="8" t="s">
-        <v>676</v>
       </c>
     </row>
     <row r="121" spans="1:6">
-      <c r="A121" s="13" t="s">
+      <c r="A121" s="14" t="s">
+        <v>673</v>
+      </c>
+      <c r="B121" s="15" t="s">
+        <v>674</v>
+      </c>
+      <c r="C121" s="9" t="s">
+        <v>675</v>
+      </c>
+      <c r="D121" s="9" t="s">
+        <v>676</v>
+      </c>
+      <c r="E121" s="21" t="s">
         <v>677</v>
       </c>
-      <c r="B121" s="19" t="s">
+      <c r="F121" s="9" t="s">
         <v>678</v>
-      </c>
-      <c r="C121" s="19" t="s">
-        <v>679</v>
-      </c>
-      <c r="D121" s="19" t="s">
-        <v>680</v>
-      </c>
-      <c r="E121" s="19" t="s">
-        <v>681</v>
-      </c>
-      <c r="F121" s="19" t="s">
-        <v>682</v>
       </c>
     </row>
     <row r="122" spans="1:6">
-      <c r="A122" s="13" t="s">
+      <c r="A122" s="14" t="s">
+        <v>679</v>
+      </c>
+      <c r="B122" s="20" t="s">
+        <v>680</v>
+      </c>
+      <c r="C122" s="20" t="s">
+        <v>681</v>
+      </c>
+      <c r="D122" s="20" t="s">
+        <v>682</v>
+      </c>
+      <c r="E122" s="20" t="s">
         <v>683</v>
       </c>
-      <c r="B122" s="14" t="s">
+      <c r="F122" s="20" t="s">
         <v>684</v>
-      </c>
-      <c r="C122" s="8" t="s">
-        <v>685</v>
-      </c>
-      <c r="D122" s="8" t="s">
-        <v>686</v>
-      </c>
-      <c r="E122" s="8" t="s">
-        <v>687</v>
-      </c>
-      <c r="F122" s="8" t="s">
-        <v>688</v>
       </c>
     </row>
     <row r="123" spans="1:6">
-      <c r="A123" s="13" t="s">
+      <c r="A123" s="14" t="s">
+        <v>685</v>
+      </c>
+      <c r="B123" s="15" t="s">
+        <v>686</v>
+      </c>
+      <c r="C123" s="9" t="s">
+        <v>687</v>
+      </c>
+      <c r="D123" s="9" t="s">
+        <v>688</v>
+      </c>
+      <c r="E123" s="9" t="s">
         <v>689</v>
       </c>
-      <c r="B123" s="14" t="s">
+      <c r="F123" s="9" t="s">
         <v>690</v>
-      </c>
-      <c r="C123" s="8" t="s">
-        <v>691</v>
-      </c>
-      <c r="D123" s="8" t="s">
-        <v>692</v>
-      </c>
-      <c r="E123" s="8" t="s">
-        <v>693</v>
-      </c>
-      <c r="F123" s="8" t="s">
-        <v>694</v>
       </c>
     </row>
     <row r="124" spans="1:6">
-      <c r="A124" s="13" t="s">
+      <c r="A124" s="14" t="s">
+        <v>691</v>
+      </c>
+      <c r="B124" s="15" t="s">
+        <v>692</v>
+      </c>
+      <c r="C124" s="9" t="s">
+        <v>693</v>
+      </c>
+      <c r="D124" s="9" t="s">
+        <v>694</v>
+      </c>
+      <c r="E124" s="9" t="s">
         <v>695</v>
       </c>
-      <c r="B124" s="14" t="s">
+      <c r="F124" s="9" t="s">
         <v>696</v>
-      </c>
-      <c r="C124" s="8" t="s">
-        <v>697</v>
-      </c>
-      <c r="D124" s="8" t="s">
-        <v>698</v>
-      </c>
-      <c r="E124" s="8" t="s">
-        <v>699</v>
-      </c>
-      <c r="F124" s="8" t="s">
-        <v>700</v>
       </c>
     </row>
     <row r="125" spans="1:6">
-      <c r="A125" s="13" t="s">
+      <c r="A125" s="14" t="s">
+        <v>697</v>
+      </c>
+      <c r="B125" s="15" t="s">
+        <v>698</v>
+      </c>
+      <c r="C125" s="9" t="s">
+        <v>699</v>
+      </c>
+      <c r="D125" s="9" t="s">
+        <v>700</v>
+      </c>
+      <c r="E125" s="9" t="s">
         <v>701</v>
       </c>
-      <c r="B125" s="14" t="s">
+      <c r="F125" s="9" t="s">
         <v>702</v>
-      </c>
-      <c r="C125" s="8" t="s">
-        <v>703</v>
-      </c>
-      <c r="D125" s="8" t="s">
-        <v>704</v>
-      </c>
-      <c r="E125" s="8" t="s">
-        <v>705</v>
-      </c>
-      <c r="F125" s="8" t="s">
-        <v>706</v>
       </c>
     </row>
     <row r="126" spans="1:6">
-      <c r="A126" s="13" t="s">
+      <c r="A126" s="14" t="s">
+        <v>703</v>
+      </c>
+      <c r="B126" s="15" t="s">
+        <v>704</v>
+      </c>
+      <c r="C126" s="9" t="s">
+        <v>705</v>
+      </c>
+      <c r="D126" s="9" t="s">
+        <v>706</v>
+      </c>
+      <c r="E126" s="9" t="s">
         <v>707</v>
       </c>
-      <c r="B126" s="14" t="s">
+      <c r="F126" s="9" t="s">
         <v>708</v>
       </c>
-      <c r="C126" s="8" t="s">
+    </row>
+    <row r="127" spans="1:6">
+      <c r="A127" s="14" t="s">
         <v>709</v>
       </c>
-      <c r="D126" s="8" t="s">
+      <c r="B127" s="15" t="s">
         <v>710</v>
       </c>
-      <c r="E126" s="8" t="s">
+      <c r="C127" s="9" t="s">
         <v>711</v>
       </c>
-      <c r="F126" s="8" t="s">
+      <c r="D127" s="9" t="s">
         <v>712</v>
       </c>
+      <c r="E127" s="9" t="s">
+        <v>713</v>
+      </c>
+      <c r="F127" s="9" t="s">
+        <v>714</v>
+      </c>
     </row>
-    <row r="127" ht="66" spans="1:6">
-      <c r="A127" s="13" t="s">
-        <v>713</v>
-      </c>
-      <c r="B127" s="14" t="s">
-        <v>714</v>
-      </c>
-      <c r="C127" s="15" t="s">
+    <row r="128" ht="66" spans="1:6">
+      <c r="A128" s="14" t="s">
         <v>715</v>
       </c>
-      <c r="D127" s="15" t="s">
+      <c r="B128" s="15" t="s">
         <v>716</v>
       </c>
-      <c r="E127" s="15" t="s">
+      <c r="C128" s="16" t="s">
         <v>717</v>
       </c>
-      <c r="F127" s="15" t="s">
+      <c r="D128" s="16" t="s">
         <v>718</v>
       </c>
-    </row>
-    <row r="128" spans="1:6">
-      <c r="A128" s="13" t="s">
+      <c r="E128" s="16" t="s">
         <v>719</v>
       </c>
-      <c r="B128" s="14" t="s">
+      <c r="F128" s="16" t="s">
         <v>720</v>
-      </c>
-      <c r="C128" s="8" t="s">
-        <v>721</v>
-      </c>
-      <c r="D128" s="8" t="s">
-        <v>722</v>
-      </c>
-      <c r="E128" s="8" t="s">
-        <v>723</v>
-      </c>
-      <c r="F128" s="8" t="s">
-        <v>724</v>
       </c>
     </row>
     <row r="129" spans="1:6">
-      <c r="A129" s="13" t="s">
+      <c r="A129" s="14" t="s">
+        <v>721</v>
+      </c>
+      <c r="B129" s="15" t="s">
+        <v>722</v>
+      </c>
+      <c r="C129" s="9" t="s">
+        <v>723</v>
+      </c>
+      <c r="D129" s="9" t="s">
+        <v>724</v>
+      </c>
+      <c r="E129" s="9" t="s">
         <v>725</v>
       </c>
-      <c r="B129" s="14" t="s">
+      <c r="F129" s="9" t="s">
         <v>726</v>
       </c>
-      <c r="C129" s="8" t="s">
+    </row>
+    <row r="130" spans="1:6">
+      <c r="A130" s="14" t="s">
         <v>727</v>
       </c>
-      <c r="D129" s="8" t="s">
-        <v>579</v>
-      </c>
-      <c r="E129" s="8" t="s">
+      <c r="B130" s="15" t="s">
         <v>728</v>
       </c>
-      <c r="F129" s="8" t="s">
+      <c r="C130" s="9" t="s">
         <v>729</v>
       </c>
+      <c r="D130" s="9" t="s">
+        <v>581</v>
+      </c>
+      <c r="E130" s="9" t="s">
+        <v>730</v>
+      </c>
+      <c r="F130" s="9" t="s">
+        <v>731</v>
+      </c>
     </row>
-    <row r="130" ht="82.5" spans="1:6">
-      <c r="A130" s="13" t="s">
-        <v>730</v>
-      </c>
-      <c r="B130" s="14" t="s">
-        <v>731</v>
-      </c>
-      <c r="C130" s="15" t="s">
+    <row r="131" ht="82.5" spans="1:6">
+      <c r="A131" s="14" t="s">
         <v>732</v>
       </c>
-      <c r="D130" s="15" t="s">
+      <c r="B131" s="15" t="s">
         <v>733</v>
       </c>
-      <c r="E130" s="15" t="s">
+      <c r="C131" s="16" t="s">
         <v>734</v>
       </c>
-      <c r="F130" s="15" t="s">
+      <c r="D131" s="16" t="s">
         <v>735</v>
       </c>
+      <c r="E131" s="16" t="s">
+        <v>736</v>
+      </c>
+      <c r="F131" s="16" t="s">
+        <v>737</v>
+      </c>
     </row>
-    <row r="131" ht="66" spans="1:6">
-      <c r="A131" s="13" t="s">
-        <v>736</v>
-      </c>
-      <c r="B131" s="14" t="s">
-        <v>737</v>
-      </c>
-      <c r="C131" s="15" t="s">
+    <row r="132" ht="66" spans="1:6">
+      <c r="A132" s="14" t="s">
         <v>738</v>
       </c>
-      <c r="D131" s="15" t="s">
+      <c r="B132" s="15" t="s">
         <v>739</v>
       </c>
-      <c r="E131" s="15" t="s">
+      <c r="C132" s="16" t="s">
         <v>740</v>
       </c>
-      <c r="F131" s="15" t="s">
-        <v>740</v>
+      <c r="D132" s="16" t="s">
+        <v>741</v>
+      </c>
+      <c r="E132" s="16" t="s">
+        <v>742</v>
+      </c>
+      <c r="F132" s="16" t="s">
+        <v>742</v>
       </c>
     </row>
-    <row r="132" ht="115.5" spans="1:6">
-      <c r="A132" s="13" t="s">
-        <v>741</v>
-      </c>
-      <c r="B132" s="14" t="s">
-        <v>742</v>
-      </c>
-      <c r="C132" s="24" t="s">
+    <row r="133" ht="115.5" spans="1:6">
+      <c r="A133" s="14" t="s">
         <v>743</v>
       </c>
-      <c r="D132" s="15" t="s">
+      <c r="B133" s="15" t="s">
         <v>744</v>
       </c>
-      <c r="E132" s="15" t="s">
+      <c r="C133" s="28" t="s">
         <v>745</v>
       </c>
-      <c r="F132" s="15" t="s">
+      <c r="D133" s="16" t="s">
         <v>746</v>
       </c>
+      <c r="E133" s="16" t="s">
+        <v>747</v>
+      </c>
+      <c r="F133" s="16" t="s">
+        <v>748</v>
+      </c>
     </row>
-    <row r="133" ht="66" spans="1:6">
-      <c r="A133" s="13" t="s">
-        <v>747</v>
-      </c>
-      <c r="B133" s="14" t="s">
-        <v>748</v>
-      </c>
-      <c r="C133" s="15" t="s">
+    <row r="134" ht="66" spans="1:6">
+      <c r="A134" s="14" t="s">
         <v>749</v>
       </c>
-      <c r="D133" s="15" t="s">
+      <c r="B134" s="15" t="s">
         <v>750</v>
       </c>
-      <c r="E133" s="15" t="s">
+      <c r="C134" s="16" t="s">
         <v>751</v>
       </c>
-      <c r="F133" s="15" t="s">
+      <c r="D134" s="16" t="s">
         <v>752</v>
       </c>
+      <c r="E134" s="16" t="s">
+        <v>753</v>
+      </c>
+      <c r="F134" s="16" t="s">
+        <v>754</v>
+      </c>
     </row>
-    <row r="134" ht="132" spans="1:6">
-      <c r="A134" s="13" t="s">
-        <v>753</v>
-      </c>
-      <c r="B134" s="14" t="s">
-        <v>754</v>
-      </c>
-      <c r="C134" s="15" t="s">
+    <row r="135" ht="132" spans="1:6">
+      <c r="A135" s="14" t="s">
         <v>755</v>
       </c>
-      <c r="D134" s="15" t="s">
+      <c r="B135" s="15" t="s">
         <v>756</v>
       </c>
-      <c r="E134" s="15" t="s">
+      <c r="C135" s="16" t="s">
         <v>757</v>
       </c>
-      <c r="F134" s="15" t="s">
+      <c r="D135" s="16" t="s">
         <v>758</v>
       </c>
+      <c r="E135" s="16" t="s">
+        <v>759</v>
+      </c>
+      <c r="F135" s="16" t="s">
+        <v>760</v>
+      </c>
     </row>
-    <row r="135" spans="1:6">
-      <c r="A135" s="13" t="s">
-        <v>759</v>
-      </c>
-      <c r="B135" s="14" t="s">
-        <v>760</v>
-      </c>
-      <c r="C135" s="16" t="s">
+    <row r="136" spans="1:6">
+      <c r="A136" s="14" t="s">
         <v>761</v>
       </c>
-      <c r="D135" s="16" t="s">
+      <c r="B136" s="15" t="s">
         <v>762</v>
       </c>
-      <c r="E135" s="8" t="s">
+      <c r="C136" s="17" t="s">
         <v>763</v>
       </c>
-      <c r="F135" s="8" t="s">
+      <c r="D136" s="17" t="s">
         <v>764</v>
       </c>
+      <c r="E136" s="9" t="s">
+        <v>765</v>
+      </c>
+      <c r="F136" s="9" t="s">
+        <v>766</v>
+      </c>
     </row>
-    <row r="136" ht="82.5" spans="1:6">
-      <c r="A136" s="13" t="s">
-        <v>765</v>
-      </c>
-      <c r="B136" s="14" t="s">
-        <v>766</v>
-      </c>
-      <c r="C136" s="15" t="s">
+    <row r="137" ht="82.5" spans="1:6">
+      <c r="A137" s="14" t="s">
         <v>767</v>
       </c>
-      <c r="D136" s="15" t="s">
+      <c r="B137" s="15" t="s">
         <v>768</v>
       </c>
-      <c r="E136" s="15" t="s">
+      <c r="C137" s="16" t="s">
         <v>769</v>
       </c>
-      <c r="F136" s="15" t="s">
+      <c r="D137" s="16" t="s">
         <v>770</v>
       </c>
-    </row>
-    <row r="137" s="2" customFormat="1" spans="1:6">
-      <c r="A137" s="13" t="s">
+      <c r="E137" s="16" t="s">
         <v>771</v>
       </c>
-      <c r="B137" s="23" t="s">
+      <c r="F137" s="16" t="s">
         <v>772</v>
-      </c>
-      <c r="C137" s="8" t="s">
-        <v>773</v>
-      </c>
-      <c r="D137" s="16" t="s">
-        <v>774</v>
-      </c>
-      <c r="E137" s="16" t="s">
-        <v>775</v>
-      </c>
-      <c r="F137" s="16" t="s">
-        <v>776</v>
       </c>
     </row>
     <row r="138" s="2" customFormat="1" spans="1:6">
-      <c r="A138" s="13" t="s">
+      <c r="A138" s="14" t="s">
+        <v>773</v>
+      </c>
+      <c r="B138" s="24" t="s">
+        <v>774</v>
+      </c>
+      <c r="C138" s="9" t="s">
+        <v>775</v>
+      </c>
+      <c r="D138" s="17" t="s">
+        <v>776</v>
+      </c>
+      <c r="E138" s="17" t="s">
         <v>777</v>
       </c>
-      <c r="B138" s="23" t="s">
+      <c r="F138" s="17" t="s">
         <v>778</v>
       </c>
-      <c r="C138" s="16" t="s">
+    </row>
+    <row r="139" s="2" customFormat="1" spans="1:6">
+      <c r="A139" s="14" t="s">
         <v>779</v>
       </c>
-      <c r="D138" s="16" t="s">
+      <c r="B139" s="24" t="s">
         <v>780</v>
       </c>
-      <c r="E138" s="16" t="s">
+      <c r="C139" s="17" t="s">
         <v>781</v>
       </c>
-      <c r="F138" s="16" t="s">
+      <c r="D139" s="17" t="s">
         <v>782</v>
+      </c>
+      <c r="E139" s="17" t="s">
+        <v>783</v>
+      </c>
+      <c r="F139" s="17" t="s">
+        <v>784</v>
       </c>
     </row>
   </sheetData>

</xml_diff>